<commit_message>
[Fonds de solidarite] Add 2020-04-29 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-naf.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-naf.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="84">
   <si>
     <t>dispositif</t>
   </si>
@@ -157,6 +157,9 @@
     <t>A</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
@@ -208,10 +211,10 @@
     <t>S</t>
   </si>
   <si>
-    <t>B</t>
+    <t>Agriculture, sylviculture et pêche</t>
   </si>
   <si>
-    <t>Agriculture, sylviculture et pêche</t>
+    <t>Industries extractives</t>
   </si>
   <si>
     <t>Industrie manufacturière</t>
@@ -263,9 +266,6 @@
   </si>
   <si>
     <t>Autres activités de services</t>
-  </si>
-  <si>
-    <t>Industries extractives</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H308"/>
+  <dimension ref="A1:H309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,10 +663,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>2273</v>
+        <v>2502</v>
       </c>
       <c r="D2">
-        <v>3074309</v>
+        <v>3391390</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -689,10 +689,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>5566</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>7014821</v>
+        <v>3823</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -715,10 +715,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>29</v>
+        <v>5689</v>
       </c>
       <c r="D4">
-        <v>38204</v>
+        <v>7162181</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -741,10 +741,10 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>249</v>
+        <v>30</v>
       </c>
       <c r="D5">
-        <v>304387</v>
+        <v>39522</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -767,10 +767,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>16070</v>
+        <v>258</v>
       </c>
       <c r="D6">
-        <v>23163406</v>
+        <v>313941</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -793,10 +793,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>20712</v>
+        <v>16436</v>
       </c>
       <c r="D7">
-        <v>27668860</v>
+        <v>23682679</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -819,10 +819,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>3960</v>
+        <v>21102</v>
       </c>
       <c r="D8">
-        <v>5482733</v>
+        <v>28173892</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -845,10 +845,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>16817</v>
+        <v>4034</v>
       </c>
       <c r="D9">
-        <v>24169016</v>
+        <v>5580872</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -871,10 +871,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>2007</v>
+        <v>17121</v>
       </c>
       <c r="D10">
-        <v>2616655</v>
+        <v>24592059</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -897,10 +897,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>950</v>
+        <v>2046</v>
       </c>
       <c r="D11">
-        <v>1338528</v>
+        <v>2665825</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -923,10 +923,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>3419</v>
+        <v>963</v>
       </c>
       <c r="D12">
-        <v>4699708</v>
+        <v>1357728</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -949,10 +949,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>10730</v>
+        <v>3508</v>
       </c>
       <c r="D13">
-        <v>14485749</v>
+        <v>4812675</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -975,10 +975,10 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>5057</v>
+        <v>10988</v>
       </c>
       <c r="D14">
-        <v>6496579</v>
+        <v>14817311</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1001,10 +1001,10 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>5160</v>
       </c>
       <c r="D15">
-        <v>4500</v>
+        <v>6623406</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1027,10 +1027,10 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>11596</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>14675937</v>
+        <v>4500</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1053,10 +1053,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>13058</v>
+        <v>11791</v>
       </c>
       <c r="D17">
-        <v>17378059</v>
+        <v>14898686</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1079,10 +1079,10 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>5523</v>
+        <v>13256</v>
       </c>
       <c r="D18">
-        <v>6674349</v>
+        <v>17630839</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1105,10 +1105,10 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>16867</v>
+        <v>5646</v>
       </c>
       <c r="D19">
-        <v>20346238</v>
+        <v>6813765</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1131,22 +1131,22 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>890</v>
+        <v>17017</v>
       </c>
       <c r="D20">
-        <v>1206504</v>
+        <v>20521102</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1157,10 +1157,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>937</v>
       </c>
       <c r="D21">
-        <v>4500</v>
+        <v>1267694</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1169,10 +1169,10 @@
         <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1183,10 +1183,10 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>1584</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>1937468</v>
+        <v>4500</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1209,10 +1209,10 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>1616</v>
       </c>
       <c r="D23">
-        <v>4500</v>
+        <v>1975316</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -1235,10 +1235,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>116</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>144575</v>
+        <v>4500</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1261,10 +1261,10 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>3989</v>
+        <v>117</v>
       </c>
       <c r="D25">
-        <v>5732942</v>
+        <v>146075</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
@@ -1287,10 +1287,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>6549</v>
+        <v>4093</v>
       </c>
       <c r="D26">
-        <v>8709321</v>
+        <v>5880041</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1313,10 +1313,10 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>514</v>
+        <v>6684</v>
       </c>
       <c r="D27">
-        <v>689813</v>
+        <v>8874819</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -1339,10 +1339,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>4943</v>
+        <v>533</v>
       </c>
       <c r="D28">
-        <v>7019499</v>
+        <v>717383</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1365,10 +1365,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>383</v>
+        <v>5046</v>
       </c>
       <c r="D29">
-        <v>474422</v>
+        <v>7160502</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
@@ -1391,10 +1391,10 @@
         <v>9</v>
       </c>
       <c r="C30">
-        <v>242</v>
+        <v>385</v>
       </c>
       <c r="D30">
-        <v>325485</v>
+        <v>477422</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
@@ -1417,10 +1417,10 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>776</v>
+        <v>252</v>
       </c>
       <c r="D31">
-        <v>1036474</v>
+        <v>337919</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -1443,10 +1443,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>2108</v>
+        <v>787</v>
       </c>
       <c r="D32">
-        <v>2813190</v>
+        <v>1047757</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
@@ -1469,10 +1469,10 @@
         <v>9</v>
       </c>
       <c r="C33">
-        <v>1123</v>
+        <v>2161</v>
       </c>
       <c r="D33">
-        <v>1405048</v>
+        <v>2889305</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1495,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>1570</v>
+        <v>1146</v>
       </c>
       <c r="D34">
-        <v>1844798</v>
+        <v>1434127</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -1507,10 +1507,10 @@
         <v>29</v>
       </c>
       <c r="G34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1521,10 +1521,10 @@
         <v>9</v>
       </c>
       <c r="C35">
-        <v>2817</v>
+        <v>1596</v>
       </c>
       <c r="D35">
-        <v>3727161</v>
+        <v>1873525</v>
       </c>
       <c r="E35" t="s">
         <v>11</v>
@@ -1547,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>1351</v>
+        <v>2870</v>
       </c>
       <c r="D36">
-        <v>1588699</v>
+        <v>3796897</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -1573,10 +1573,10 @@
         <v>9</v>
       </c>
       <c r="C37">
-        <v>5352</v>
+        <v>1396</v>
       </c>
       <c r="D37">
-        <v>6572645</v>
+        <v>1639482</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>
@@ -1599,22 +1599,22 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>833</v>
+        <v>5407</v>
       </c>
       <c r="D38">
-        <v>1134506</v>
+        <v>6642962</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G38" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H38" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1625,10 +1625,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>2054</v>
+        <v>872</v>
       </c>
       <c r="D39">
-        <v>2433413</v>
+        <v>1186640</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1637,10 +1637,10 @@
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1651,10 +1651,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>2091</v>
       </c>
       <c r="D40">
-        <v>7342</v>
+        <v>2474242</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -1677,10 +1677,10 @@
         <v>9</v>
       </c>
       <c r="C41">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="D41">
-        <v>87902</v>
+        <v>7342</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -1703,10 +1703,10 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>4537</v>
+        <v>78</v>
       </c>
       <c r="D42">
-        <v>6511242</v>
+        <v>90573</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -1729,10 +1729,10 @@
         <v>9</v>
       </c>
       <c r="C43">
-        <v>7323</v>
+        <v>4631</v>
       </c>
       <c r="D43">
-        <v>9839072</v>
+        <v>6642245</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1755,10 +1755,10 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>683</v>
+        <v>7446</v>
       </c>
       <c r="D44">
-        <v>925901</v>
+        <v>9981353</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -1781,10 +1781,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>6718</v>
+        <v>699</v>
       </c>
       <c r="D45">
-        <v>9607531</v>
+        <v>944485</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1807,10 +1807,10 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>606</v>
+        <v>6815</v>
       </c>
       <c r="D46">
-        <v>761940</v>
+        <v>9744962</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -1833,10 +1833,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>282</v>
+        <v>625</v>
       </c>
       <c r="D47">
-        <v>398028</v>
+        <v>787469</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -1859,10 +1859,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>1051</v>
+        <v>290</v>
       </c>
       <c r="D48">
-        <v>1373540</v>
+        <v>408830</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -1885,10 +1885,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>3149</v>
+        <v>1075</v>
       </c>
       <c r="D49">
-        <v>4208268</v>
+        <v>1403375</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -1911,10 +1911,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>1413</v>
+        <v>3219</v>
       </c>
       <c r="D50">
-        <v>1743189</v>
+        <v>4300078</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -1937,10 +1937,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>1751</v>
+        <v>1439</v>
       </c>
       <c r="D51">
-        <v>2110225</v>
+        <v>1771811</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -1949,10 +1949,10 @@
         <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1963,10 +1963,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>4636</v>
+        <v>1784</v>
       </c>
       <c r="D52">
-        <v>6204942</v>
+        <v>2148784</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -1989,10 +1989,10 @@
         <v>9</v>
       </c>
       <c r="C53">
-        <v>1651</v>
+        <v>4726</v>
       </c>
       <c r="D53">
-        <v>1928711</v>
+        <v>6325143</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -2015,10 +2015,10 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>6018</v>
+        <v>1692</v>
       </c>
       <c r="D54">
-        <v>7388271</v>
+        <v>1970164</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
@@ -2041,22 +2041,22 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>641</v>
+        <v>6083</v>
       </c>
       <c r="D55">
-        <v>872451</v>
+        <v>7452039</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G55" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H55" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2067,10 +2067,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>1255</v>
+        <v>663</v>
       </c>
       <c r="D56">
-        <v>1561329</v>
+        <v>903623</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -2079,10 +2079,10 @@
         <v>31</v>
       </c>
       <c r="G56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2093,10 +2093,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>1281</v>
       </c>
       <c r="D57">
-        <v>4500</v>
+        <v>1597459</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
@@ -2119,10 +2119,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="D58">
-        <v>62060</v>
+        <v>4500</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -2145,10 +2145,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>3918</v>
+        <v>64</v>
       </c>
       <c r="D59">
-        <v>5585785</v>
+        <v>64060</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
@@ -2171,10 +2171,10 @@
         <v>9</v>
       </c>
       <c r="C60">
-        <v>5305</v>
+        <v>4006</v>
       </c>
       <c r="D60">
-        <v>6928275</v>
+        <v>5705008</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
@@ -2197,10 +2197,10 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <v>618</v>
+        <v>5421</v>
       </c>
       <c r="D61">
-        <v>868992</v>
+        <v>7064023</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -2223,10 +2223,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>3831</v>
+        <v>634</v>
       </c>
       <c r="D62">
-        <v>5445027</v>
+        <v>892372</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -2249,10 +2249,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>382</v>
+        <v>3879</v>
       </c>
       <c r="D63">
-        <v>483811</v>
+        <v>5513459</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -2275,10 +2275,10 @@
         <v>9</v>
       </c>
       <c r="C64">
-        <v>209</v>
+        <v>394</v>
       </c>
       <c r="D64">
-        <v>293477</v>
+        <v>499854</v>
       </c>
       <c r="E64" t="s">
         <v>13</v>
@@ -2301,10 +2301,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>754</v>
+        <v>216</v>
       </c>
       <c r="D65">
-        <v>1001077</v>
+        <v>303547</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -2327,10 +2327,10 @@
         <v>9</v>
       </c>
       <c r="C66">
-        <v>1988</v>
+        <v>768</v>
       </c>
       <c r="D66">
-        <v>2645368</v>
+        <v>1019473</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -2353,10 +2353,10 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>1058</v>
+        <v>2036</v>
       </c>
       <c r="D67">
-        <v>1323737</v>
+        <v>2708871</v>
       </c>
       <c r="E67" t="s">
         <v>13</v>
@@ -2379,10 +2379,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>1234</v>
+        <v>1086</v>
       </c>
       <c r="D68">
-        <v>1498450</v>
+        <v>1357284</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -2391,10 +2391,10 @@
         <v>31</v>
       </c>
       <c r="G68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2405,10 +2405,10 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>2329</v>
+        <v>1264</v>
       </c>
       <c r="D69">
-        <v>3051920</v>
+        <v>1530889</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -2431,10 +2431,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>1205</v>
+        <v>2375</v>
       </c>
       <c r="D70">
-        <v>1423368</v>
+        <v>3108798</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -2457,10 +2457,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>4731</v>
+        <v>1228</v>
       </c>
       <c r="D71">
-        <v>5757327</v>
+        <v>1447726</v>
       </c>
       <c r="E71" t="s">
         <v>13</v>
@@ -2483,22 +2483,22 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>558</v>
+        <v>4777</v>
       </c>
       <c r="D72">
-        <v>772877</v>
+        <v>5809474</v>
       </c>
       <c r="E72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G72" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H72" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2509,10 +2509,10 @@
         <v>9</v>
       </c>
       <c r="C73">
-        <v>477</v>
+        <v>602</v>
       </c>
       <c r="D73">
-        <v>622053</v>
+        <v>831705</v>
       </c>
       <c r="E73" t="s">
         <v>14</v>
@@ -2521,10 +2521,10 @@
         <v>32</v>
       </c>
       <c r="G73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2535,10 +2535,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>3</v>
+        <v>497</v>
       </c>
       <c r="D74">
-        <v>4363</v>
+        <v>648010</v>
       </c>
       <c r="E74" t="s">
         <v>14</v>
@@ -2547,10 +2547,10 @@
         <v>32</v>
       </c>
       <c r="G74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H74" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2561,10 +2561,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>1300</v>
+        <v>3</v>
       </c>
       <c r="D75">
-        <v>1843412</v>
+        <v>4363</v>
       </c>
       <c r="E75" t="s">
         <v>14</v>
@@ -2587,10 +2587,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>1272</v>
+        <v>1335</v>
       </c>
       <c r="D76">
-        <v>1748334</v>
+        <v>1894098</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
@@ -2613,10 +2613,10 @@
         <v>9</v>
       </c>
       <c r="C77">
-        <v>164</v>
+        <v>1296</v>
       </c>
       <c r="D77">
-        <v>229989</v>
+        <v>1780787</v>
       </c>
       <c r="E77" t="s">
         <v>14</v>
@@ -2639,10 +2639,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>1114</v>
+        <v>167</v>
       </c>
       <c r="D78">
-        <v>1577962</v>
+        <v>234489</v>
       </c>
       <c r="E78" t="s">
         <v>14</v>
@@ -2665,10 +2665,10 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>85</v>
+        <v>1145</v>
       </c>
       <c r="D79">
-        <v>108322</v>
+        <v>1621035</v>
       </c>
       <c r="E79" t="s">
         <v>14</v>
@@ -2691,10 +2691,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="D80">
-        <v>43471</v>
+        <v>111265</v>
       </c>
       <c r="E80" t="s">
         <v>14</v>
@@ -2717,10 +2717,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>244</v>
+        <v>33</v>
       </c>
       <c r="D81">
-        <v>326334</v>
+        <v>44971</v>
       </c>
       <c r="E81" t="s">
         <v>14</v>
@@ -2743,10 +2743,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>839</v>
+        <v>254</v>
       </c>
       <c r="D82">
-        <v>1162156</v>
+        <v>338165</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2769,10 +2769,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>458</v>
+        <v>860</v>
       </c>
       <c r="D83">
-        <v>572001</v>
+        <v>1191627</v>
       </c>
       <c r="E83" t="s">
         <v>14</v>
@@ -2795,10 +2795,10 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>245</v>
+        <v>470</v>
       </c>
       <c r="D84">
-        <v>296768</v>
+        <v>586908</v>
       </c>
       <c r="E84" t="s">
         <v>14</v>
@@ -2807,10 +2807,10 @@
         <v>32</v>
       </c>
       <c r="G84" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2821,10 +2821,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>489</v>
+        <v>251</v>
       </c>
       <c r="D85">
-        <v>645648</v>
+        <v>304098</v>
       </c>
       <c r="E85" t="s">
         <v>14</v>
@@ -2847,10 +2847,10 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>249</v>
+        <v>503</v>
       </c>
       <c r="D86">
-        <v>309915</v>
+        <v>663994</v>
       </c>
       <c r="E86" t="s">
         <v>14</v>
@@ -2873,10 +2873,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>879</v>
+        <v>254</v>
       </c>
       <c r="D87">
-        <v>1020781</v>
+        <v>316406</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -2899,22 +2899,22 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>1130</v>
+        <v>895</v>
       </c>
       <c r="D88">
-        <v>1550999</v>
+        <v>1034851</v>
       </c>
       <c r="E88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G88" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H88" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2925,10 +2925,10 @@
         <v>9</v>
       </c>
       <c r="C89">
-        <v>3</v>
+        <v>1193</v>
       </c>
       <c r="D89">
-        <v>4500</v>
+        <v>1639114</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -2937,10 +2937,10 @@
         <v>33</v>
       </c>
       <c r="G89" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H89" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2951,10 +2951,10 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>2657</v>
+        <v>4</v>
       </c>
       <c r="D90">
-        <v>3395110</v>
+        <v>4827</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -2977,10 +2977,10 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>3</v>
+        <v>2716</v>
       </c>
       <c r="D91">
-        <v>3310</v>
+        <v>3469943</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -3003,10 +3003,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>190</v>
+        <v>3</v>
       </c>
       <c r="D92">
-        <v>220326</v>
+        <v>3310</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -3029,10 +3029,10 @@
         <v>9</v>
       </c>
       <c r="C93">
-        <v>8116</v>
+        <v>195</v>
       </c>
       <c r="D93">
-        <v>11703782</v>
+        <v>226156</v>
       </c>
       <c r="E93" t="s">
         <v>15</v>
@@ -3055,10 +3055,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>11792</v>
+        <v>8364</v>
       </c>
       <c r="D94">
-        <v>15765944</v>
+        <v>12054213</v>
       </c>
       <c r="E94" t="s">
         <v>15</v>
@@ -3081,10 +3081,10 @@
         <v>9</v>
       </c>
       <c r="C95">
-        <v>1446</v>
+        <v>12063</v>
       </c>
       <c r="D95">
-        <v>1967268</v>
+        <v>16114541</v>
       </c>
       <c r="E95" t="s">
         <v>15</v>
@@ -3107,10 +3107,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>8149</v>
+        <v>1478</v>
       </c>
       <c r="D96">
-        <v>11779878</v>
+        <v>2008231</v>
       </c>
       <c r="E96" t="s">
         <v>15</v>
@@ -3133,10 +3133,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>854</v>
+        <v>8320</v>
       </c>
       <c r="D97">
-        <v>1093930</v>
+        <v>12014259</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
@@ -3159,10 +3159,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>498</v>
+        <v>877</v>
       </c>
       <c r="D98">
-        <v>690736</v>
+        <v>1121833</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -3185,10 +3185,10 @@
         <v>9</v>
       </c>
       <c r="C99">
-        <v>1273</v>
+        <v>508</v>
       </c>
       <c r="D99">
-        <v>1723707</v>
+        <v>705736</v>
       </c>
       <c r="E99" t="s">
         <v>15</v>
@@ -3211,10 +3211,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>4578</v>
+        <v>1302</v>
       </c>
       <c r="D100">
-        <v>6150518</v>
+        <v>1761424</v>
       </c>
       <c r="E100" t="s">
         <v>15</v>
@@ -3237,10 +3237,10 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>2101</v>
+        <v>4686</v>
       </c>
       <c r="D101">
-        <v>2643198</v>
+        <v>6290027</v>
       </c>
       <c r="E101" t="s">
         <v>15</v>
@@ -3263,10 +3263,10 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>2623</v>
+        <v>2150</v>
       </c>
       <c r="D102">
-        <v>3147583</v>
+        <v>2707823</v>
       </c>
       <c r="E102" t="s">
         <v>15</v>
@@ -3275,10 +3275,10 @@
         <v>33</v>
       </c>
       <c r="G102" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H102" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3289,10 +3289,10 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>5347</v>
+        <v>2677</v>
       </c>
       <c r="D103">
-        <v>7233114</v>
+        <v>3204878</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
@@ -3315,10 +3315,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>2289</v>
+        <v>5503</v>
       </c>
       <c r="D104">
-        <v>2676538</v>
+        <v>7443816</v>
       </c>
       <c r="E104" t="s">
         <v>15</v>
@@ -3341,10 +3341,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>10647</v>
+        <v>2355</v>
       </c>
       <c r="D105">
-        <v>12579975</v>
+        <v>2754734</v>
       </c>
       <c r="E105" t="s">
         <v>15</v>
@@ -3367,22 +3367,22 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>437</v>
+        <v>10762</v>
       </c>
       <c r="D106">
-        <v>607220</v>
+        <v>12701677</v>
       </c>
       <c r="E106" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F106" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G106" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H106" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3393,10 +3393,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>590</v>
+        <v>458</v>
       </c>
       <c r="D107">
-        <v>813654</v>
+        <v>637000</v>
       </c>
       <c r="E107" t="s">
         <v>16</v>
@@ -3405,10 +3405,10 @@
         <v>34</v>
       </c>
       <c r="G107" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H107" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3419,10 +3419,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>3</v>
+        <v>610</v>
       </c>
       <c r="D108">
-        <v>4500</v>
+        <v>840835</v>
       </c>
       <c r="E108" t="s">
         <v>16</v>
@@ -3445,10 +3445,10 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D109">
-        <v>22000</v>
+        <v>6000</v>
       </c>
       <c r="E109" t="s">
         <v>16</v>
@@ -3471,10 +3471,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>981</v>
+        <v>15</v>
       </c>
       <c r="D110">
-        <v>1412222</v>
+        <v>22000</v>
       </c>
       <c r="E110" t="s">
         <v>16</v>
@@ -3497,10 +3497,10 @@
         <v>9</v>
       </c>
       <c r="C111">
-        <v>1540</v>
+        <v>1022</v>
       </c>
       <c r="D111">
-        <v>2116661</v>
+        <v>1471562</v>
       </c>
       <c r="E111" t="s">
         <v>16</v>
@@ -3523,10 +3523,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>378</v>
+        <v>1599</v>
       </c>
       <c r="D112">
-        <v>537557</v>
+        <v>2198114</v>
       </c>
       <c r="E112" t="s">
         <v>16</v>
@@ -3549,10 +3549,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>937</v>
+        <v>389</v>
       </c>
       <c r="D113">
-        <v>1331140</v>
+        <v>551819</v>
       </c>
       <c r="E113" t="s">
         <v>16</v>
@@ -3575,10 +3575,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>149</v>
+        <v>958</v>
       </c>
       <c r="D114">
-        <v>201941</v>
+        <v>1360582</v>
       </c>
       <c r="E114" t="s">
         <v>16</v>
@@ -3601,10 +3601,10 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="D115">
-        <v>54201</v>
+        <v>210366</v>
       </c>
       <c r="E115" t="s">
         <v>16</v>
@@ -3627,10 +3627,10 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="D116">
-        <v>283160</v>
+        <v>58701</v>
       </c>
       <c r="E116" t="s">
         <v>16</v>
@@ -3653,10 +3653,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>621</v>
+        <v>208</v>
       </c>
       <c r="D117">
-        <v>857955</v>
+        <v>288314</v>
       </c>
       <c r="E117" t="s">
         <v>16</v>
@@ -3679,10 +3679,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>630</v>
+        <v>644</v>
       </c>
       <c r="D118">
-        <v>835396</v>
+        <v>889317</v>
       </c>
       <c r="E118" t="s">
         <v>16</v>
@@ -3705,10 +3705,10 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>352</v>
+        <v>651</v>
       </c>
       <c r="D119">
-        <v>443038</v>
+        <v>863957</v>
       </c>
       <c r="E119" t="s">
         <v>16</v>
@@ -3717,10 +3717,10 @@
         <v>34</v>
       </c>
       <c r="G119" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H119" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -3731,10 +3731,10 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>516</v>
+        <v>358</v>
       </c>
       <c r="D120">
-        <v>719360</v>
+        <v>449527</v>
       </c>
       <c r="E120" t="s">
         <v>16</v>
@@ -3757,10 +3757,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>211</v>
+        <v>531</v>
       </c>
       <c r="D121">
-        <v>277319</v>
+        <v>741310</v>
       </c>
       <c r="E121" t="s">
         <v>16</v>
@@ -3783,10 +3783,10 @@
         <v>9</v>
       </c>
       <c r="C122">
-        <v>644</v>
+        <v>216</v>
       </c>
       <c r="D122">
-        <v>793583</v>
+        <v>284819</v>
       </c>
       <c r="E122" t="s">
         <v>16</v>
@@ -3809,22 +3809,22 @@
         <v>9</v>
       </c>
       <c r="C123">
-        <v>178</v>
+        <v>659</v>
       </c>
       <c r="D123">
-        <v>246522</v>
+        <v>811104</v>
       </c>
       <c r="E123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F123" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G123" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H123" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3835,10 +3835,10 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>112</v>
+        <v>190</v>
       </c>
       <c r="D124">
-        <v>156625</v>
+        <v>263203</v>
       </c>
       <c r="E124" t="s">
         <v>17</v>
@@ -3847,10 +3847,10 @@
         <v>35</v>
       </c>
       <c r="G124" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H124" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -3861,10 +3861,10 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="D125">
-        <v>4500</v>
+        <v>161125</v>
       </c>
       <c r="E125" t="s">
         <v>17</v>
@@ -3873,10 +3873,10 @@
         <v>35</v>
       </c>
       <c r="G125" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H125" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -3887,10 +3887,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="D126">
-        <v>306903</v>
+        <v>4500</v>
       </c>
       <c r="E126" t="s">
         <v>17</v>
@@ -3913,10 +3913,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>303</v>
+        <v>221</v>
       </c>
       <c r="D127">
-        <v>426870</v>
+        <v>323720</v>
       </c>
       <c r="E127" t="s">
         <v>17</v>
@@ -3939,10 +3939,10 @@
         <v>9</v>
       </c>
       <c r="C128">
-        <v>60</v>
+        <v>309</v>
       </c>
       <c r="D128">
-        <v>86740</v>
+        <v>435870</v>
       </c>
       <c r="E128" t="s">
         <v>17</v>
@@ -3965,10 +3965,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>193</v>
+        <v>66</v>
       </c>
       <c r="D129">
-        <v>273308</v>
+        <v>95740</v>
       </c>
       <c r="E129" t="s">
         <v>17</v>
@@ -3991,10 +3991,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>30</v>
+        <v>201</v>
       </c>
       <c r="D130">
-        <v>42360</v>
+        <v>285308</v>
       </c>
       <c r="E130" t="s">
         <v>17</v>
@@ -4017,10 +4017,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D131">
-        <v>28162</v>
+        <v>43860</v>
       </c>
       <c r="E131" t="s">
         <v>17</v>
@@ -4043,10 +4043,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D132">
-        <v>25405</v>
+        <v>28162</v>
       </c>
       <c r="E132" t="s">
         <v>17</v>
@@ -4069,10 +4069,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>151</v>
+        <v>19</v>
       </c>
       <c r="D133">
-        <v>213177</v>
+        <v>26905</v>
       </c>
       <c r="E133" t="s">
         <v>17</v>
@@ -4095,10 +4095,10 @@
         <v>9</v>
       </c>
       <c r="C134">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="D134">
-        <v>158887</v>
+        <v>222532</v>
       </c>
       <c r="E134" t="s">
         <v>17</v>
@@ -4121,10 +4121,10 @@
         <v>9</v>
       </c>
       <c r="C135">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="D135">
-        <v>104808</v>
+        <v>158887</v>
       </c>
       <c r="E135" t="s">
         <v>17</v>
@@ -4133,10 +4133,10 @@
         <v>35</v>
       </c>
       <c r="G135" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H135" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -4147,10 +4147,10 @@
         <v>9</v>
       </c>
       <c r="C136">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D136">
-        <v>123225</v>
+        <v>109076</v>
       </c>
       <c r="E136" t="s">
         <v>17</v>
@@ -4173,10 +4173,10 @@
         <v>9</v>
       </c>
       <c r="C137">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="D137">
-        <v>58647</v>
+        <v>130725</v>
       </c>
       <c r="E137" t="s">
         <v>17</v>
@@ -4199,10 +4199,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="D138">
-        <v>156551</v>
+        <v>60147</v>
       </c>
       <c r="E138" t="s">
         <v>17</v>
@@ -4225,22 +4225,22 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>688</v>
+        <v>124</v>
       </c>
       <c r="D139">
-        <v>915513</v>
+        <v>161751</v>
       </c>
       <c r="E139" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F139" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G139" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H139" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -4251,10 +4251,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>2148</v>
+        <v>723</v>
       </c>
       <c r="D140">
-        <v>2602085</v>
+        <v>959989</v>
       </c>
       <c r="E140" t="s">
         <v>18</v>
@@ -4263,10 +4263,10 @@
         <v>36</v>
       </c>
       <c r="G140" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H140" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -4277,10 +4277,10 @@
         <v>9</v>
       </c>
       <c r="C141">
-        <v>7</v>
+        <v>2204</v>
       </c>
       <c r="D141">
-        <v>9525</v>
+        <v>2667301</v>
       </c>
       <c r="E141" t="s">
         <v>18</v>
@@ -4303,10 +4303,10 @@
         <v>9</v>
       </c>
       <c r="C142">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D142">
-        <v>125144</v>
+        <v>9525</v>
       </c>
       <c r="E142" t="s">
         <v>18</v>
@@ -4329,10 +4329,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>7093</v>
+        <v>107</v>
       </c>
       <c r="D143">
-        <v>10052396</v>
+        <v>126174</v>
       </c>
       <c r="E143" t="s">
         <v>18</v>
@@ -4355,10 +4355,10 @@
         <v>9</v>
       </c>
       <c r="C144">
-        <v>11832</v>
+        <v>7244</v>
       </c>
       <c r="D144">
-        <v>15108987</v>
+        <v>10262530</v>
       </c>
       <c r="E144" t="s">
         <v>18</v>
@@ -4381,10 +4381,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>2256</v>
+        <v>12071</v>
       </c>
       <c r="D145">
-        <v>3074610</v>
+        <v>15393404</v>
       </c>
       <c r="E145" t="s">
         <v>18</v>
@@ -4407,10 +4407,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>7964</v>
+        <v>2298</v>
       </c>
       <c r="D146">
-        <v>11480809</v>
+        <v>3131993</v>
       </c>
       <c r="E146" t="s">
         <v>18</v>
@@ -4433,10 +4433,10 @@
         <v>9</v>
       </c>
       <c r="C147">
-        <v>792</v>
+        <v>8126</v>
       </c>
       <c r="D147">
-        <v>1008150</v>
+        <v>11711885</v>
       </c>
       <c r="E147" t="s">
         <v>18</v>
@@ -4459,10 +4459,10 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>496</v>
+        <v>813</v>
       </c>
       <c r="D148">
-        <v>690400</v>
+        <v>1035000</v>
       </c>
       <c r="E148" t="s">
         <v>18</v>
@@ -4485,10 +4485,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>1239</v>
+        <v>511</v>
       </c>
       <c r="D149">
-        <v>1643654</v>
+        <v>712678</v>
       </c>
       <c r="E149" t="s">
         <v>18</v>
@@ -4511,10 +4511,10 @@
         <v>9</v>
       </c>
       <c r="C150">
-        <v>4566</v>
+        <v>1267</v>
       </c>
       <c r="D150">
-        <v>6152691</v>
+        <v>1681193</v>
       </c>
       <c r="E150" t="s">
         <v>18</v>
@@ -4537,10 +4537,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>2174</v>
+        <v>4676</v>
       </c>
       <c r="D151">
-        <v>2700776</v>
+        <v>6292805</v>
       </c>
       <c r="E151" t="s">
         <v>18</v>
@@ -4563,10 +4563,10 @@
         <v>9</v>
       </c>
       <c r="C152">
-        <v>2375</v>
+        <v>2216</v>
       </c>
       <c r="D152">
-        <v>2918478</v>
+        <v>2752129</v>
       </c>
       <c r="E152" t="s">
         <v>18</v>
@@ -4575,10 +4575,10 @@
         <v>36</v>
       </c>
       <c r="G152" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H152" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -4589,10 +4589,10 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>5415</v>
+        <v>2403</v>
       </c>
       <c r="D153">
-        <v>7288427</v>
+        <v>2947654</v>
       </c>
       <c r="E153" t="s">
         <v>18</v>
@@ -4615,10 +4615,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>2288</v>
+        <v>5530</v>
       </c>
       <c r="D154">
-        <v>2711781</v>
+        <v>7436993</v>
       </c>
       <c r="E154" t="s">
         <v>18</v>
@@ -4641,10 +4641,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>10424</v>
+        <v>2347</v>
       </c>
       <c r="D155">
-        <v>11927999</v>
+        <v>2778944</v>
       </c>
       <c r="E155" t="s">
         <v>18</v>
@@ -4667,22 +4667,22 @@
         <v>9</v>
       </c>
       <c r="C156">
-        <v>617</v>
+        <v>10512</v>
       </c>
       <c r="D156">
-        <v>826115</v>
+        <v>12012965</v>
       </c>
       <c r="E156" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F156" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G156" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H156" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -4693,10 +4693,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>1073</v>
+        <v>659</v>
       </c>
       <c r="D157">
-        <v>1427375</v>
+        <v>881317</v>
       </c>
       <c r="E157" t="s">
         <v>19</v>
@@ -4705,10 +4705,10 @@
         <v>37</v>
       </c>
       <c r="G157" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H157" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -4719,10 +4719,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>19</v>
+        <v>1108</v>
       </c>
       <c r="D158">
-        <v>28500</v>
+        <v>1473024</v>
       </c>
       <c r="E158" t="s">
         <v>19</v>
@@ -4731,10 +4731,10 @@
         <v>37</v>
       </c>
       <c r="G158" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H158" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -4745,10 +4745,10 @@
         <v>9</v>
       </c>
       <c r="C159">
-        <v>2087</v>
+        <v>20</v>
       </c>
       <c r="D159">
-        <v>3052357</v>
+        <v>30000</v>
       </c>
       <c r="E159" t="s">
         <v>19</v>
@@ -4771,10 +4771,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>3455</v>
+        <v>2161</v>
       </c>
       <c r="D160">
-        <v>4711046</v>
+        <v>3156584</v>
       </c>
       <c r="E160" t="s">
         <v>19</v>
@@ -4797,10 +4797,10 @@
         <v>9</v>
       </c>
       <c r="C161">
-        <v>468</v>
+        <v>3555</v>
       </c>
       <c r="D161">
-        <v>658851</v>
+        <v>4843487</v>
       </c>
       <c r="E161" t="s">
         <v>19</v>
@@ -4823,10 +4823,10 @@
         <v>9</v>
       </c>
       <c r="C162">
-        <v>1707</v>
+        <v>485</v>
       </c>
       <c r="D162">
-        <v>2397801</v>
+        <v>684351</v>
       </c>
       <c r="E162" t="s">
         <v>19</v>
@@ -4849,10 +4849,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>229</v>
+        <v>1758</v>
       </c>
       <c r="D163">
-        <v>310126</v>
+        <v>2468779</v>
       </c>
       <c r="E163" t="s">
         <v>19</v>
@@ -4875,10 +4875,10 @@
         <v>9</v>
       </c>
       <c r="C164">
-        <v>103</v>
+        <v>235</v>
       </c>
       <c r="D164">
-        <v>149144</v>
+        <v>316691</v>
       </c>
       <c r="E164" t="s">
         <v>19</v>
@@ -4901,10 +4901,10 @@
         <v>9</v>
       </c>
       <c r="C165">
-        <v>296</v>
+        <v>104</v>
       </c>
       <c r="D165">
-        <v>411479</v>
+        <v>150644</v>
       </c>
       <c r="E165" t="s">
         <v>19</v>
@@ -4927,10 +4927,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>1064</v>
+        <v>304</v>
       </c>
       <c r="D166">
-        <v>1498770</v>
+        <v>423478</v>
       </c>
       <c r="E166" t="s">
         <v>19</v>
@@ -4953,10 +4953,10 @@
         <v>9</v>
       </c>
       <c r="C167">
-        <v>587</v>
+        <v>1099</v>
       </c>
       <c r="D167">
-        <v>802464</v>
+        <v>1547929</v>
       </c>
       <c r="E167" t="s">
         <v>19</v>
@@ -4979,10 +4979,10 @@
         <v>9</v>
       </c>
       <c r="C168">
-        <v>904</v>
+        <v>599</v>
       </c>
       <c r="D168">
-        <v>1141251</v>
+        <v>819007</v>
       </c>
       <c r="E168" t="s">
         <v>19</v>
@@ -4991,10 +4991,10 @@
         <v>37</v>
       </c>
       <c r="G168" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H168" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -5005,10 +5005,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>1234</v>
+        <v>922</v>
       </c>
       <c r="D169">
-        <v>1736482</v>
+        <v>1165785</v>
       </c>
       <c r="E169" t="s">
         <v>19</v>
@@ -5031,10 +5031,10 @@
         <v>9</v>
       </c>
       <c r="C170">
-        <v>496</v>
+        <v>1267</v>
       </c>
       <c r="D170">
-        <v>637726</v>
+        <v>1782593</v>
       </c>
       <c r="E170" t="s">
         <v>19</v>
@@ -5057,10 +5057,10 @@
         <v>9</v>
       </c>
       <c r="C171">
-        <v>1505</v>
+        <v>509</v>
       </c>
       <c r="D171">
-        <v>1874383</v>
+        <v>654894</v>
       </c>
       <c r="E171" t="s">
         <v>19</v>
@@ -5083,22 +5083,22 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>212</v>
+        <v>1535</v>
       </c>
       <c r="D172">
-        <v>266958</v>
+        <v>1914061</v>
       </c>
       <c r="E172" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F172" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G172" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H172" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -5109,10 +5109,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>450</v>
+        <v>243</v>
       </c>
       <c r="D173">
-        <v>602450</v>
+        <v>307589</v>
       </c>
       <c r="E173" t="s">
         <v>20</v>
@@ -5121,10 +5121,10 @@
         <v>38</v>
       </c>
       <c r="G173" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H173" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -5135,10 +5135,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>7</v>
+        <v>461</v>
       </c>
       <c r="D174">
-        <v>10500</v>
+        <v>616162</v>
       </c>
       <c r="E174" t="s">
         <v>20</v>
@@ -5147,10 +5147,10 @@
         <v>38</v>
       </c>
       <c r="G174" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H174" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -5161,10 +5161,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>652</v>
+        <v>7</v>
       </c>
       <c r="D175">
-        <v>940270</v>
+        <v>10500</v>
       </c>
       <c r="E175" t="s">
         <v>20</v>
@@ -5187,10 +5187,10 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>1180</v>
+        <v>676</v>
       </c>
       <c r="D176">
-        <v>1614357</v>
+        <v>974083</v>
       </c>
       <c r="E176" t="s">
         <v>20</v>
@@ -5213,10 +5213,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>350</v>
+        <v>1203</v>
       </c>
       <c r="D177">
-        <v>487278</v>
+        <v>1646623</v>
       </c>
       <c r="E177" t="s">
         <v>20</v>
@@ -5239,10 +5239,10 @@
         <v>9</v>
       </c>
       <c r="C178">
-        <v>637</v>
+        <v>367</v>
       </c>
       <c r="D178">
-        <v>917094</v>
+        <v>510993</v>
       </c>
       <c r="E178" t="s">
         <v>20</v>
@@ -5265,10 +5265,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>98</v>
+        <v>663</v>
       </c>
       <c r="D179">
-        <v>131767</v>
+        <v>955583</v>
       </c>
       <c r="E179" t="s">
         <v>20</v>
@@ -5291,10 +5291,10 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="D180">
-        <v>68546</v>
+        <v>133267</v>
       </c>
       <c r="E180" t="s">
         <v>20</v>
@@ -5317,10 +5317,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="D181">
-        <v>182535</v>
+        <v>70046</v>
       </c>
       <c r="E181" t="s">
         <v>20</v>
@@ -5343,10 +5343,10 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>551</v>
+        <v>134</v>
       </c>
       <c r="D182">
-        <v>761533</v>
+        <v>187311</v>
       </c>
       <c r="E182" t="s">
         <v>20</v>
@@ -5369,10 +5369,10 @@
         <v>9</v>
       </c>
       <c r="C183">
-        <v>482</v>
+        <v>569</v>
       </c>
       <c r="D183">
-        <v>655194</v>
+        <v>787837</v>
       </c>
       <c r="E183" t="s">
         <v>20</v>
@@ -5395,10 +5395,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>285</v>
+        <v>490</v>
       </c>
       <c r="D184">
-        <v>362636</v>
+        <v>665203</v>
       </c>
       <c r="E184" t="s">
         <v>20</v>
@@ -5407,10 +5407,10 @@
         <v>38</v>
       </c>
       <c r="G184" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H184" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5421,10 +5421,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>485</v>
+        <v>293</v>
       </c>
       <c r="D185">
-        <v>663706</v>
+        <v>373252</v>
       </c>
       <c r="E185" t="s">
         <v>20</v>
@@ -5447,10 +5447,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>187</v>
+        <v>501</v>
       </c>
       <c r="D186">
-        <v>242763</v>
+        <v>686960</v>
       </c>
       <c r="E186" t="s">
         <v>20</v>
@@ -5473,10 +5473,10 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>687</v>
+        <v>191</v>
       </c>
       <c r="D187">
-        <v>869666</v>
+        <v>247769</v>
       </c>
       <c r="E187" t="s">
         <v>20</v>
@@ -5499,22 +5499,22 @@
         <v>9</v>
       </c>
       <c r="C188">
+        <v>695</v>
+      </c>
+      <c r="D188">
+        <v>879883</v>
+      </c>
+      <c r="E188" t="s">
         <v>20</v>
       </c>
-      <c r="D188">
-        <v>27864</v>
-      </c>
-      <c r="E188" t="s">
-        <v>21</v>
-      </c>
       <c r="F188" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G188" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H188" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5525,10 +5525,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D189">
-        <v>61306</v>
+        <v>27864</v>
       </c>
       <c r="E189" t="s">
         <v>21</v>
@@ -5537,10 +5537,10 @@
         <v>39</v>
       </c>
       <c r="G189" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H189" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5551,10 +5551,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="D190">
-        <v>3520</v>
+        <v>64124</v>
       </c>
       <c r="E190" t="s">
         <v>21</v>
@@ -5563,10 +5563,10 @@
         <v>39</v>
       </c>
       <c r="G190" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H190" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -5577,10 +5577,10 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="D191">
-        <v>170241</v>
+        <v>3520</v>
       </c>
       <c r="E191" t="s">
         <v>21</v>
@@ -5603,10 +5603,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>267</v>
+        <v>119</v>
       </c>
       <c r="D192">
-        <v>374516</v>
+        <v>173241</v>
       </c>
       <c r="E192" t="s">
         <v>21</v>
@@ -5629,10 +5629,10 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="D193">
-        <v>96561</v>
+        <v>383516</v>
       </c>
       <c r="E193" t="s">
         <v>21</v>
@@ -5655,10 +5655,10 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D194">
-        <v>118915</v>
+        <v>102461</v>
       </c>
       <c r="E194" t="s">
         <v>21</v>
@@ -5681,10 +5681,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="D195">
-        <v>19043</v>
+        <v>118915</v>
       </c>
       <c r="E195" t="s">
         <v>21</v>
@@ -5707,10 +5707,10 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D196">
-        <v>4500</v>
+        <v>19043</v>
       </c>
       <c r="E196" t="s">
         <v>21</v>
@@ -5733,10 +5733,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="D197">
-        <v>59586</v>
+        <v>4500</v>
       </c>
       <c r="E197" t="s">
         <v>21</v>
@@ -5745,10 +5745,10 @@
         <v>39</v>
       </c>
       <c r="G197" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H197" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -5759,10 +5759,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D198">
-        <v>41895</v>
+        <v>61086</v>
       </c>
       <c r="E198" t="s">
         <v>21</v>
@@ -5785,10 +5785,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D199">
-        <v>53765</v>
+        <v>41895</v>
       </c>
       <c r="E199" t="s">
         <v>21</v>
@@ -5797,10 +5797,10 @@
         <v>39</v>
       </c>
       <c r="G199" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H199" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -5811,10 +5811,10 @@
         <v>9</v>
       </c>
       <c r="C200">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D200">
-        <v>35992</v>
+        <v>58265</v>
       </c>
       <c r="E200" t="s">
         <v>21</v>
@@ -5837,10 +5837,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D201">
-        <v>25200</v>
+        <v>35992</v>
       </c>
       <c r="E201" t="s">
         <v>21</v>
@@ -5863,10 +5863,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D202">
-        <v>51205</v>
+        <v>26700</v>
       </c>
       <c r="E202" t="s">
         <v>21</v>
@@ -5889,22 +5889,22 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>799</v>
+        <v>37</v>
       </c>
       <c r="D203">
-        <v>1087991</v>
+        <v>52705</v>
       </c>
       <c r="E203" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F203" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G203" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H203" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -5915,10 +5915,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>1460</v>
+        <v>841</v>
       </c>
       <c r="D204">
-        <v>1808144</v>
+        <v>1141893</v>
       </c>
       <c r="E204" t="s">
         <v>22</v>
@@ -5927,10 +5927,10 @@
         <v>40</v>
       </c>
       <c r="G204" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H204" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -5941,10 +5941,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>78</v>
+        <v>1494</v>
       </c>
       <c r="D205">
-        <v>95960</v>
+        <v>1850875</v>
       </c>
       <c r="E205" t="s">
         <v>22</v>
@@ -5953,10 +5953,10 @@
         <v>40</v>
       </c>
       <c r="G205" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H205" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -5967,10 +5967,10 @@
         <v>9</v>
       </c>
       <c r="C206">
-        <v>4405</v>
+        <v>83</v>
       </c>
       <c r="D206">
-        <v>6306076</v>
+        <v>101349</v>
       </c>
       <c r="E206" t="s">
         <v>22</v>
@@ -5993,10 +5993,10 @@
         <v>9</v>
       </c>
       <c r="C207">
-        <v>7727</v>
+        <v>4502</v>
       </c>
       <c r="D207">
-        <v>10193979</v>
+        <v>6444027</v>
       </c>
       <c r="E207" t="s">
         <v>22</v>
@@ -6019,10 +6019,10 @@
         <v>9</v>
       </c>
       <c r="C208">
-        <v>767</v>
+        <v>7842</v>
       </c>
       <c r="D208">
-        <v>1032909</v>
+        <v>10336603</v>
       </c>
       <c r="E208" t="s">
         <v>22</v>
@@ -6045,10 +6045,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>5314</v>
+        <v>783</v>
       </c>
       <c r="D209">
-        <v>7609307</v>
+        <v>1054583</v>
       </c>
       <c r="E209" t="s">
         <v>22</v>
@@ -6071,10 +6071,10 @@
         <v>9</v>
       </c>
       <c r="C210">
-        <v>431</v>
+        <v>5394</v>
       </c>
       <c r="D210">
-        <v>534170</v>
+        <v>7720315</v>
       </c>
       <c r="E210" t="s">
         <v>22</v>
@@ -6097,10 +6097,10 @@
         <v>9</v>
       </c>
       <c r="C211">
-        <v>318</v>
+        <v>439</v>
       </c>
       <c r="D211">
-        <v>444855</v>
+        <v>543925</v>
       </c>
       <c r="E211" t="s">
         <v>22</v>
@@ -6123,10 +6123,10 @@
         <v>9</v>
       </c>
       <c r="C212">
-        <v>875</v>
+        <v>328</v>
       </c>
       <c r="D212">
-        <v>1150622</v>
+        <v>458145</v>
       </c>
       <c r="E212" t="s">
         <v>22</v>
@@ -6149,10 +6149,10 @@
         <v>9</v>
       </c>
       <c r="C213">
-        <v>2612</v>
+        <v>898</v>
       </c>
       <c r="D213">
-        <v>3513063</v>
+        <v>1178794</v>
       </c>
       <c r="E213" t="s">
         <v>22</v>
@@ -6175,10 +6175,10 @@
         <v>9</v>
       </c>
       <c r="C214">
-        <v>1236</v>
+        <v>2664</v>
       </c>
       <c r="D214">
-        <v>1513916</v>
+        <v>3582151</v>
       </c>
       <c r="E214" t="s">
         <v>22</v>
@@ -6201,10 +6201,10 @@
         <v>9</v>
       </c>
       <c r="C215">
-        <v>1545</v>
+        <v>1268</v>
       </c>
       <c r="D215">
-        <v>1814031</v>
+        <v>1554617</v>
       </c>
       <c r="E215" t="s">
         <v>22</v>
@@ -6213,10 +6213,10 @@
         <v>40</v>
       </c>
       <c r="G215" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H215" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -6227,10 +6227,10 @@
         <v>9</v>
       </c>
       <c r="C216">
-        <v>2869</v>
+        <v>1562</v>
       </c>
       <c r="D216">
-        <v>3762268</v>
+        <v>1833054</v>
       </c>
       <c r="E216" t="s">
         <v>22</v>
@@ -6253,10 +6253,10 @@
         <v>9</v>
       </c>
       <c r="C217">
-        <v>1503</v>
+        <v>2914</v>
       </c>
       <c r="D217">
-        <v>1787732</v>
+        <v>3821007</v>
       </c>
       <c r="E217" t="s">
         <v>22</v>
@@ -6279,10 +6279,10 @@
         <v>9</v>
       </c>
       <c r="C218">
-        <v>6420</v>
+        <v>1551</v>
       </c>
       <c r="D218">
-        <v>7654337</v>
+        <v>1844096</v>
       </c>
       <c r="E218" t="s">
         <v>22</v>
@@ -6305,22 +6305,22 @@
         <v>9</v>
       </c>
       <c r="C219">
-        <v>2896</v>
+        <v>6478</v>
       </c>
       <c r="D219">
-        <v>3987340</v>
+        <v>7715214</v>
       </c>
       <c r="E219" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F219" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G219" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H219" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -6331,10 +6331,10 @@
         <v>9</v>
       </c>
       <c r="C220">
-        <v>13</v>
+        <v>3014</v>
       </c>
       <c r="D220">
-        <v>18428</v>
+        <v>4148078</v>
       </c>
       <c r="E220" t="s">
         <v>23</v>
@@ -6343,10 +6343,10 @@
         <v>41</v>
       </c>
       <c r="G220" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H220" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -6357,10 +6357,10 @@
         <v>9</v>
       </c>
       <c r="C221">
-        <v>4629</v>
+        <v>13</v>
       </c>
       <c r="D221">
-        <v>5600298</v>
+        <v>18428</v>
       </c>
       <c r="E221" t="s">
         <v>23</v>
@@ -6383,10 +6383,10 @@
         <v>9</v>
       </c>
       <c r="C222">
-        <v>20</v>
+        <v>4701</v>
       </c>
       <c r="D222">
-        <v>26759</v>
+        <v>5680129</v>
       </c>
       <c r="E222" t="s">
         <v>23</v>
@@ -6409,10 +6409,10 @@
         <v>9</v>
       </c>
       <c r="C223">
-        <v>223</v>
+        <v>21</v>
       </c>
       <c r="D223">
-        <v>238879</v>
+        <v>28259</v>
       </c>
       <c r="E223" t="s">
         <v>23</v>
@@ -6435,10 +6435,10 @@
         <v>9</v>
       </c>
       <c r="C224">
-        <v>12788</v>
+        <v>229</v>
       </c>
       <c r="D224">
-        <v>18204723</v>
+        <v>246443</v>
       </c>
       <c r="E224" t="s">
         <v>23</v>
@@ -6461,10 +6461,10 @@
         <v>9</v>
       </c>
       <c r="C225">
-        <v>17337</v>
+        <v>13065</v>
       </c>
       <c r="D225">
-        <v>22835659</v>
+        <v>18594134</v>
       </c>
       <c r="E225" t="s">
         <v>23</v>
@@ -6487,10 +6487,10 @@
         <v>9</v>
       </c>
       <c r="C226">
-        <v>2047</v>
+        <v>17639</v>
       </c>
       <c r="D226">
-        <v>2777544</v>
+        <v>23216158</v>
       </c>
       <c r="E226" t="s">
         <v>23</v>
@@ -6513,10 +6513,10 @@
         <v>9</v>
       </c>
       <c r="C227">
-        <v>11602</v>
+        <v>2084</v>
       </c>
       <c r="D227">
-        <v>16311148</v>
+        <v>2825110</v>
       </c>
       <c r="E227" t="s">
         <v>23</v>
@@ -6539,10 +6539,10 @@
         <v>9</v>
       </c>
       <c r="C228">
-        <v>1366</v>
+        <v>11776</v>
       </c>
       <c r="D228">
-        <v>1764891</v>
+        <v>16555790</v>
       </c>
       <c r="E228" t="s">
         <v>23</v>
@@ -6565,10 +6565,10 @@
         <v>9</v>
       </c>
       <c r="C229">
-        <v>728</v>
+        <v>1389</v>
       </c>
       <c r="D229">
-        <v>1013555</v>
+        <v>1793634</v>
       </c>
       <c r="E229" t="s">
         <v>23</v>
@@ -6591,10 +6591,10 @@
         <v>9</v>
       </c>
       <c r="C230">
-        <v>2577</v>
+        <v>747</v>
       </c>
       <c r="D230">
-        <v>3427375</v>
+        <v>1034725</v>
       </c>
       <c r="E230" t="s">
         <v>23</v>
@@ -6617,10 +6617,10 @@
         <v>9</v>
       </c>
       <c r="C231">
-        <v>7833</v>
+        <v>2646</v>
       </c>
       <c r="D231">
-        <v>10460283</v>
+        <v>3514450</v>
       </c>
       <c r="E231" t="s">
         <v>23</v>
@@ -6643,10 +6643,10 @@
         <v>9</v>
       </c>
       <c r="C232">
-        <v>4007</v>
+        <v>7979</v>
       </c>
       <c r="D232">
-        <v>4934223</v>
+        <v>10643469</v>
       </c>
       <c r="E232" t="s">
         <v>23</v>
@@ -6669,10 +6669,10 @@
         <v>9</v>
       </c>
       <c r="C233">
-        <v>4405</v>
+        <v>4078</v>
       </c>
       <c r="D233">
-        <v>5045667</v>
+        <v>5020155</v>
       </c>
       <c r="E233" t="s">
         <v>23</v>
@@ -6681,10 +6681,10 @@
         <v>41</v>
       </c>
       <c r="G233" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H233" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -6695,10 +6695,10 @@
         <v>9</v>
       </c>
       <c r="C234">
-        <v>9514</v>
+        <v>4480</v>
       </c>
       <c r="D234">
-        <v>12431642</v>
+        <v>5124447</v>
       </c>
       <c r="E234" t="s">
         <v>23</v>
@@ -6721,10 +6721,10 @@
         <v>9</v>
       </c>
       <c r="C235">
-        <v>3737</v>
+        <v>9665</v>
       </c>
       <c r="D235">
-        <v>4378273</v>
+        <v>12615862</v>
       </c>
       <c r="E235" t="s">
         <v>23</v>
@@ -6747,10 +6747,10 @@
         <v>9</v>
       </c>
       <c r="C236">
-        <v>14107</v>
+        <v>3834</v>
       </c>
       <c r="D236">
-        <v>16722758</v>
+        <v>4487248</v>
       </c>
       <c r="E236" t="s">
         <v>23</v>
@@ -6773,22 +6773,22 @@
         <v>9</v>
       </c>
       <c r="C237">
-        <v>2948</v>
+        <v>14250</v>
       </c>
       <c r="D237">
-        <v>3957729</v>
+        <v>16876226</v>
       </c>
       <c r="E237" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F237" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G237" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H237" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -6799,10 +6799,10 @@
         <v>9</v>
       </c>
       <c r="C238">
-        <v>10</v>
+        <v>3051</v>
       </c>
       <c r="D238">
-        <v>15000</v>
+        <v>4095726</v>
       </c>
       <c r="E238" t="s">
         <v>24</v>
@@ -6811,10 +6811,10 @@
         <v>42</v>
       </c>
       <c r="G238" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H238" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -6825,10 +6825,10 @@
         <v>9</v>
       </c>
       <c r="C239">
-        <v>4707</v>
+        <v>10</v>
       </c>
       <c r="D239">
-        <v>5664045</v>
+        <v>15000</v>
       </c>
       <c r="E239" t="s">
         <v>24</v>
@@ -6851,10 +6851,10 @@
         <v>9</v>
       </c>
       <c r="C240">
-        <v>21</v>
+        <v>4803</v>
       </c>
       <c r="D240">
-        <v>28259</v>
+        <v>5780930</v>
       </c>
       <c r="E240" t="s">
         <v>24</v>
@@ -6877,10 +6877,10 @@
         <v>9</v>
       </c>
       <c r="C241">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="D241">
-        <v>189534</v>
+        <v>31259</v>
       </c>
       <c r="E241" t="s">
         <v>24</v>
@@ -6903,10 +6903,10 @@
         <v>9</v>
       </c>
       <c r="C242">
-        <v>15744</v>
+        <v>159</v>
       </c>
       <c r="D242">
-        <v>22288613</v>
+        <v>199480</v>
       </c>
       <c r="E242" t="s">
         <v>24</v>
@@ -6929,10 +6929,10 @@
         <v>9</v>
       </c>
       <c r="C243">
-        <v>19047</v>
+        <v>16097</v>
       </c>
       <c r="D243">
-        <v>24840908</v>
+        <v>22786142</v>
       </c>
       <c r="E243" t="s">
         <v>24</v>
@@ -6955,10 +6955,10 @@
         <v>9</v>
       </c>
       <c r="C244">
-        <v>2225</v>
+        <v>19410</v>
       </c>
       <c r="D244">
-        <v>2935508</v>
+        <v>25291261</v>
       </c>
       <c r="E244" t="s">
         <v>24</v>
@@ -6981,10 +6981,10 @@
         <v>9</v>
       </c>
       <c r="C245">
-        <v>13499</v>
+        <v>2270</v>
       </c>
       <c r="D245">
-        <v>18973502</v>
+        <v>2993300</v>
       </c>
       <c r="E245" t="s">
         <v>24</v>
@@ -7007,10 +7007,10 @@
         <v>9</v>
       </c>
       <c r="C246">
-        <v>1496</v>
+        <v>13713</v>
       </c>
       <c r="D246">
-        <v>1889961</v>
+        <v>19273087</v>
       </c>
       <c r="E246" t="s">
         <v>24</v>
@@ -7033,10 +7033,10 @@
         <v>9</v>
       </c>
       <c r="C247">
-        <v>784</v>
+        <v>1527</v>
       </c>
       <c r="D247">
-        <v>1080788</v>
+        <v>1928974</v>
       </c>
       <c r="E247" t="s">
         <v>24</v>
@@ -7059,10 +7059,10 @@
         <v>9</v>
       </c>
       <c r="C248">
-        <v>2987</v>
+        <v>804</v>
       </c>
       <c r="D248">
-        <v>3988323</v>
+        <v>1108717</v>
       </c>
       <c r="E248" t="s">
         <v>24</v>
@@ -7085,10 +7085,10 @@
         <v>9</v>
       </c>
       <c r="C249">
-        <v>8653</v>
+        <v>3076</v>
       </c>
       <c r="D249">
-        <v>11681686</v>
+        <v>4095641</v>
       </c>
       <c r="E249" t="s">
         <v>24</v>
@@ -7111,10 +7111,10 @@
         <v>9</v>
       </c>
       <c r="C250">
-        <v>4321</v>
+        <v>8830</v>
       </c>
       <c r="D250">
-        <v>5328333</v>
+        <v>11918109</v>
       </c>
       <c r="E250" t="s">
         <v>24</v>
@@ -7137,10 +7137,10 @@
         <v>9</v>
       </c>
       <c r="C251">
-        <v>5255</v>
+        <v>4410</v>
       </c>
       <c r="D251">
-        <v>6005360</v>
+        <v>5432057</v>
       </c>
       <c r="E251" t="s">
         <v>24</v>
@@ -7149,10 +7149,10 @@
         <v>42</v>
       </c>
       <c r="G251" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H251" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -7163,10 +7163,10 @@
         <v>9</v>
       </c>
       <c r="C252">
-        <v>9179</v>
+        <v>5368</v>
       </c>
       <c r="D252">
-        <v>11900885</v>
+        <v>6126166</v>
       </c>
       <c r="E252" t="s">
         <v>24</v>
@@ -7189,10 +7189,10 @@
         <v>9</v>
       </c>
       <c r="C253">
-        <v>4310</v>
+        <v>9337</v>
       </c>
       <c r="D253">
-        <v>5028857</v>
+        <v>12106870</v>
       </c>
       <c r="E253" t="s">
         <v>24</v>
@@ -7215,10 +7215,10 @@
         <v>9</v>
       </c>
       <c r="C254">
-        <v>14318</v>
+        <v>4425</v>
       </c>
       <c r="D254">
-        <v>16278419</v>
+        <v>5160554</v>
       </c>
       <c r="E254" t="s">
         <v>24</v>
@@ -7241,22 +7241,22 @@
         <v>9</v>
       </c>
       <c r="C255">
-        <v>1054</v>
+        <v>14459</v>
       </c>
       <c r="D255">
-        <v>1452268</v>
+        <v>16424286</v>
       </c>
       <c r="E255" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F255" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G255" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H255" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -7267,10 +7267,10 @@
         <v>9</v>
       </c>
       <c r="C256">
-        <v>18</v>
+        <v>1096</v>
       </c>
       <c r="D256">
-        <v>18318</v>
+        <v>1513679</v>
       </c>
       <c r="E256" t="s">
         <v>25</v>
@@ -7279,10 +7279,10 @@
         <v>43</v>
       </c>
       <c r="G256" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H256" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -7293,10 +7293,10 @@
         <v>9</v>
       </c>
       <c r="C257">
-        <v>1952</v>
+        <v>20</v>
       </c>
       <c r="D257">
-        <v>2374222</v>
+        <v>20468</v>
       </c>
       <c r="E257" t="s">
         <v>25</v>
@@ -7319,10 +7319,10 @@
         <v>9</v>
       </c>
       <c r="C258">
-        <v>4</v>
+        <v>1980</v>
       </c>
       <c r="D258">
-        <v>4758</v>
+        <v>2405582</v>
       </c>
       <c r="E258" t="s">
         <v>25</v>
@@ -7345,10 +7345,10 @@
         <v>9</v>
       </c>
       <c r="C259">
-        <v>107</v>
+        <v>4</v>
       </c>
       <c r="D259">
-        <v>139457</v>
+        <v>4758</v>
       </c>
       <c r="E259" t="s">
         <v>25</v>
@@ -7371,10 +7371,10 @@
         <v>9</v>
       </c>
       <c r="C260">
-        <v>5037</v>
+        <v>111</v>
       </c>
       <c r="D260">
-        <v>7228488</v>
+        <v>143251</v>
       </c>
       <c r="E260" t="s">
         <v>25</v>
@@ -7397,10 +7397,10 @@
         <v>9</v>
       </c>
       <c r="C261">
-        <v>7884</v>
+        <v>5138</v>
       </c>
       <c r="D261">
-        <v>10317371</v>
+        <v>7368004</v>
       </c>
       <c r="E261" t="s">
         <v>25</v>
@@ -7423,10 +7423,10 @@
         <v>9</v>
       </c>
       <c r="C262">
-        <v>899</v>
+        <v>8007</v>
       </c>
       <c r="D262">
-        <v>1245912</v>
+        <v>10464641</v>
       </c>
       <c r="E262" t="s">
         <v>25</v>
@@ -7449,10 +7449,10 @@
         <v>9</v>
       </c>
       <c r="C263">
-        <v>5641</v>
+        <v>921</v>
       </c>
       <c r="D263">
-        <v>8083330</v>
+        <v>1274403</v>
       </c>
       <c r="E263" t="s">
         <v>25</v>
@@ -7475,10 +7475,10 @@
         <v>9</v>
       </c>
       <c r="C264">
-        <v>687</v>
+        <v>5739</v>
       </c>
       <c r="D264">
-        <v>867376</v>
+        <v>8218619</v>
       </c>
       <c r="E264" t="s">
         <v>25</v>
@@ -7501,10 +7501,10 @@
         <v>9</v>
       </c>
       <c r="C265">
-        <v>443</v>
+        <v>711</v>
       </c>
       <c r="D265">
-        <v>622793</v>
+        <v>896040</v>
       </c>
       <c r="E265" t="s">
         <v>25</v>
@@ -7527,10 +7527,10 @@
         <v>9</v>
       </c>
       <c r="C266">
-        <v>1309</v>
+        <v>451</v>
       </c>
       <c r="D266">
-        <v>1758489</v>
+        <v>634547</v>
       </c>
       <c r="E266" t="s">
         <v>25</v>
@@ -7553,10 +7553,10 @@
         <v>9</v>
       </c>
       <c r="C267">
-        <v>3990</v>
+        <v>1341</v>
       </c>
       <c r="D267">
-        <v>5394075</v>
+        <v>1796995</v>
       </c>
       <c r="E267" t="s">
         <v>25</v>
@@ -7579,10 +7579,10 @@
         <v>9</v>
       </c>
       <c r="C268">
-        <v>1533</v>
+        <v>4065</v>
       </c>
       <c r="D268">
-        <v>1949682</v>
+        <v>5493789</v>
       </c>
       <c r="E268" t="s">
         <v>25</v>
@@ -7605,10 +7605,10 @@
         <v>9</v>
       </c>
       <c r="C269">
-        <v>1932</v>
+        <v>1567</v>
       </c>
       <c r="D269">
-        <v>2292046</v>
+        <v>1990219</v>
       </c>
       <c r="E269" t="s">
         <v>25</v>
@@ -7617,10 +7617,10 @@
         <v>43</v>
       </c>
       <c r="G269" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H269" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="270" spans="1:8">
@@ -7631,10 +7631,10 @@
         <v>9</v>
       </c>
       <c r="C270">
-        <v>5137</v>
+        <v>1968</v>
       </c>
       <c r="D270">
-        <v>6740822</v>
+        <v>2332623</v>
       </c>
       <c r="E270" t="s">
         <v>25</v>
@@ -7657,10 +7657,10 @@
         <v>9</v>
       </c>
       <c r="C271">
-        <v>2037</v>
+        <v>5221</v>
       </c>
       <c r="D271">
-        <v>2405988</v>
+        <v>6844568</v>
       </c>
       <c r="E271" t="s">
         <v>25</v>
@@ -7683,10 +7683,10 @@
         <v>9</v>
       </c>
       <c r="C272">
-        <v>7364</v>
+        <v>2088</v>
       </c>
       <c r="D272">
-        <v>8970454</v>
+        <v>2466278</v>
       </c>
       <c r="E272" t="s">
         <v>25</v>
@@ -7709,22 +7709,22 @@
         <v>9</v>
       </c>
       <c r="C273">
-        <v>1422</v>
+        <v>7427</v>
       </c>
       <c r="D273">
-        <v>1927505</v>
+        <v>9028454</v>
       </c>
       <c r="E273" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F273" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G273" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H273" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="274" spans="1:8">
@@ -7735,10 +7735,10 @@
         <v>9</v>
       </c>
       <c r="C274">
-        <v>3</v>
+        <v>1477</v>
       </c>
       <c r="D274">
-        <v>4500</v>
+        <v>1998138</v>
       </c>
       <c r="E274" t="s">
         <v>26</v>
@@ -7747,10 +7747,10 @@
         <v>44</v>
       </c>
       <c r="G274" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H274" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="275" spans="1:8">
@@ -7761,10 +7761,10 @@
         <v>9</v>
       </c>
       <c r="C275">
-        <v>4611</v>
+        <v>3</v>
       </c>
       <c r="D275">
-        <v>5889794</v>
+        <v>4500</v>
       </c>
       <c r="E275" t="s">
         <v>26</v>
@@ -7787,10 +7787,10 @@
         <v>9</v>
       </c>
       <c r="C276">
-        <v>15</v>
+        <v>4698</v>
       </c>
       <c r="D276">
-        <v>22309</v>
+        <v>5996569</v>
       </c>
       <c r="E276" t="s">
         <v>26</v>
@@ -7813,10 +7813,10 @@
         <v>9</v>
       </c>
       <c r="C277">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="D277">
-        <v>99193</v>
+        <v>22309</v>
       </c>
       <c r="E277" t="s">
         <v>26</v>
@@ -7839,10 +7839,10 @@
         <v>9</v>
       </c>
       <c r="C278">
-        <v>13604</v>
+        <v>84</v>
       </c>
       <c r="D278">
-        <v>19388460</v>
+        <v>105388</v>
       </c>
       <c r="E278" t="s">
         <v>26</v>
@@ -7865,10 +7865,10 @@
         <v>9</v>
       </c>
       <c r="C279">
-        <v>20454</v>
+        <v>13950</v>
       </c>
       <c r="D279">
-        <v>27088689</v>
+        <v>19881684</v>
       </c>
       <c r="E279" t="s">
         <v>26</v>
@@ -7891,10 +7891,10 @@
         <v>9</v>
       </c>
       <c r="C280">
-        <v>4000</v>
+        <v>20802</v>
       </c>
       <c r="D280">
-        <v>5525650</v>
+        <v>27541174</v>
       </c>
       <c r="E280" t="s">
         <v>26</v>
@@ -7917,10 +7917,10 @@
         <v>9</v>
       </c>
       <c r="C281">
-        <v>13108</v>
+        <v>4070</v>
       </c>
       <c r="D281">
-        <v>18810991</v>
+        <v>5621955</v>
       </c>
       <c r="E281" t="s">
         <v>26</v>
@@ -7943,10 +7943,10 @@
         <v>9</v>
       </c>
       <c r="C282">
-        <v>1731</v>
+        <v>13367</v>
       </c>
       <c r="D282">
-        <v>2243741</v>
+        <v>19181470</v>
       </c>
       <c r="E282" t="s">
         <v>26</v>
@@ -7969,10 +7969,10 @@
         <v>9</v>
       </c>
       <c r="C283">
-        <v>863</v>
+        <v>1768</v>
       </c>
       <c r="D283">
-        <v>1213421</v>
+        <v>2288970</v>
       </c>
       <c r="E283" t="s">
         <v>26</v>
@@ -7995,10 +7995,10 @@
         <v>9</v>
       </c>
       <c r="C284">
-        <v>3676</v>
+        <v>876</v>
       </c>
       <c r="D284">
-        <v>5071809</v>
+        <v>1232821</v>
       </c>
       <c r="E284" t="s">
         <v>26</v>
@@ -8021,10 +8021,10 @@
         <v>9</v>
       </c>
       <c r="C285">
-        <v>9562</v>
+        <v>3763</v>
       </c>
       <c r="D285">
-        <v>12963772</v>
+        <v>5190124</v>
       </c>
       <c r="E285" t="s">
         <v>26</v>
@@ -8047,10 +8047,10 @@
         <v>9</v>
       </c>
       <c r="C286">
-        <v>5272</v>
+        <v>9767</v>
       </c>
       <c r="D286">
-        <v>6736270</v>
+        <v>13239307</v>
       </c>
       <c r="E286" t="s">
         <v>26</v>
@@ -8073,10 +8073,10 @@
         <v>9</v>
       </c>
       <c r="C287">
-        <v>5842</v>
+        <v>5357</v>
       </c>
       <c r="D287">
-        <v>7004697</v>
+        <v>6842557</v>
       </c>
       <c r="E287" t="s">
         <v>26</v>
@@ -8085,10 +8085,10 @@
         <v>44</v>
       </c>
       <c r="G287" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H287" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="288" spans="1:8">
@@ -8099,10 +8099,10 @@
         <v>9</v>
       </c>
       <c r="C288">
-        <v>9209</v>
+        <v>5944</v>
       </c>
       <c r="D288">
-        <v>12071767</v>
+        <v>7114542</v>
       </c>
       <c r="E288" t="s">
         <v>26</v>
@@ -8125,10 +8125,10 @@
         <v>9</v>
       </c>
       <c r="C289">
-        <v>4231</v>
+        <v>9375</v>
       </c>
       <c r="D289">
-        <v>5160630</v>
+        <v>12281980</v>
       </c>
       <c r="E289" t="s">
         <v>26</v>
@@ -8151,10 +8151,10 @@
         <v>9</v>
       </c>
       <c r="C290">
-        <v>13641</v>
+        <v>4336</v>
       </c>
       <c r="D290">
-        <v>15907442</v>
+        <v>5280842</v>
       </c>
       <c r="E290" t="s">
         <v>26</v>
@@ -8177,22 +8177,22 @@
         <v>9</v>
       </c>
       <c r="C291">
-        <v>229</v>
+        <v>13815</v>
       </c>
       <c r="D291">
-        <v>311974</v>
+        <v>16096818</v>
       </c>
       <c r="E291" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F291" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G291" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H291" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="292" spans="1:8">
@@ -8203,10 +8203,10 @@
         <v>9</v>
       </c>
       <c r="C292">
-        <v>5145</v>
+        <v>235</v>
       </c>
       <c r="D292">
-        <v>6810148</v>
+        <v>320807</v>
       </c>
       <c r="E292" t="s">
         <v>27</v>
@@ -8215,10 +8215,10 @@
         <v>45</v>
       </c>
       <c r="G292" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H292" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="293" spans="1:8">
@@ -8229,10 +8229,10 @@
         <v>9</v>
       </c>
       <c r="C293">
-        <v>38</v>
+        <v>5290</v>
       </c>
       <c r="D293">
-        <v>54365</v>
+        <v>7003512</v>
       </c>
       <c r="E293" t="s">
         <v>27</v>
@@ -8255,10 +8255,10 @@
         <v>9</v>
       </c>
       <c r="C294">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="D294">
-        <v>188969</v>
+        <v>55865</v>
       </c>
       <c r="E294" t="s">
         <v>27</v>
@@ -8281,10 +8281,10 @@
         <v>9</v>
       </c>
       <c r="C295">
-        <v>15481</v>
+        <v>145</v>
       </c>
       <c r="D295">
-        <v>22324124</v>
+        <v>194045</v>
       </c>
       <c r="E295" t="s">
         <v>27</v>
@@ -8307,10 +8307,10 @@
         <v>9</v>
       </c>
       <c r="C296">
-        <v>28148</v>
+        <v>15997</v>
       </c>
       <c r="D296">
-        <v>38477653</v>
+        <v>23079776</v>
       </c>
       <c r="E296" t="s">
         <v>27</v>
@@ -8333,10 +8333,10 @@
         <v>9</v>
       </c>
       <c r="C297">
-        <v>26610</v>
+        <v>28879</v>
       </c>
       <c r="D297">
-        <v>38155064</v>
+        <v>39477641</v>
       </c>
       <c r="E297" t="s">
         <v>27</v>
@@ -8359,10 +8359,10 @@
         <v>9</v>
       </c>
       <c r="C298">
-        <v>17974</v>
+        <v>27098</v>
       </c>
       <c r="D298">
-        <v>26437239</v>
+        <v>38845807</v>
       </c>
       <c r="E298" t="s">
         <v>27</v>
@@ -8385,10 +8385,10 @@
         <v>9</v>
       </c>
       <c r="C299">
-        <v>7347</v>
+        <v>18486</v>
       </c>
       <c r="D299">
-        <v>10049764</v>
+        <v>27197292</v>
       </c>
       <c r="E299" t="s">
         <v>27</v>
@@ -8411,10 +8411,10 @@
         <v>9</v>
       </c>
       <c r="C300">
-        <v>1912</v>
+        <v>7561</v>
       </c>
       <c r="D300">
-        <v>2735879</v>
+        <v>10337093</v>
       </c>
       <c r="E300" t="s">
         <v>27</v>
@@ -8437,10 +8437,10 @@
         <v>9</v>
       </c>
       <c r="C301">
-        <v>4777</v>
+        <v>1979</v>
       </c>
       <c r="D301">
-        <v>6795414</v>
+        <v>2831923</v>
       </c>
       <c r="E301" t="s">
         <v>27</v>
@@ -8463,10 +8463,10 @@
         <v>9</v>
       </c>
       <c r="C302">
-        <v>28996</v>
+        <v>4923</v>
       </c>
       <c r="D302">
-        <v>39929847</v>
+        <v>7001776</v>
       </c>
       <c r="E302" t="s">
         <v>27</v>
@@ -8489,10 +8489,10 @@
         <v>9</v>
       </c>
       <c r="C303">
-        <v>7623</v>
+        <v>29687</v>
       </c>
       <c r="D303">
-        <v>10125530</v>
+        <v>40869342</v>
       </c>
       <c r="E303" t="s">
         <v>27</v>
@@ -8515,10 +8515,10 @@
         <v>9</v>
       </c>
       <c r="C304">
-        <v>3</v>
+        <v>7818</v>
       </c>
       <c r="D304">
-        <v>3475</v>
+        <v>10387559</v>
       </c>
       <c r="E304" t="s">
         <v>27</v>
@@ -8541,10 +8541,10 @@
         <v>9</v>
       </c>
       <c r="C305">
-        <v>8215</v>
+        <v>3</v>
       </c>
       <c r="D305">
-        <v>9985338</v>
+        <v>3475</v>
       </c>
       <c r="E305" t="s">
         <v>27</v>
@@ -8567,10 +8567,10 @@
         <v>9</v>
       </c>
       <c r="C306">
-        <v>15178</v>
+        <v>8380</v>
       </c>
       <c r="D306">
-        <v>20349745</v>
+        <v>10184148</v>
       </c>
       <c r="E306" t="s">
         <v>27</v>
@@ -8593,10 +8593,10 @@
         <v>9</v>
       </c>
       <c r="C307">
-        <v>11022</v>
+        <v>15484</v>
       </c>
       <c r="D307">
-        <v>14084598</v>
+        <v>20744850</v>
       </c>
       <c r="E307" t="s">
         <v>27</v>
@@ -8619,10 +8619,10 @@
         <v>9</v>
       </c>
       <c r="C308">
-        <v>17899</v>
+        <v>11291</v>
       </c>
       <c r="D308">
-        <v>22959402</v>
+        <v>14415786</v>
       </c>
       <c r="E308" t="s">
         <v>27</v>
@@ -8635,6 +8635,32 @@
       </c>
       <c r="H308" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8">
+      <c r="A309" t="s">
+        <v>8</v>
+      </c>
+      <c r="B309" t="s">
+        <v>9</v>
+      </c>
+      <c r="C309">
+        <v>18267</v>
+      </c>
+      <c r="D309">
+        <v>23431285</v>
+      </c>
+      <c r="E309" t="s">
+        <v>27</v>
+      </c>
+      <c r="F309" t="s">
+        <v>45</v>
+      </c>
+      <c r="G309" t="s">
+        <v>64</v>
+      </c>
+      <c r="H309" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-05-03 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-naf.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-naf.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="84">
   <si>
     <t>dispositif</t>
   </si>
@@ -229,7 +229,7 @@
     <t>Construction</t>
   </si>
   <si>
-    <t>Commerce ; réparation d'automobiles et de motocycles</t>
+    <t>Commerce</t>
   </si>
   <si>
     <t>Transports et entreposage</t>
@@ -623,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H313"/>
+  <dimension ref="A1:H314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,10 +663,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>3104</v>
+        <v>3278</v>
       </c>
       <c r="D2">
-        <v>4207193</v>
+        <v>4441450</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -715,10 +715,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>6852</v>
+        <v>7587</v>
       </c>
       <c r="D4">
-        <v>8672296</v>
+        <v>9608658</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -741,10 +741,10 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D5">
-        <v>49522</v>
+        <v>53995</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -767,10 +767,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>340</v>
+        <v>372</v>
       </c>
       <c r="D6">
-        <v>418706</v>
+        <v>461954</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -793,10 +793,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>19612</v>
+        <v>21367</v>
       </c>
       <c r="D7">
-        <v>28276291</v>
+        <v>30811050</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -819,10 +819,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>25909</v>
+        <v>28583</v>
       </c>
       <c r="D8">
-        <v>34663229</v>
+        <v>38348688</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -845,10 +845,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>5223</v>
+        <v>5818</v>
       </c>
       <c r="D9">
-        <v>7251358</v>
+        <v>8080271</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -871,10 +871,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>20494</v>
+        <v>22278</v>
       </c>
       <c r="D10">
-        <v>29475680</v>
+        <v>32074313</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -897,10 +897,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>2596</v>
+        <v>2889</v>
       </c>
       <c r="D11">
-        <v>3397674</v>
+        <v>3787019</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -923,10 +923,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>1220</v>
+        <v>1327</v>
       </c>
       <c r="D12">
-        <v>1727624</v>
+        <v>1873320</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -949,10 +949,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>4457</v>
+        <v>4940</v>
       </c>
       <c r="D13">
-        <v>6120804</v>
+        <v>6800742</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -975,10 +975,10 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>13752</v>
+        <v>15278</v>
       </c>
       <c r="D14">
-        <v>18606588</v>
+        <v>20676082</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1001,10 +1001,10 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>6607</v>
+        <v>7350</v>
       </c>
       <c r="D15">
-        <v>8524692</v>
+        <v>9499799</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1053,10 +1053,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>14669</v>
+        <v>16576</v>
       </c>
       <c r="D17">
-        <v>18704687</v>
+        <v>21249746</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1079,10 +1079,10 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>16676</v>
+        <v>18937</v>
       </c>
       <c r="D18">
-        <v>22327408</v>
+        <v>25473512</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1105,10 +1105,10 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>7103</v>
+        <v>7982</v>
       </c>
       <c r="D19">
-        <v>8644744</v>
+        <v>9760161</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1131,10 +1131,10 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>21959</v>
+        <v>24436</v>
       </c>
       <c r="D20">
-        <v>26912526</v>
+        <v>30072010</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1157,10 +1157,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>1132</v>
+        <v>1207</v>
       </c>
       <c r="D21">
-        <v>1539522</v>
+        <v>1642208</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1209,10 +1209,10 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>1980</v>
+        <v>2142</v>
       </c>
       <c r="D23">
-        <v>2434241</v>
+        <v>2627953</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -1235,10 +1235,10 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -1261,10 +1261,10 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D25">
-        <v>189949</v>
+        <v>208030</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
@@ -1287,10 +1287,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>4897</v>
+        <v>5294</v>
       </c>
       <c r="D26">
-        <v>7036791</v>
+        <v>7599416</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1313,10 +1313,10 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>8313</v>
+        <v>9180</v>
       </c>
       <c r="D27">
-        <v>11041190</v>
+        <v>12221314</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -1339,10 +1339,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>691</v>
+        <v>776</v>
       </c>
       <c r="D28">
-        <v>937726</v>
+        <v>1050834</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1365,10 +1365,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>6087</v>
+        <v>6633</v>
       </c>
       <c r="D29">
-        <v>8670853</v>
+        <v>9459020</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
@@ -1391,10 +1391,10 @@
         <v>9</v>
       </c>
       <c r="C30">
-        <v>515</v>
+        <v>558</v>
       </c>
       <c r="D30">
-        <v>636578</v>
+        <v>693786</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
@@ -1417,10 +1417,10 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>311</v>
+        <v>348</v>
       </c>
       <c r="D31">
-        <v>416684</v>
+        <v>469871</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -1443,10 +1443,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>1030</v>
+        <v>1126</v>
       </c>
       <c r="D32">
-        <v>1375353</v>
+        <v>1505837</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
@@ -1469,10 +1469,10 @@
         <v>9</v>
       </c>
       <c r="C33">
-        <v>2729</v>
+        <v>3006</v>
       </c>
       <c r="D33">
-        <v>3668881</v>
+        <v>4053400</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1495,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>1470</v>
+        <v>1621</v>
       </c>
       <c r="D34">
-        <v>1848614</v>
+        <v>2045895</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -1547,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>2105</v>
+        <v>2346</v>
       </c>
       <c r="D36">
-        <v>2501883</v>
+        <v>2816925</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -1573,10 +1573,10 @@
         <v>9</v>
       </c>
       <c r="C37">
-        <v>3667</v>
+        <v>4160</v>
       </c>
       <c r="D37">
-        <v>4908165</v>
+        <v>5571047</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>
@@ -1599,10 +1599,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>1764</v>
+        <v>1954</v>
       </c>
       <c r="D38">
-        <v>2089118</v>
+        <v>2320802</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
@@ -1625,10 +1625,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>6903</v>
+        <v>7713</v>
       </c>
       <c r="D39">
-        <v>8575179</v>
+        <v>9631322</v>
       </c>
       <c r="E39" t="s">
         <v>11</v>
@@ -1651,10 +1651,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>1030</v>
+        <v>1096</v>
       </c>
       <c r="D40">
-        <v>1403344</v>
+        <v>1495061</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -1703,10 +1703,10 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>2535</v>
+        <v>2811</v>
       </c>
       <c r="D42">
-        <v>3014793</v>
+        <v>3365143</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -1729,10 +1729,10 @@
         <v>9</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>8842</v>
+        <v>10342</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1755,10 +1755,10 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D44">
-        <v>121542</v>
+        <v>138201</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -1781,10 +1781,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>5426</v>
+        <v>5911</v>
       </c>
       <c r="D45">
-        <v>7790920</v>
+        <v>8478948</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1807,10 +1807,10 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>9156</v>
+        <v>10058</v>
       </c>
       <c r="D46">
-        <v>12305577</v>
+        <v>13544853</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -1833,10 +1833,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>906</v>
+        <v>1036</v>
       </c>
       <c r="D47">
-        <v>1213436</v>
+        <v>1394176</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -1859,10 +1859,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>8118</v>
+        <v>8850</v>
       </c>
       <c r="D48">
-        <v>11637172</v>
+        <v>12700210</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -1885,10 +1885,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>755</v>
+        <v>854</v>
       </c>
       <c r="D49">
-        <v>954748</v>
+        <v>1070575</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -1911,10 +1911,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>372</v>
+        <v>394</v>
       </c>
       <c r="D50">
-        <v>524055</v>
+        <v>555951</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -1937,10 +1937,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>1406</v>
+        <v>1561</v>
       </c>
       <c r="D51">
-        <v>1855516</v>
+        <v>2055551</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -1963,10 +1963,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>4026</v>
+        <v>4461</v>
       </c>
       <c r="D52">
-        <v>5402089</v>
+        <v>5997926</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -1989,10 +1989,10 @@
         <v>9</v>
       </c>
       <c r="C53">
-        <v>1812</v>
+        <v>2002</v>
       </c>
       <c r="D53">
-        <v>2240095</v>
+        <v>2487581</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -2015,10 +2015,10 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>2259</v>
+        <v>2535</v>
       </c>
       <c r="D54">
-        <v>2754076</v>
+        <v>3100403</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
@@ -2041,10 +2041,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>5937</v>
+        <v>6758</v>
       </c>
       <c r="D55">
-        <v>8026357</v>
+        <v>9173306</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2067,10 +2067,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>2112</v>
+        <v>2400</v>
       </c>
       <c r="D56">
-        <v>2487131</v>
+        <v>2846497</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2093,10 +2093,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>7707</v>
+        <v>8551</v>
       </c>
       <c r="D57">
-        <v>9600216</v>
+        <v>10704206</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2119,10 +2119,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>797</v>
+        <v>853</v>
       </c>
       <c r="D58">
-        <v>1088116</v>
+        <v>1166613</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -2145,10 +2145,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>1590</v>
+        <v>1751</v>
       </c>
       <c r="D59">
-        <v>2003263</v>
+        <v>2203280</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
@@ -2197,10 +2197,10 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D61">
-        <v>85717</v>
+        <v>99170</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -2223,10 +2223,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>4847</v>
+        <v>5274</v>
       </c>
       <c r="D62">
-        <v>6921475</v>
+        <v>7533339</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -2249,10 +2249,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>6797</v>
+        <v>7487</v>
       </c>
       <c r="D63">
-        <v>8912243</v>
+        <v>9829085</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -2275,10 +2275,10 @@
         <v>9</v>
       </c>
       <c r="C64">
-        <v>828</v>
+        <v>939</v>
       </c>
       <c r="D64">
-        <v>1163152</v>
+        <v>1320317</v>
       </c>
       <c r="E64" t="s">
         <v>13</v>
@@ -2301,10 +2301,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>4780</v>
+        <v>5239</v>
       </c>
       <c r="D65">
-        <v>6823433</v>
+        <v>7495893</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -2327,10 +2327,10 @@
         <v>9</v>
       </c>
       <c r="C66">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="D66">
-        <v>646859</v>
+        <v>740402</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -2353,10 +2353,10 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>259</v>
+        <v>294</v>
       </c>
       <c r="D67">
-        <v>367674</v>
+        <v>417445</v>
       </c>
       <c r="E67" t="s">
         <v>13</v>
@@ -2379,10 +2379,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>1034</v>
+        <v>1167</v>
       </c>
       <c r="D68">
-        <v>1385767</v>
+        <v>1574723</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -2405,10 +2405,10 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>2552</v>
+        <v>2854</v>
       </c>
       <c r="D69">
-        <v>3412565</v>
+        <v>3832721</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -2431,10 +2431,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>1396</v>
+        <v>1546</v>
       </c>
       <c r="D70">
-        <v>1745772</v>
+        <v>1945204</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -2457,10 +2457,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>1676</v>
+        <v>1877</v>
       </c>
       <c r="D71">
-        <v>2075824</v>
+        <v>2338673</v>
       </c>
       <c r="E71" t="s">
         <v>13</v>
@@ -2483,10 +2483,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>3095</v>
+        <v>3529</v>
       </c>
       <c r="D72">
-        <v>4098171</v>
+        <v>4699647</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -2509,10 +2509,10 @@
         <v>9</v>
       </c>
       <c r="C73">
-        <v>1603</v>
+        <v>1804</v>
       </c>
       <c r="D73">
-        <v>1928830</v>
+        <v>2179349</v>
       </c>
       <c r="E73" t="s">
         <v>13</v>
@@ -2535,10 +2535,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>6230</v>
+        <v>6939</v>
       </c>
       <c r="D74">
-        <v>7728934</v>
+        <v>8651126</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -2561,10 +2561,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>713</v>
+        <v>766</v>
       </c>
       <c r="D75">
-        <v>983899</v>
+        <v>1055323</v>
       </c>
       <c r="E75" t="s">
         <v>14</v>
@@ -2587,10 +2587,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>619</v>
+        <v>686</v>
       </c>
       <c r="D76">
-        <v>812019</v>
+        <v>902916</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
@@ -2639,10 +2639,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>1559</v>
+        <v>1704</v>
       </c>
       <c r="D78">
-        <v>2216484</v>
+        <v>2427054</v>
       </c>
       <c r="E78" t="s">
         <v>14</v>
@@ -2665,10 +2665,10 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>1598</v>
+        <v>1772</v>
       </c>
       <c r="D79">
-        <v>2203069</v>
+        <v>2445768</v>
       </c>
       <c r="E79" t="s">
         <v>14</v>
@@ -2691,10 +2691,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="D80">
-        <v>307478</v>
+        <v>330520</v>
       </c>
       <c r="E80" t="s">
         <v>14</v>
@@ -2717,10 +2717,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>1426</v>
+        <v>1581</v>
       </c>
       <c r="D81">
-        <v>2029122</v>
+        <v>2256448</v>
       </c>
       <c r="E81" t="s">
         <v>14</v>
@@ -2743,10 +2743,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="D82">
-        <v>135383</v>
+        <v>154938</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2769,10 +2769,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D83">
-        <v>61379</v>
+        <v>63418</v>
       </c>
       <c r="E83" t="s">
         <v>14</v>
@@ -2795,10 +2795,10 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="D84">
-        <v>440571</v>
+        <v>477088</v>
       </c>
       <c r="E84" t="s">
         <v>14</v>
@@ -2821,10 +2821,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>1057</v>
+        <v>1166</v>
       </c>
       <c r="D85">
-        <v>1470236</v>
+        <v>1625273</v>
       </c>
       <c r="E85" t="s">
         <v>14</v>
@@ -2847,10 +2847,10 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>626</v>
+        <v>690</v>
       </c>
       <c r="D86">
-        <v>785626</v>
+        <v>871863</v>
       </c>
       <c r="E86" t="s">
         <v>14</v>
@@ -2873,10 +2873,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>332</v>
+        <v>366</v>
       </c>
       <c r="D87">
-        <v>406920</v>
+        <v>447584</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -2899,10 +2899,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>622</v>
+        <v>681</v>
       </c>
       <c r="D88">
-        <v>825422</v>
+        <v>908027</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -2925,10 +2925,10 @@
         <v>9</v>
       </c>
       <c r="C89">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="D89">
-        <v>400209</v>
+        <v>435737</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
@@ -2951,10 +2951,10 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>1132</v>
+        <v>1248</v>
       </c>
       <c r="D90">
-        <v>1333193</v>
+        <v>1474749</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
@@ -2977,10 +2977,10 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>1455</v>
+        <v>1549</v>
       </c>
       <c r="D91">
-        <v>2004807</v>
+        <v>2128555</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -3029,10 +3029,10 @@
         <v>9</v>
       </c>
       <c r="C93">
-        <v>3322</v>
+        <v>3620</v>
       </c>
       <c r="D93">
-        <v>4254233</v>
+        <v>4639536</v>
       </c>
       <c r="E93" t="s">
         <v>15</v>
@@ -3055,10 +3055,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D94">
-        <v>6310</v>
+        <v>10810</v>
       </c>
       <c r="E94" t="s">
         <v>15</v>
@@ -3081,10 +3081,10 @@
         <v>9</v>
       </c>
       <c r="C95">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="D95">
-        <v>305666</v>
+        <v>330720</v>
       </c>
       <c r="E95" t="s">
         <v>15</v>
@@ -3107,10 +3107,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>10016</v>
+        <v>10931</v>
       </c>
       <c r="D96">
-        <v>14449661</v>
+        <v>15769669</v>
       </c>
       <c r="E96" t="s">
         <v>15</v>
@@ -3133,10 +3133,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>14827</v>
+        <v>16182</v>
       </c>
       <c r="D97">
-        <v>19854949</v>
+        <v>21697141</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
@@ -3159,10 +3159,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>1891</v>
+        <v>2117</v>
       </c>
       <c r="D98">
-        <v>2583459</v>
+        <v>2900319</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -3185,10 +3185,10 @@
         <v>9</v>
       </c>
       <c r="C99">
-        <v>9877</v>
+        <v>10679</v>
       </c>
       <c r="D99">
-        <v>14280495</v>
+        <v>15444833</v>
       </c>
       <c r="E99" t="s">
         <v>15</v>
@@ -3211,10 +3211,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>1102</v>
+        <v>1220</v>
       </c>
       <c r="D100">
-        <v>1407001</v>
+        <v>1558243</v>
       </c>
       <c r="E100" t="s">
         <v>15</v>
@@ -3237,10 +3237,10 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>629</v>
+        <v>693</v>
       </c>
       <c r="D101">
-        <v>875279</v>
+        <v>968654</v>
       </c>
       <c r="E101" t="s">
         <v>15</v>
@@ -3263,10 +3263,10 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>1653</v>
+        <v>1838</v>
       </c>
       <c r="D102">
-        <v>2247632</v>
+        <v>2509642</v>
       </c>
       <c r="E102" t="s">
         <v>15</v>
@@ -3289,10 +3289,10 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>5847</v>
+        <v>6468</v>
       </c>
       <c r="D103">
-        <v>7835787</v>
+        <v>8682368</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
@@ -3315,10 +3315,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>2742</v>
+        <v>3051</v>
       </c>
       <c r="D104">
-        <v>3470809</v>
+        <v>3868592</v>
       </c>
       <c r="E104" t="s">
         <v>15</v>
@@ -3341,10 +3341,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>3457</v>
+        <v>3868</v>
       </c>
       <c r="D105">
-        <v>4204833</v>
+        <v>4725763</v>
       </c>
       <c r="E105" t="s">
         <v>15</v>
@@ -3367,10 +3367,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>7012</v>
+        <v>7901</v>
       </c>
       <c r="D106">
-        <v>9551434</v>
+        <v>10790752</v>
       </c>
       <c r="E106" t="s">
         <v>15</v>
@@ -3393,10 +3393,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>2977</v>
+        <v>3368</v>
       </c>
       <c r="D107">
-        <v>3504627</v>
+        <v>3977771</v>
       </c>
       <c r="E107" t="s">
         <v>15</v>
@@ -3419,10 +3419,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>13958</v>
+        <v>15481</v>
       </c>
       <c r="D108">
-        <v>16766240</v>
+        <v>18704620</v>
       </c>
       <c r="E108" t="s">
         <v>15</v>
@@ -3445,10 +3445,10 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>570</v>
+        <v>637</v>
       </c>
       <c r="D109">
-        <v>795668</v>
+        <v>888950</v>
       </c>
       <c r="E109" t="s">
         <v>16</v>
@@ -3471,10 +3471,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>726</v>
+        <v>794</v>
       </c>
       <c r="D110">
-        <v>1007624</v>
+        <v>1106715</v>
       </c>
       <c r="E110" t="s">
         <v>16</v>
@@ -3523,10 +3523,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D112">
-        <v>25000</v>
+        <v>28000</v>
       </c>
       <c r="E112" t="s">
         <v>16</v>
@@ -3549,10 +3549,10 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>1249</v>
+        <v>1343</v>
       </c>
       <c r="D113">
-        <v>1801081</v>
+        <v>1937450</v>
       </c>
       <c r="E113" t="s">
         <v>16</v>
@@ -3575,10 +3575,10 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>1987</v>
+        <v>2194</v>
       </c>
       <c r="D114">
-        <v>2738249</v>
+        <v>3036964</v>
       </c>
       <c r="E114" t="s">
         <v>16</v>
@@ -3601,10 +3601,10 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>488</v>
+        <v>533</v>
       </c>
       <c r="D115">
-        <v>696146</v>
+        <v>757960</v>
       </c>
       <c r="E115" t="s">
         <v>16</v>
@@ -3627,10 +3627,10 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>1182</v>
+        <v>1316</v>
       </c>
       <c r="D116">
-        <v>1686144</v>
+        <v>1881576</v>
       </c>
       <c r="E116" t="s">
         <v>16</v>
@@ -3653,10 +3653,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="D117">
-        <v>261792</v>
+        <v>288915</v>
       </c>
       <c r="E117" t="s">
         <v>16</v>
@@ -3679,10 +3679,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D118">
-        <v>90886</v>
+        <v>97706</v>
       </c>
       <c r="E118" t="s">
         <v>16</v>
@@ -3705,10 +3705,10 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>274</v>
+        <v>302</v>
       </c>
       <c r="D119">
-        <v>381717</v>
+        <v>420038</v>
       </c>
       <c r="E119" t="s">
         <v>16</v>
@@ -3731,10 +3731,10 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>797</v>
+        <v>872</v>
       </c>
       <c r="D120">
-        <v>1109001</v>
+        <v>1209946</v>
       </c>
       <c r="E120" t="s">
         <v>16</v>
@@ -3757,10 +3757,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>811</v>
+        <v>918</v>
       </c>
       <c r="D121">
-        <v>1083240</v>
+        <v>1226268</v>
       </c>
       <c r="E121" t="s">
         <v>16</v>
@@ -3783,10 +3783,10 @@
         <v>9</v>
       </c>
       <c r="C122">
-        <v>444</v>
+        <v>498</v>
       </c>
       <c r="D122">
-        <v>563916</v>
+        <v>634691</v>
       </c>
       <c r="E122" t="s">
         <v>16</v>
@@ -3809,10 +3809,10 @@
         <v>9</v>
       </c>
       <c r="C123">
-        <v>663</v>
+        <v>753</v>
       </c>
       <c r="D123">
-        <v>925278</v>
+        <v>1057231</v>
       </c>
       <c r="E123" t="s">
         <v>16</v>
@@ -3835,10 +3835,10 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>262</v>
+        <v>302</v>
       </c>
       <c r="D124">
-        <v>345790</v>
+        <v>397547</v>
       </c>
       <c r="E124" t="s">
         <v>16</v>
@@ -3861,10 +3861,10 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>834</v>
+        <v>925</v>
       </c>
       <c r="D125">
-        <v>1049437</v>
+        <v>1170932</v>
       </c>
       <c r="E125" t="s">
         <v>16</v>
@@ -3887,10 +3887,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D126">
-        <v>378626</v>
+        <v>383126</v>
       </c>
       <c r="E126" t="s">
         <v>17</v>
@@ -3913,10 +3913,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D127">
-        <v>190725</v>
+        <v>201952</v>
       </c>
       <c r="E127" t="s">
         <v>17</v>
@@ -3965,10 +3965,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="D129">
-        <v>403870</v>
+        <v>437270</v>
       </c>
       <c r="E129" t="s">
         <v>17</v>
@@ -3991,10 +3991,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>369</v>
+        <v>403</v>
       </c>
       <c r="D130">
-        <v>522586</v>
+        <v>572026</v>
       </c>
       <c r="E130" t="s">
         <v>17</v>
@@ -4017,10 +4017,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D131">
-        <v>131389</v>
+        <v>140079</v>
       </c>
       <c r="E131" t="s">
         <v>17</v>
@@ -4043,10 +4043,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D132">
-        <v>355367</v>
+        <v>384237</v>
       </c>
       <c r="E132" t="s">
         <v>17</v>
@@ -4069,10 +4069,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D133">
-        <v>51360</v>
+        <v>54360</v>
       </c>
       <c r="E133" t="s">
         <v>17</v>
@@ -4121,10 +4121,10 @@
         <v>9</v>
       </c>
       <c r="C135">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D135">
-        <v>29905</v>
+        <v>35905</v>
       </c>
       <c r="E135" t="s">
         <v>17</v>
@@ -4147,10 +4147,10 @@
         <v>9</v>
       </c>
       <c r="C136">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D136">
-        <v>258522</v>
+        <v>273522</v>
       </c>
       <c r="E136" t="s">
         <v>17</v>
@@ -4173,10 +4173,10 @@
         <v>9</v>
       </c>
       <c r="C137">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D137">
-        <v>199587</v>
+        <v>213519</v>
       </c>
       <c r="E137" t="s">
         <v>17</v>
@@ -4199,10 +4199,10 @@
         <v>9</v>
       </c>
       <c r="C138">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D138">
-        <v>136882</v>
+        <v>150336</v>
       </c>
       <c r="E138" t="s">
         <v>17</v>
@@ -4225,10 +4225,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D139">
-        <v>154725</v>
+        <v>175400</v>
       </c>
       <c r="E139" t="s">
         <v>17</v>
@@ -4251,10 +4251,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D140">
-        <v>69694</v>
+        <v>74194</v>
       </c>
       <c r="E140" t="s">
         <v>17</v>
@@ -4277,10 +4277,10 @@
         <v>9</v>
       </c>
       <c r="C141">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D141">
-        <v>197193</v>
+        <v>208857</v>
       </c>
       <c r="E141" t="s">
         <v>17</v>
@@ -4303,10 +4303,10 @@
         <v>9</v>
       </c>
       <c r="C142">
-        <v>896</v>
+        <v>976</v>
       </c>
       <c r="D142">
-        <v>1195421</v>
+        <v>1302031</v>
       </c>
       <c r="E142" t="s">
         <v>18</v>
@@ -4329,10 +4329,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>2689</v>
+        <v>2950</v>
       </c>
       <c r="D143">
-        <v>3276754</v>
+        <v>3593804</v>
       </c>
       <c r="E143" t="s">
         <v>18</v>
@@ -4355,10 +4355,10 @@
         <v>9</v>
       </c>
       <c r="C144">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D144">
-        <v>11025</v>
+        <v>15525</v>
       </c>
       <c r="E144" t="s">
         <v>18</v>
@@ -4381,10 +4381,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="D145">
-        <v>161952</v>
+        <v>181960</v>
       </c>
       <c r="E145" t="s">
         <v>18</v>
@@ -4407,10 +4407,10 @@
         <v>9</v>
       </c>
       <c r="C146">
-        <v>8782</v>
+        <v>9604</v>
       </c>
       <c r="D146">
-        <v>12449022</v>
+        <v>13614980</v>
       </c>
       <c r="E146" t="s">
         <v>18</v>
@@ -4433,10 +4433,10 @@
         <v>9</v>
       </c>
       <c r="C147">
-        <v>14932</v>
+        <v>16536</v>
       </c>
       <c r="D147">
-        <v>19136339</v>
+        <v>21228444</v>
       </c>
       <c r="E147" t="s">
         <v>18</v>
@@ -4459,10 +4459,10 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>3158</v>
+        <v>3512</v>
       </c>
       <c r="D148">
-        <v>4347694</v>
+        <v>4843812</v>
       </c>
       <c r="E148" t="s">
         <v>18</v>
@@ -4485,10 +4485,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>9701</v>
+        <v>10512</v>
       </c>
       <c r="D149">
-        <v>14014777</v>
+        <v>15194870</v>
       </c>
       <c r="E149" t="s">
         <v>18</v>
@@ -4511,10 +4511,10 @@
         <v>9</v>
       </c>
       <c r="C150">
-        <v>1025</v>
+        <v>1133</v>
       </c>
       <c r="D150">
-        <v>1306525</v>
+        <v>1448287</v>
       </c>
       <c r="E150" t="s">
         <v>18</v>
@@ -4537,10 +4537,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>664</v>
+        <v>723</v>
       </c>
       <c r="D151">
-        <v>928817</v>
+        <v>1015117</v>
       </c>
       <c r="E151" t="s">
         <v>18</v>
@@ -4563,10 +4563,10 @@
         <v>9</v>
       </c>
       <c r="C152">
-        <v>1667</v>
+        <v>1876</v>
       </c>
       <c r="D152">
-        <v>2242282</v>
+        <v>2528971</v>
       </c>
       <c r="E152" t="s">
         <v>18</v>
@@ -4589,10 +4589,10 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>5953</v>
+        <v>6640</v>
       </c>
       <c r="D153">
-        <v>8033699</v>
+        <v>8971277</v>
       </c>
       <c r="E153" t="s">
         <v>18</v>
@@ -4615,10 +4615,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>2834</v>
+        <v>3172</v>
       </c>
       <c r="D154">
-        <v>3543390</v>
+        <v>3982009</v>
       </c>
       <c r="E154" t="s">
         <v>18</v>
@@ -4641,10 +4641,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>3170</v>
+        <v>3532</v>
       </c>
       <c r="D155">
-        <v>3940933</v>
+        <v>4400370</v>
       </c>
       <c r="E155" t="s">
         <v>18</v>
@@ -4667,10 +4667,10 @@
         <v>9</v>
       </c>
       <c r="C156">
-        <v>7107</v>
+        <v>8061</v>
       </c>
       <c r="D156">
-        <v>9639341</v>
+        <v>10960531</v>
       </c>
       <c r="E156" t="s">
         <v>18</v>
@@ -4693,10 +4693,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>3002</v>
+        <v>3371</v>
       </c>
       <c r="D157">
-        <v>3585633</v>
+        <v>4028183</v>
       </c>
       <c r="E157" t="s">
         <v>18</v>
@@ -4719,10 +4719,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>13869</v>
+        <v>15414</v>
       </c>
       <c r="D158">
-        <v>16186788</v>
+        <v>18087035</v>
       </c>
       <c r="E158" t="s">
         <v>18</v>
@@ -4745,10 +4745,10 @@
         <v>9</v>
       </c>
       <c r="C159">
-        <v>827</v>
+        <v>892</v>
       </c>
       <c r="D159">
-        <v>1110553</v>
+        <v>1201596</v>
       </c>
       <c r="E159" t="s">
         <v>19</v>
@@ -4771,10 +4771,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>1337</v>
+        <v>1444</v>
       </c>
       <c r="D160">
-        <v>1788288</v>
+        <v>1934107</v>
       </c>
       <c r="E160" t="s">
         <v>19</v>
@@ -4823,10 +4823,10 @@
         <v>9</v>
       </c>
       <c r="C162">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D162">
-        <v>40173</v>
+        <v>44673</v>
       </c>
       <c r="E162" t="s">
         <v>19</v>
@@ -4849,10 +4849,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>2595</v>
+        <v>2763</v>
       </c>
       <c r="D163">
-        <v>3783705</v>
+        <v>4030612</v>
       </c>
       <c r="E163" t="s">
         <v>19</v>
@@ -4875,10 +4875,10 @@
         <v>9</v>
       </c>
       <c r="C164">
-        <v>4447</v>
+        <v>4892</v>
       </c>
       <c r="D164">
-        <v>6093308</v>
+        <v>6713915</v>
       </c>
       <c r="E164" t="s">
         <v>19</v>
@@ -4901,10 +4901,10 @@
         <v>9</v>
       </c>
       <c r="C165">
-        <v>578</v>
+        <v>628</v>
       </c>
       <c r="D165">
-        <v>816504</v>
+        <v>884867</v>
       </c>
       <c r="E165" t="s">
         <v>19</v>
@@ -4927,10 +4927,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>2219</v>
+        <v>2425</v>
       </c>
       <c r="D166">
-        <v>3127653</v>
+        <v>3423100</v>
       </c>
       <c r="E166" t="s">
         <v>19</v>
@@ -4953,10 +4953,10 @@
         <v>9</v>
       </c>
       <c r="C167">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="D167">
-        <v>405016</v>
+        <v>430040</v>
       </c>
       <c r="E167" t="s">
         <v>19</v>
@@ -4979,10 +4979,10 @@
         <v>9</v>
       </c>
       <c r="C168">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D168">
-        <v>189503</v>
+        <v>198483</v>
       </c>
       <c r="E168" t="s">
         <v>19</v>
@@ -5005,10 +5005,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>467</v>
+        <v>495</v>
       </c>
       <c r="D169">
-        <v>657755</v>
+        <v>696255</v>
       </c>
       <c r="E169" t="s">
         <v>19</v>
@@ -5031,10 +5031,10 @@
         <v>9</v>
       </c>
       <c r="C170">
-        <v>1354</v>
+        <v>1474</v>
       </c>
       <c r="D170">
-        <v>1912716</v>
+        <v>2086537</v>
       </c>
       <c r="E170" t="s">
         <v>19</v>
@@ -5057,10 +5057,10 @@
         <v>9</v>
       </c>
       <c r="C171">
-        <v>774</v>
+        <v>839</v>
       </c>
       <c r="D171">
-        <v>1067983</v>
+        <v>1160612</v>
       </c>
       <c r="E171" t="s">
         <v>19</v>
@@ -5083,10 +5083,10 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>1194</v>
+        <v>1320</v>
       </c>
       <c r="D172">
-        <v>1542867</v>
+        <v>1711970</v>
       </c>
       <c r="E172" t="s">
         <v>19</v>
@@ -5109,10 +5109,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>1616</v>
+        <v>1784</v>
       </c>
       <c r="D173">
-        <v>2280331</v>
+        <v>2518928</v>
       </c>
       <c r="E173" t="s">
         <v>19</v>
@@ -5135,10 +5135,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>656</v>
+        <v>714</v>
       </c>
       <c r="D174">
-        <v>854224</v>
+        <v>934892</v>
       </c>
       <c r="E174" t="s">
         <v>19</v>
@@ -5161,10 +5161,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>1989</v>
+        <v>2168</v>
       </c>
       <c r="D175">
-        <v>2536565</v>
+        <v>2774319</v>
       </c>
       <c r="E175" t="s">
         <v>19</v>
@@ -5187,10 +5187,10 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="D176">
-        <v>441906</v>
+        <v>469058</v>
       </c>
       <c r="E176" t="s">
         <v>20</v>
@@ -5213,10 +5213,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>557</v>
+        <v>602</v>
       </c>
       <c r="D177">
-        <v>743615</v>
+        <v>805284</v>
       </c>
       <c r="E177" t="s">
         <v>20</v>
@@ -5265,10 +5265,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>797</v>
+        <v>839</v>
       </c>
       <c r="D179">
-        <v>1149148</v>
+        <v>1210877</v>
       </c>
       <c r="E179" t="s">
         <v>20</v>
@@ -5291,10 +5291,10 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>1459</v>
+        <v>1603</v>
       </c>
       <c r="D180">
-        <v>2007665</v>
+        <v>2208655</v>
       </c>
       <c r="E180" t="s">
         <v>20</v>
@@ -5317,10 +5317,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>460</v>
+        <v>488</v>
       </c>
       <c r="D181">
-        <v>641572</v>
+        <v>681057</v>
       </c>
       <c r="E181" t="s">
         <v>20</v>
@@ -5343,10 +5343,10 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>802</v>
+        <v>872</v>
       </c>
       <c r="D182">
-        <v>1155254</v>
+        <v>1260052</v>
       </c>
       <c r="E182" t="s">
         <v>20</v>
@@ -5369,10 +5369,10 @@
         <v>9</v>
       </c>
       <c r="C183">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="D183">
-        <v>169292</v>
+        <v>187381</v>
       </c>
       <c r="E183" t="s">
         <v>20</v>
@@ -5395,10 +5395,10 @@
         <v>9</v>
       </c>
       <c r="C184">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D184">
-        <v>78896</v>
+        <v>90896</v>
       </c>
       <c r="E184" t="s">
         <v>20</v>
@@ -5421,10 +5421,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="D185">
-        <v>237026</v>
+        <v>269726</v>
       </c>
       <c r="E185" t="s">
         <v>20</v>
@@ -5447,10 +5447,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>700</v>
+        <v>766</v>
       </c>
       <c r="D186">
-        <v>971419</v>
+        <v>1066565</v>
       </c>
       <c r="E186" t="s">
         <v>20</v>
@@ -5473,10 +5473,10 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D187">
-        <v>838558</v>
+        <v>919425</v>
       </c>
       <c r="E187" t="s">
         <v>20</v>
@@ -5499,10 +5499,10 @@
         <v>9</v>
       </c>
       <c r="C188">
-        <v>377</v>
+        <v>414</v>
       </c>
       <c r="D188">
-        <v>485277</v>
+        <v>533888</v>
       </c>
       <c r="E188" t="s">
         <v>20</v>
@@ -5525,10 +5525,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>617</v>
+        <v>676</v>
       </c>
       <c r="D189">
-        <v>849443</v>
+        <v>936239</v>
       </c>
       <c r="E189" t="s">
         <v>20</v>
@@ -5551,10 +5551,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="D190">
-        <v>304009</v>
+        <v>336378</v>
       </c>
       <c r="E190" t="s">
         <v>20</v>
@@ -5577,10 +5577,10 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>842</v>
+        <v>942</v>
       </c>
       <c r="D191">
-        <v>1080489</v>
+        <v>1221159</v>
       </c>
       <c r="E191" t="s">
         <v>20</v>
@@ -5603,10 +5603,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D192">
-        <v>56714</v>
+        <v>59714</v>
       </c>
       <c r="E192" t="s">
         <v>21</v>
@@ -5629,10 +5629,10 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D193">
-        <v>77624</v>
+        <v>86624</v>
       </c>
       <c r="E193" t="s">
         <v>21</v>
@@ -5681,10 +5681,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D195">
-        <v>218241</v>
+        <v>225741</v>
       </c>
       <c r="E195" t="s">
         <v>21</v>
@@ -5707,10 +5707,10 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="D196">
-        <v>524561</v>
+        <v>556861</v>
       </c>
       <c r="E196" t="s">
         <v>21</v>
@@ -5733,10 +5733,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D197">
-        <v>143959</v>
+        <v>154459</v>
       </c>
       <c r="E197" t="s">
         <v>21</v>
@@ -5759,10 +5759,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D198">
-        <v>167441</v>
+        <v>183941</v>
       </c>
       <c r="E198" t="s">
         <v>21</v>
@@ -5785,10 +5785,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D199">
-        <v>23543</v>
+        <v>25043</v>
       </c>
       <c r="E199" t="s">
         <v>21</v>
@@ -5837,10 +5837,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D201">
-        <v>85086</v>
+        <v>94086</v>
       </c>
       <c r="E201" t="s">
         <v>21</v>
@@ -5863,10 +5863,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D202">
-        <v>59456</v>
+        <v>66893</v>
       </c>
       <c r="E202" t="s">
         <v>21</v>
@@ -5889,10 +5889,10 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D203">
-        <v>82265</v>
+        <v>92725</v>
       </c>
       <c r="E203" t="s">
         <v>21</v>
@@ -5915,10 +5915,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D204">
-        <v>43492</v>
+        <v>50992</v>
       </c>
       <c r="E204" t="s">
         <v>21</v>
@@ -5941,10 +5941,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D205">
-        <v>34200</v>
+        <v>43200</v>
       </c>
       <c r="E205" t="s">
         <v>21</v>
@@ -5967,10 +5967,10 @@
         <v>9</v>
       </c>
       <c r="C206">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D206">
-        <v>67182</v>
+        <v>76182</v>
       </c>
       <c r="E206" t="s">
         <v>21</v>
@@ -5993,10 +5993,10 @@
         <v>9</v>
       </c>
       <c r="C207">
-        <v>1011</v>
+        <v>1092</v>
       </c>
       <c r="D207">
-        <v>1373775</v>
+        <v>1484105</v>
       </c>
       <c r="E207" t="s">
         <v>22</v>
@@ -6019,10 +6019,10 @@
         <v>9</v>
       </c>
       <c r="C208">
-        <v>1806</v>
+        <v>1977</v>
       </c>
       <c r="D208">
-        <v>2240873</v>
+        <v>2455582</v>
       </c>
       <c r="E208" t="s">
         <v>22</v>
@@ -6045,10 +6045,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D209">
-        <v>125132</v>
+        <v>136852</v>
       </c>
       <c r="E209" t="s">
         <v>22</v>
@@ -6071,10 +6071,10 @@
         <v>9</v>
       </c>
       <c r="C210">
-        <v>5405</v>
+        <v>5848</v>
       </c>
       <c r="D210">
-        <v>7738709</v>
+        <v>8373954</v>
       </c>
       <c r="E210" t="s">
         <v>22</v>
@@ -6097,10 +6097,10 @@
         <v>9</v>
       </c>
       <c r="C211">
-        <v>9671</v>
+        <v>10685</v>
       </c>
       <c r="D211">
-        <v>12757582</v>
+        <v>14115855</v>
       </c>
       <c r="E211" t="s">
         <v>22</v>
@@ -6123,10 +6123,10 @@
         <v>9</v>
       </c>
       <c r="C212">
-        <v>1004</v>
+        <v>1143</v>
       </c>
       <c r="D212">
-        <v>1366638</v>
+        <v>1556993</v>
       </c>
       <c r="E212" t="s">
         <v>22</v>
@@ -6149,10 +6149,10 @@
         <v>9</v>
       </c>
       <c r="C213">
-        <v>6562</v>
+        <v>7158</v>
       </c>
       <c r="D213">
-        <v>9406385</v>
+        <v>10261834</v>
       </c>
       <c r="E213" t="s">
         <v>22</v>
@@ -6175,10 +6175,10 @@
         <v>9</v>
       </c>
       <c r="C214">
-        <v>549</v>
+        <v>617</v>
       </c>
       <c r="D214">
-        <v>685406</v>
+        <v>768027</v>
       </c>
       <c r="E214" t="s">
         <v>22</v>
@@ -6201,10 +6201,10 @@
         <v>9</v>
       </c>
       <c r="C215">
-        <v>414</v>
+        <v>452</v>
       </c>
       <c r="D215">
-        <v>578621</v>
+        <v>631700</v>
       </c>
       <c r="E215" t="s">
         <v>22</v>
@@ -6227,10 +6227,10 @@
         <v>9</v>
       </c>
       <c r="C216">
-        <v>1134</v>
+        <v>1252</v>
       </c>
       <c r="D216">
-        <v>1498051</v>
+        <v>1662687</v>
       </c>
       <c r="E216" t="s">
         <v>22</v>
@@ -6253,10 +6253,10 @@
         <v>9</v>
       </c>
       <c r="C217">
-        <v>3384</v>
+        <v>3762</v>
       </c>
       <c r="D217">
-        <v>4574372</v>
+        <v>5095166</v>
       </c>
       <c r="E217" t="s">
         <v>22</v>
@@ -6279,10 +6279,10 @@
         <v>9</v>
       </c>
       <c r="C218">
-        <v>1617</v>
+        <v>1803</v>
       </c>
       <c r="D218">
-        <v>1996284</v>
+        <v>2230747</v>
       </c>
       <c r="E218" t="s">
         <v>22</v>
@@ -6305,10 +6305,10 @@
         <v>9</v>
       </c>
       <c r="C219">
-        <v>2026</v>
+        <v>2261</v>
       </c>
       <c r="D219">
-        <v>2417293</v>
+        <v>2707158</v>
       </c>
       <c r="E219" t="s">
         <v>22</v>
@@ -6331,10 +6331,10 @@
         <v>9</v>
       </c>
       <c r="C220">
-        <v>3798</v>
+        <v>4303</v>
       </c>
       <c r="D220">
-        <v>5040751</v>
+        <v>5732509</v>
       </c>
       <c r="E220" t="s">
         <v>22</v>
@@ -6357,10 +6357,10 @@
         <v>9</v>
       </c>
       <c r="C221">
-        <v>1966</v>
+        <v>2206</v>
       </c>
       <c r="D221">
-        <v>2371572</v>
+        <v>2666304</v>
       </c>
       <c r="E221" t="s">
         <v>22</v>
@@ -6383,10 +6383,10 @@
         <v>9</v>
       </c>
       <c r="C222">
-        <v>8409</v>
+        <v>9358</v>
       </c>
       <c r="D222">
-        <v>10199324</v>
+        <v>11434266</v>
       </c>
       <c r="E222" t="s">
         <v>22</v>
@@ -6409,10 +6409,10 @@
         <v>9</v>
       </c>
       <c r="C223">
-        <v>3556</v>
+        <v>3825</v>
       </c>
       <c r="D223">
-        <v>4908503</v>
+        <v>5280983</v>
       </c>
       <c r="E223" t="s">
         <v>23</v>
@@ -6435,10 +6435,10 @@
         <v>9</v>
       </c>
       <c r="C224">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D224">
-        <v>27428</v>
+        <v>28123</v>
       </c>
       <c r="E224" t="s">
         <v>23</v>
@@ -6461,10 +6461,10 @@
         <v>9</v>
       </c>
       <c r="C225">
-        <v>5707</v>
+        <v>6315</v>
       </c>
       <c r="D225">
-        <v>6955522</v>
+        <v>7706173</v>
       </c>
       <c r="E225" t="s">
         <v>23</v>
@@ -6487,10 +6487,10 @@
         <v>9</v>
       </c>
       <c r="C226">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D226">
-        <v>29759</v>
+        <v>31259</v>
       </c>
       <c r="E226" t="s">
         <v>23</v>
@@ -6513,10 +6513,10 @@
         <v>9</v>
       </c>
       <c r="C227">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="D227">
-        <v>305244</v>
+        <v>337345</v>
       </c>
       <c r="E227" t="s">
         <v>23</v>
@@ -6539,10 +6539,10 @@
         <v>9</v>
       </c>
       <c r="C228">
-        <v>15711</v>
+        <v>17163</v>
       </c>
       <c r="D228">
-        <v>22368225</v>
+        <v>24439123</v>
       </c>
       <c r="E228" t="s">
         <v>23</v>
@@ -6565,10 +6565,10 @@
         <v>9</v>
       </c>
       <c r="C229">
-        <v>22054</v>
+        <v>24469</v>
       </c>
       <c r="D229">
-        <v>29174158</v>
+        <v>32465505</v>
       </c>
       <c r="E229" t="s">
         <v>23</v>
@@ -6591,10 +6591,10 @@
         <v>9</v>
       </c>
       <c r="C230">
-        <v>2750</v>
+        <v>3108</v>
       </c>
       <c r="D230">
-        <v>3740900</v>
+        <v>4234738</v>
       </c>
       <c r="E230" t="s">
         <v>23</v>
@@ -6617,10 +6617,10 @@
         <v>9</v>
       </c>
       <c r="C231">
-        <v>14448</v>
+        <v>15880</v>
       </c>
       <c r="D231">
-        <v>20388666</v>
+        <v>22439566</v>
       </c>
       <c r="E231" t="s">
         <v>23</v>
@@ -6643,10 +6643,10 @@
         <v>9</v>
       </c>
       <c r="C232">
-        <v>1722</v>
+        <v>1913</v>
       </c>
       <c r="D232">
-        <v>2225403</v>
+        <v>2468632</v>
       </c>
       <c r="E232" t="s">
         <v>23</v>
@@ -6669,10 +6669,10 @@
         <v>9</v>
       </c>
       <c r="C233">
-        <v>932</v>
+        <v>1032</v>
       </c>
       <c r="D233">
-        <v>1300433</v>
+        <v>1439001</v>
       </c>
       <c r="E233" t="s">
         <v>23</v>
@@ -6695,10 +6695,10 @@
         <v>9</v>
       </c>
       <c r="C234">
-        <v>3400</v>
+        <v>3809</v>
       </c>
       <c r="D234">
-        <v>4545118</v>
+        <v>5098270</v>
       </c>
       <c r="E234" t="s">
         <v>23</v>
@@ -6721,10 +6721,10 @@
         <v>9</v>
       </c>
       <c r="C235">
-        <v>10141</v>
+        <v>11265</v>
       </c>
       <c r="D235">
-        <v>13573092</v>
+        <v>15108502</v>
       </c>
       <c r="E235" t="s">
         <v>23</v>
@@ -6747,10 +6747,10 @@
         <v>9</v>
       </c>
       <c r="C236">
-        <v>5226</v>
+        <v>5879</v>
       </c>
       <c r="D236">
-        <v>6480279</v>
+        <v>7312793</v>
       </c>
       <c r="E236" t="s">
         <v>23</v>
@@ -6773,10 +6773,10 @@
         <v>9</v>
       </c>
       <c r="C237">
-        <v>5843</v>
+        <v>6616</v>
       </c>
       <c r="D237">
-        <v>6806466</v>
+        <v>7758119</v>
       </c>
       <c r="E237" t="s">
         <v>23</v>
@@ -6799,10 +6799,10 @@
         <v>9</v>
       </c>
       <c r="C238">
-        <v>12300</v>
+        <v>14064</v>
       </c>
       <c r="D238">
-        <v>16224872</v>
+        <v>18608538</v>
       </c>
       <c r="E238" t="s">
         <v>23</v>
@@ -6825,10 +6825,10 @@
         <v>9</v>
       </c>
       <c r="C239">
-        <v>4917</v>
+        <v>5523</v>
       </c>
       <c r="D239">
-        <v>5850093</v>
+        <v>6605209</v>
       </c>
       <c r="E239" t="s">
         <v>23</v>
@@ -6851,10 +6851,10 @@
         <v>9</v>
       </c>
       <c r="C240">
-        <v>18474</v>
+        <v>20637</v>
       </c>
       <c r="D240">
-        <v>22315066</v>
+        <v>25059819</v>
       </c>
       <c r="E240" t="s">
         <v>23</v>
@@ -6877,10 +6877,10 @@
         <v>9</v>
       </c>
       <c r="C241">
-        <v>3624</v>
+        <v>3888</v>
       </c>
       <c r="D241">
-        <v>4872398</v>
+        <v>5231892</v>
       </c>
       <c r="E241" t="s">
         <v>24</v>
@@ -6929,10 +6929,10 @@
         <v>9</v>
       </c>
       <c r="C243">
-        <v>5814</v>
+        <v>6421</v>
       </c>
       <c r="D243">
-        <v>7072049</v>
+        <v>7855898</v>
       </c>
       <c r="E243" t="s">
         <v>24</v>
@@ -6955,10 +6955,10 @@
         <v>9</v>
       </c>
       <c r="C244">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D244">
-        <v>45661</v>
+        <v>48661</v>
       </c>
       <c r="E244" t="s">
         <v>24</v>
@@ -6981,10 +6981,10 @@
         <v>9</v>
       </c>
       <c r="C245">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="D245">
-        <v>237298</v>
+        <v>274076</v>
       </c>
       <c r="E245" t="s">
         <v>24</v>
@@ -7007,10 +7007,10 @@
         <v>9</v>
       </c>
       <c r="C246">
-        <v>19081</v>
+        <v>20772</v>
       </c>
       <c r="D246">
-        <v>27034827</v>
+        <v>29429987</v>
       </c>
       <c r="E246" t="s">
         <v>24</v>
@@ -7033,10 +7033,10 @@
         <v>9</v>
       </c>
       <c r="C247">
-        <v>24142</v>
+        <v>26712</v>
       </c>
       <c r="D247">
-        <v>31656436</v>
+        <v>35105868</v>
       </c>
       <c r="E247" t="s">
         <v>24</v>
@@ -7059,10 +7059,10 @@
         <v>9</v>
       </c>
       <c r="C248">
-        <v>3001</v>
+        <v>3350</v>
       </c>
       <c r="D248">
-        <v>3975585</v>
+        <v>4441402</v>
       </c>
       <c r="E248" t="s">
         <v>24</v>
@@ -7085,10 +7085,10 @@
         <v>9</v>
       </c>
       <c r="C249">
-        <v>16798</v>
+        <v>18372</v>
       </c>
       <c r="D249">
-        <v>23715799</v>
+        <v>25971717</v>
       </c>
       <c r="E249" t="s">
         <v>24</v>
@@ -7111,10 +7111,10 @@
         <v>9</v>
       </c>
       <c r="C250">
-        <v>1908</v>
+        <v>2142</v>
       </c>
       <c r="D250">
-        <v>2424767</v>
+        <v>2732268</v>
       </c>
       <c r="E250" t="s">
         <v>24</v>
@@ -7137,10 +7137,10 @@
         <v>9</v>
       </c>
       <c r="C251">
-        <v>991</v>
+        <v>1073</v>
       </c>
       <c r="D251">
-        <v>1372798</v>
+        <v>1485582</v>
       </c>
       <c r="E251" t="s">
         <v>24</v>
@@ -7163,10 +7163,10 @@
         <v>9</v>
       </c>
       <c r="C252">
-        <v>3867</v>
+        <v>4312</v>
       </c>
       <c r="D252">
-        <v>5184345</v>
+        <v>5788408</v>
       </c>
       <c r="E252" t="s">
         <v>24</v>
@@ -7189,10 +7189,10 @@
         <v>9</v>
       </c>
       <c r="C253">
-        <v>11042</v>
+        <v>12249</v>
       </c>
       <c r="D253">
-        <v>14968864</v>
+        <v>16609758</v>
       </c>
       <c r="E253" t="s">
         <v>24</v>
@@ -7215,10 +7215,10 @@
         <v>9</v>
       </c>
       <c r="C254">
-        <v>5542</v>
+        <v>6176</v>
       </c>
       <c r="D254">
-        <v>6879279</v>
+        <v>7690308</v>
       </c>
       <c r="E254" t="s">
         <v>24</v>
@@ -7267,10 +7267,10 @@
         <v>9</v>
       </c>
       <c r="C256">
-        <v>6893</v>
+        <v>7727</v>
       </c>
       <c r="D256">
-        <v>8028039</v>
+        <v>9082059</v>
       </c>
       <c r="E256" t="s">
         <v>24</v>
@@ -7293,10 +7293,10 @@
         <v>9</v>
       </c>
       <c r="C257">
-        <v>11937</v>
+        <v>13601</v>
       </c>
       <c r="D257">
-        <v>15652260</v>
+        <v>17941843</v>
       </c>
       <c r="E257" t="s">
         <v>24</v>
@@ -7319,10 +7319,10 @@
         <v>9</v>
       </c>
       <c r="C258">
-        <v>5495</v>
+        <v>6169</v>
       </c>
       <c r="D258">
-        <v>6531536</v>
+        <v>7362860</v>
       </c>
       <c r="E258" t="s">
         <v>24</v>
@@ -7345,10 +7345,10 @@
         <v>9</v>
       </c>
       <c r="C259">
-        <v>18409</v>
+        <v>20533</v>
       </c>
       <c r="D259">
-        <v>21361359</v>
+        <v>23971483</v>
       </c>
       <c r="E259" t="s">
         <v>24</v>
@@ -7371,10 +7371,10 @@
         <v>9</v>
       </c>
       <c r="C260">
-        <v>1287</v>
+        <v>1382</v>
       </c>
       <c r="D260">
-        <v>1778097</v>
+        <v>1911145</v>
       </c>
       <c r="E260" t="s">
         <v>25</v>
@@ -7397,10 +7397,10 @@
         <v>9</v>
       </c>
       <c r="C261">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D261">
-        <v>33968</v>
+        <v>38468</v>
       </c>
       <c r="E261" t="s">
         <v>25</v>
@@ -7423,10 +7423,10 @@
         <v>9</v>
       </c>
       <c r="C262">
-        <v>2420</v>
+        <v>2693</v>
       </c>
       <c r="D262">
-        <v>2962072</v>
+        <v>3299119</v>
       </c>
       <c r="E262" t="s">
         <v>25</v>
@@ -7475,10 +7475,10 @@
         <v>9</v>
       </c>
       <c r="C264">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="D264">
-        <v>202714</v>
+        <v>227177</v>
       </c>
       <c r="E264" t="s">
         <v>25</v>
@@ -7501,10 +7501,10 @@
         <v>9</v>
       </c>
       <c r="C265">
-        <v>6077</v>
+        <v>6671</v>
       </c>
       <c r="D265">
-        <v>8718780</v>
+        <v>9578727</v>
       </c>
       <c r="E265" t="s">
         <v>25</v>
@@ -7527,10 +7527,10 @@
         <v>9</v>
       </c>
       <c r="C266">
-        <v>9935</v>
+        <v>11033</v>
       </c>
       <c r="D266">
-        <v>13073759</v>
+        <v>14562275</v>
       </c>
       <c r="E266" t="s">
         <v>25</v>
@@ -7553,10 +7553,10 @@
         <v>9</v>
       </c>
       <c r="C267">
-        <v>1224</v>
+        <v>1404</v>
       </c>
       <c r="D267">
-        <v>1702313</v>
+        <v>1958174</v>
       </c>
       <c r="E267" t="s">
         <v>25</v>
@@ -7579,10 +7579,10 @@
         <v>9</v>
       </c>
       <c r="C268">
-        <v>6989</v>
+        <v>7654</v>
       </c>
       <c r="D268">
-        <v>10041175</v>
+        <v>11019332</v>
       </c>
       <c r="E268" t="s">
         <v>25</v>
@@ -7605,10 +7605,10 @@
         <v>9</v>
       </c>
       <c r="C269">
-        <v>899</v>
+        <v>1019</v>
       </c>
       <c r="D269">
-        <v>1146100</v>
+        <v>1296144</v>
       </c>
       <c r="E269" t="s">
         <v>25</v>
@@ -7631,10 +7631,10 @@
         <v>9</v>
       </c>
       <c r="C270">
-        <v>563</v>
+        <v>604</v>
       </c>
       <c r="D270">
-        <v>792837</v>
+        <v>852540</v>
       </c>
       <c r="E270" t="s">
         <v>25</v>
@@ -7657,10 +7657,10 @@
         <v>9</v>
       </c>
       <c r="C271">
-        <v>1746</v>
+        <v>1944</v>
       </c>
       <c r="D271">
-        <v>2344366</v>
+        <v>2617388</v>
       </c>
       <c r="E271" t="s">
         <v>25</v>
@@ -7683,10 +7683,10 @@
         <v>9</v>
       </c>
       <c r="C272">
-        <v>5115</v>
+        <v>5682</v>
       </c>
       <c r="D272">
-        <v>6933264</v>
+        <v>7695367</v>
       </c>
       <c r="E272" t="s">
         <v>25</v>
@@ -7709,10 +7709,10 @@
         <v>9</v>
       </c>
       <c r="C273">
-        <v>2007</v>
+        <v>2248</v>
       </c>
       <c r="D273">
-        <v>2562321</v>
+        <v>2881014</v>
       </c>
       <c r="E273" t="s">
         <v>25</v>
@@ -7735,10 +7735,10 @@
         <v>9</v>
       </c>
       <c r="C274">
-        <v>2495</v>
+        <v>2827</v>
       </c>
       <c r="D274">
-        <v>3003160</v>
+        <v>3428015</v>
       </c>
       <c r="E274" t="s">
         <v>25</v>
@@ -7761,10 +7761,10 @@
         <v>9</v>
       </c>
       <c r="C275">
-        <v>6659</v>
+        <v>7658</v>
       </c>
       <c r="D275">
-        <v>8819353</v>
+        <v>10206649</v>
       </c>
       <c r="E275" t="s">
         <v>25</v>
@@ -7787,10 +7787,10 @@
         <v>9</v>
       </c>
       <c r="C276">
-        <v>2640</v>
+        <v>2968</v>
       </c>
       <c r="D276">
-        <v>3164898</v>
+        <v>3583411</v>
       </c>
       <c r="E276" t="s">
         <v>25</v>
@@ -7813,10 +7813,10 @@
         <v>9</v>
       </c>
       <c r="C277">
-        <v>9522</v>
+        <v>10692</v>
       </c>
       <c r="D277">
-        <v>11791306</v>
+        <v>13346867</v>
       </c>
       <c r="E277" t="s">
         <v>25</v>
@@ -7839,10 +7839,10 @@
         <v>9</v>
       </c>
       <c r="C278">
-        <v>1760</v>
+        <v>1876</v>
       </c>
       <c r="D278">
-        <v>2392172</v>
+        <v>2555503</v>
       </c>
       <c r="E278" t="s">
         <v>26</v>
@@ -7865,10 +7865,10 @@
         <v>9</v>
       </c>
       <c r="C279">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D279">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E279" t="s">
         <v>26</v>
@@ -7891,10 +7891,10 @@
         <v>9</v>
       </c>
       <c r="C280">
-        <v>5758</v>
+        <v>6359</v>
       </c>
       <c r="D280">
-        <v>7406137</v>
+        <v>8182511</v>
       </c>
       <c r="E280" t="s">
         <v>26</v>
@@ -7943,10 +7943,10 @@
         <v>9</v>
       </c>
       <c r="C282">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D282">
-        <v>133297</v>
+        <v>149227</v>
       </c>
       <c r="E282" t="s">
         <v>26</v>
@@ -7969,10 +7969,10 @@
         <v>9</v>
       </c>
       <c r="C283">
-        <v>16807</v>
+        <v>18204</v>
       </c>
       <c r="D283">
-        <v>23985901</v>
+        <v>25992346</v>
       </c>
       <c r="E283" t="s">
         <v>26</v>
@@ -7995,10 +7995,10 @@
         <v>9</v>
       </c>
       <c r="C284">
-        <v>26022</v>
+        <v>28710</v>
       </c>
       <c r="D284">
-        <v>34619161</v>
+        <v>38276890</v>
       </c>
       <c r="E284" t="s">
         <v>26</v>
@@ -8021,10 +8021,10 @@
         <v>9</v>
       </c>
       <c r="C285">
-        <v>5503</v>
+        <v>6188</v>
       </c>
       <c r="D285">
-        <v>7673871</v>
+        <v>8643362</v>
       </c>
       <c r="E285" t="s">
         <v>26</v>
@@ -8047,10 +8047,10 @@
         <v>9</v>
       </c>
       <c r="C286">
-        <v>16384</v>
+        <v>17945</v>
       </c>
       <c r="D286">
-        <v>23587212</v>
+        <v>25855515</v>
       </c>
       <c r="E286" t="s">
         <v>26</v>
@@ -8073,10 +8073,10 @@
         <v>9</v>
       </c>
       <c r="C287">
-        <v>2232</v>
+        <v>2486</v>
       </c>
       <c r="D287">
-        <v>2913907</v>
+        <v>3245622</v>
       </c>
       <c r="E287" t="s">
         <v>26</v>
@@ -8099,10 +8099,10 @@
         <v>9</v>
       </c>
       <c r="C288">
-        <v>1138</v>
+        <v>1250</v>
       </c>
       <c r="D288">
-        <v>1604296</v>
+        <v>1766426</v>
       </c>
       <c r="E288" t="s">
         <v>26</v>
@@ -8125,10 +8125,10 @@
         <v>9</v>
       </c>
       <c r="C289">
-        <v>4763</v>
+        <v>5256</v>
       </c>
       <c r="D289">
-        <v>6598758</v>
+        <v>7288417</v>
       </c>
       <c r="E289" t="s">
         <v>26</v>
@@ -8151,10 +8151,10 @@
         <v>9</v>
       </c>
       <c r="C290">
-        <v>12369</v>
+        <v>13714</v>
       </c>
       <c r="D290">
-        <v>16845663</v>
+        <v>18701942</v>
       </c>
       <c r="E290" t="s">
         <v>26</v>
@@ -8177,10 +8177,10 @@
         <v>9</v>
       </c>
       <c r="C291">
-        <v>6814</v>
+        <v>7564</v>
       </c>
       <c r="D291">
-        <v>8762050</v>
+        <v>9743080</v>
       </c>
       <c r="E291" t="s">
         <v>26</v>
@@ -8203,10 +8203,10 @@
         <v>9</v>
       </c>
       <c r="C292">
-        <v>7698</v>
+        <v>3</v>
       </c>
       <c r="D292">
-        <v>9353289</v>
+        <v>4219</v>
       </c>
       <c r="E292" t="s">
         <v>26</v>
@@ -8215,10 +8215,10 @@
         <v>44</v>
       </c>
       <c r="G292" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H292" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="293" spans="1:8">
@@ -8229,10 +8229,10 @@
         <v>9</v>
       </c>
       <c r="C293">
-        <v>11921</v>
+        <v>8626</v>
       </c>
       <c r="D293">
-        <v>15751269</v>
+        <v>10539443</v>
       </c>
       <c r="E293" t="s">
         <v>26</v>
@@ -8241,10 +8241,10 @@
         <v>44</v>
       </c>
       <c r="G293" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H293" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="294" spans="1:8">
@@ -8255,10 +8255,10 @@
         <v>9</v>
       </c>
       <c r="C294">
-        <v>5467</v>
+        <v>13403</v>
       </c>
       <c r="D294">
-        <v>6729888</v>
+        <v>17769263</v>
       </c>
       <c r="E294" t="s">
         <v>26</v>
@@ -8267,10 +8267,10 @@
         <v>44</v>
       </c>
       <c r="G294" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H294" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="295" spans="1:8">
@@ -8281,10 +8281,10 @@
         <v>9</v>
       </c>
       <c r="C295">
-        <v>17755</v>
+        <v>6110</v>
       </c>
       <c r="D295">
-        <v>21097418</v>
+        <v>7542627</v>
       </c>
       <c r="E295" t="s">
         <v>26</v>
@@ -8293,10 +8293,10 @@
         <v>44</v>
       </c>
       <c r="G295" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H295" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="296" spans="1:8">
@@ -8307,22 +8307,22 @@
         <v>9</v>
       </c>
       <c r="C296">
-        <v>275</v>
+        <v>19790</v>
       </c>
       <c r="D296">
-        <v>375075</v>
+        <v>23651581</v>
       </c>
       <c r="E296" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F296" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G296" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="H296" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="297" spans="1:8">
@@ -8333,10 +8333,10 @@
         <v>9</v>
       </c>
       <c r="C297">
-        <v>6459</v>
+        <v>300</v>
       </c>
       <c r="D297">
-        <v>8612561</v>
+        <v>411744</v>
       </c>
       <c r="E297" t="s">
         <v>27</v>
@@ -8345,10 +8345,10 @@
         <v>45</v>
       </c>
       <c r="G297" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H297" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="298" spans="1:8">
@@ -8359,10 +8359,10 @@
         <v>9</v>
       </c>
       <c r="C298">
-        <v>49</v>
+        <v>7152</v>
       </c>
       <c r="D298">
-        <v>70865</v>
+        <v>9557847</v>
       </c>
       <c r="E298" t="s">
         <v>27</v>
@@ -8371,10 +8371,10 @@
         <v>45</v>
       </c>
       <c r="G298" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H298" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="299" spans="1:8">
@@ -8385,10 +8385,10 @@
         <v>9</v>
       </c>
       <c r="C299">
-        <v>201</v>
+        <v>56</v>
       </c>
       <c r="D299">
-        <v>265868</v>
+        <v>80598</v>
       </c>
       <c r="E299" t="s">
         <v>27</v>
@@ -8397,10 +8397,10 @@
         <v>45</v>
       </c>
       <c r="G299" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H299" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="300" spans="1:8">
@@ -8411,10 +8411,10 @@
         <v>9</v>
       </c>
       <c r="C300">
-        <v>19370</v>
+        <v>217</v>
       </c>
       <c r="D300">
-        <v>27977250</v>
+        <v>288251</v>
       </c>
       <c r="E300" t="s">
         <v>27</v>
@@ -8423,10 +8423,10 @@
         <v>45</v>
       </c>
       <c r="G300" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H300" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="301" spans="1:8">
@@ -8437,10 +8437,10 @@
         <v>9</v>
       </c>
       <c r="C301">
-        <v>35610</v>
+        <v>21038</v>
       </c>
       <c r="D301">
-        <v>48852675</v>
+        <v>30414420</v>
       </c>
       <c r="E301" t="s">
         <v>27</v>
@@ -8449,10 +8449,10 @@
         <v>45</v>
       </c>
       <c r="G301" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H301" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="302" spans="1:8">
@@ -8463,10 +8463,10 @@
         <v>9</v>
       </c>
       <c r="C302">
-        <v>36924</v>
+        <v>39211</v>
       </c>
       <c r="D302">
-        <v>53152271</v>
+        <v>53884041</v>
       </c>
       <c r="E302" t="s">
         <v>27</v>
@@ -8475,10 +8475,10 @@
         <v>45</v>
       </c>
       <c r="G302" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H302" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="303" spans="1:8">
@@ -8489,10 +8489,10 @@
         <v>9</v>
       </c>
       <c r="C303">
-        <v>22099</v>
+        <v>41622</v>
       </c>
       <c r="D303">
-        <v>32535915</v>
+        <v>60011477</v>
       </c>
       <c r="E303" t="s">
         <v>27</v>
@@ -8501,10 +8501,10 @@
         <v>45</v>
       </c>
       <c r="G303" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H303" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="304" spans="1:8">
@@ -8515,10 +8515,10 @@
         <v>9</v>
       </c>
       <c r="C304">
-        <v>9459</v>
+        <v>24150</v>
       </c>
       <c r="D304">
-        <v>12976234</v>
+        <v>35561345</v>
       </c>
       <c r="E304" t="s">
         <v>27</v>
@@ -8527,10 +8527,10 @@
         <v>45</v>
       </c>
       <c r="G304" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H304" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="305" spans="1:8">
@@ -8541,10 +8541,10 @@
         <v>9</v>
       </c>
       <c r="C305">
-        <v>2488</v>
+        <v>10480</v>
       </c>
       <c r="D305">
-        <v>3562768</v>
+        <v>14380751</v>
       </c>
       <c r="E305" t="s">
         <v>27</v>
@@ -8553,10 +8553,10 @@
         <v>45</v>
       </c>
       <c r="G305" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H305" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="306" spans="1:8">
@@ -8567,10 +8567,10 @@
         <v>9</v>
       </c>
       <c r="C306">
-        <v>6256</v>
+        <v>2703</v>
       </c>
       <c r="D306">
-        <v>8907032</v>
+        <v>3875874</v>
       </c>
       <c r="E306" t="s">
         <v>27</v>
@@ -8579,10 +8579,10 @@
         <v>45</v>
       </c>
       <c r="G306" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H306" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="307" spans="1:8">
@@ -8593,10 +8593,10 @@
         <v>9</v>
       </c>
       <c r="C307">
-        <v>37629</v>
+        <v>6934</v>
       </c>
       <c r="D307">
-        <v>51979508</v>
+        <v>9887107</v>
       </c>
       <c r="E307" t="s">
         <v>27</v>
@@ -8605,10 +8605,10 @@
         <v>45</v>
       </c>
       <c r="G307" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H307" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="308" spans="1:8">
@@ -8619,10 +8619,10 @@
         <v>9</v>
       </c>
       <c r="C308">
-        <v>10072</v>
+        <v>41812</v>
       </c>
       <c r="D308">
-        <v>13478307</v>
+        <v>57820671</v>
       </c>
       <c r="E308" t="s">
         <v>27</v>
@@ -8631,10 +8631,10 @@
         <v>45</v>
       </c>
       <c r="G308" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H308" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="309" spans="1:8">
@@ -8645,10 +8645,10 @@
         <v>9</v>
       </c>
       <c r="C309">
-        <v>5</v>
+        <v>11194</v>
       </c>
       <c r="D309">
-        <v>5675</v>
+        <v>14992994</v>
       </c>
       <c r="E309" t="s">
         <v>27</v>
@@ -8657,10 +8657,10 @@
         <v>45</v>
       </c>
       <c r="G309" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H309" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="310" spans="1:8">
@@ -8671,10 +8671,10 @@
         <v>9</v>
       </c>
       <c r="C310">
-        <v>10892</v>
+        <v>5</v>
       </c>
       <c r="D310">
-        <v>13474146</v>
+        <v>5675</v>
       </c>
       <c r="E310" t="s">
         <v>27</v>
@@ -8683,10 +8683,10 @@
         <v>45</v>
       </c>
       <c r="G310" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H310" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="311" spans="1:8">
@@ -8697,10 +8697,10 @@
         <v>9</v>
       </c>
       <c r="C311">
-        <v>20177</v>
+        <v>12301</v>
       </c>
       <c r="D311">
-        <v>27294910</v>
+        <v>15303197</v>
       </c>
       <c r="E311" t="s">
         <v>27</v>
@@ -8709,10 +8709,10 @@
         <v>45</v>
       </c>
       <c r="G311" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H311" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="312" spans="1:8">
@@ -8723,10 +8723,10 @@
         <v>9</v>
       </c>
       <c r="C312">
-        <v>14249</v>
+        <v>23045</v>
       </c>
       <c r="D312">
-        <v>18324089</v>
+        <v>31324427</v>
       </c>
       <c r="E312" t="s">
         <v>27</v>
@@ -8735,10 +8735,10 @@
         <v>45</v>
       </c>
       <c r="G312" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H312" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="313" spans="1:8">
@@ -8749,10 +8749,10 @@
         <v>9</v>
       </c>
       <c r="C313">
-        <v>23130</v>
+        <v>15928</v>
       </c>
       <c r="D313">
-        <v>29941726</v>
+        <v>20541040</v>
       </c>
       <c r="E313" t="s">
         <v>27</v>
@@ -8761,9 +8761,35 @@
         <v>45</v>
       </c>
       <c r="G313" t="s">
+        <v>63</v>
+      </c>
+      <c r="H313" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8">
+      <c r="A314" t="s">
+        <v>8</v>
+      </c>
+      <c r="B314" t="s">
+        <v>9</v>
+      </c>
+      <c r="C314">
+        <v>25783</v>
+      </c>
+      <c r="D314">
+        <v>33526854</v>
+      </c>
+      <c r="E314" t="s">
+        <v>27</v>
+      </c>
+      <c r="F314" t="s">
+        <v>45</v>
+      </c>
+      <c r="G314" t="s">
         <v>64</v>
       </c>
-      <c r="H313" t="s">
+      <c r="H314" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Fonds de solidarite] Add 2020-05-15 data + 2020-05-16 data + 2020-05-17 data
</commit_message>
<xml_diff>
--- a/published-data/fonds-solidarite-volet-1-regional-naf.xlsx
+++ b/published-data/fonds-solidarite-volet-1-regional-naf.xlsx
@@ -663,10 +663,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>5201</v>
+        <v>5461</v>
       </c>
       <c r="D2">
-        <v>7089599</v>
+        <v>7439709</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -715,10 +715,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>12523</v>
+        <v>12866</v>
       </c>
       <c r="D4">
-        <v>16121700</v>
+        <v>16568724</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -741,10 +741,10 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D5">
-        <v>84633</v>
+        <v>92133</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -767,10 +767,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>612</v>
+        <v>632</v>
       </c>
       <c r="D6">
-        <v>756441</v>
+        <v>778521</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -793,10 +793,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>35517</v>
+        <v>36653</v>
       </c>
       <c r="D7">
-        <v>51384011</v>
+        <v>53031932</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -819,10 +819,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>46173</v>
+        <v>47390</v>
       </c>
       <c r="D8">
-        <v>62441788</v>
+        <v>64045395</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -845,10 +845,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>9318</v>
+        <v>9604</v>
       </c>
       <c r="D9">
-        <v>13016604</v>
+        <v>13405261</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -871,10 +871,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>35492</v>
+        <v>36205</v>
       </c>
       <c r="D10">
-        <v>51351014</v>
+        <v>52370361</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -897,10 +897,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>4609</v>
+        <v>4739</v>
       </c>
       <c r="D11">
-        <v>6066134</v>
+        <v>6234897</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -923,10 +923,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>2106</v>
+        <v>2161</v>
       </c>
       <c r="D12">
-        <v>2976500</v>
+        <v>3051667</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -949,10 +949,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>8056</v>
+        <v>8308</v>
       </c>
       <c r="D13">
-        <v>11065606</v>
+        <v>11391527</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -975,10 +975,10 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>25061</v>
+        <v>25732</v>
       </c>
       <c r="D14">
-        <v>34151056</v>
+        <v>35049385</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1001,10 +1001,10 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>11705</v>
+        <v>12011</v>
       </c>
       <c r="D15">
-        <v>15228833</v>
+        <v>15629327</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1053,10 +1053,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>24924</v>
+        <v>25412</v>
       </c>
       <c r="D17">
-        <v>32046353</v>
+        <v>32642652</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1079,10 +1079,10 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>30503</v>
+        <v>31207</v>
       </c>
       <c r="D18">
-        <v>41460393</v>
+        <v>42429830</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1105,10 +1105,10 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>12691</v>
+        <v>13009</v>
       </c>
       <c r="D19">
-        <v>15585815</v>
+        <v>15972177</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1131,10 +1131,10 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>35253</v>
+        <v>35795</v>
       </c>
       <c r="D20">
-        <v>44168250</v>
+        <v>44806369</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1157,10 +1157,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>1973</v>
+        <v>2043</v>
       </c>
       <c r="D21">
-        <v>2714427</v>
+        <v>2808761</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1209,10 +1209,10 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>3526</v>
+        <v>3629</v>
       </c>
       <c r="D23">
-        <v>4455033</v>
+        <v>4586266</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -1261,10 +1261,10 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="D25">
-        <v>334801</v>
+        <v>347941</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
@@ -1287,10 +1287,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>8773</v>
+        <v>9028</v>
       </c>
       <c r="D26">
-        <v>12647718</v>
+        <v>13006049</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1313,10 +1313,10 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>14593</v>
+        <v>14906</v>
       </c>
       <c r="D27">
-        <v>19597520</v>
+        <v>20009676</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -1339,10 +1339,10 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>1373</v>
+        <v>1415</v>
       </c>
       <c r="D28">
-        <v>1883616</v>
+        <v>1937304</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1365,10 +1365,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>10461</v>
+        <v>10640</v>
       </c>
       <c r="D29">
-        <v>15009114</v>
+        <v>15263706</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
@@ -1391,10 +1391,10 @@
         <v>9</v>
       </c>
       <c r="C30">
-        <v>864</v>
+        <v>878</v>
       </c>
       <c r="D30">
-        <v>1085123</v>
+        <v>1100764</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
@@ -1417,10 +1417,10 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="D31">
-        <v>748711</v>
+        <v>758011</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -1443,10 +1443,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>1825</v>
+        <v>1883</v>
       </c>
       <c r="D32">
-        <v>2443550</v>
+        <v>2518482</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
@@ -1469,10 +1469,10 @@
         <v>9</v>
       </c>
       <c r="C33">
-        <v>4911</v>
+        <v>5026</v>
       </c>
       <c r="D33">
-        <v>6683102</v>
+        <v>6839342</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1495,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>2494</v>
+        <v>2543</v>
       </c>
       <c r="D34">
-        <v>3187609</v>
+        <v>3251711</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -1547,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>3504</v>
+        <v>3558</v>
       </c>
       <c r="D36">
-        <v>4233443</v>
+        <v>4302321</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -1573,10 +1573,10 @@
         <v>9</v>
       </c>
       <c r="C37">
-        <v>6690</v>
+        <v>6813</v>
       </c>
       <c r="D37">
-        <v>9035510</v>
+        <v>9198954</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>
@@ -1599,10 +1599,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>3213</v>
+        <v>3303</v>
       </c>
       <c r="D38">
-        <v>3888312</v>
+        <v>3976660</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
@@ -1625,10 +1625,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>11197</v>
+        <v>11334</v>
       </c>
       <c r="D39">
-        <v>14203432</v>
+        <v>14371603</v>
       </c>
       <c r="E39" t="s">
         <v>11</v>
@@ -1651,10 +1651,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>1758</v>
+        <v>1818</v>
       </c>
       <c r="D40">
-        <v>2414740</v>
+        <v>2496257</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -1677,10 +1677,10 @@
         <v>9</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D41">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -1703,10 +1703,10 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>4802</v>
+        <v>4907</v>
       </c>
       <c r="D42">
-        <v>5947646</v>
+        <v>6071676</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -1729,10 +1729,10 @@
         <v>9</v>
       </c>
       <c r="C43">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D43">
-        <v>19314</v>
+        <v>20805</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1755,10 +1755,10 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D44">
-        <v>226713</v>
+        <v>237247</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -1781,10 +1781,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>10187</v>
+        <v>10452</v>
       </c>
       <c r="D45">
-        <v>14664348</v>
+        <v>15049560</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1807,10 +1807,10 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>16307</v>
+        <v>16615</v>
       </c>
       <c r="D46">
-        <v>22182696</v>
+        <v>22597717</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -1833,10 +1833,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>1803</v>
+        <v>1848</v>
       </c>
       <c r="D47">
-        <v>2480154</v>
+        <v>2539374</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -1859,10 +1859,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>14159</v>
+        <v>14408</v>
       </c>
       <c r="D48">
-        <v>20447775</v>
+        <v>20811508</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -1885,10 +1885,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>1395</v>
+        <v>1421</v>
       </c>
       <c r="D49">
-        <v>1760921</v>
+        <v>1792922</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -1911,10 +1911,10 @@
         <v>9</v>
       </c>
       <c r="C50">
-        <v>658</v>
+        <v>673</v>
       </c>
       <c r="D50">
-        <v>930988</v>
+        <v>953488</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -1937,10 +1937,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>2617</v>
+        <v>2687</v>
       </c>
       <c r="D51">
-        <v>3485671</v>
+        <v>3566620</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -1963,10 +1963,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>7371</v>
+        <v>7530</v>
       </c>
       <c r="D52">
-        <v>9996165</v>
+        <v>10205898</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -1989,10 +1989,10 @@
         <v>9</v>
       </c>
       <c r="C53">
-        <v>3227</v>
+        <v>3301</v>
       </c>
       <c r="D53">
-        <v>4029411</v>
+        <v>4116065</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -2041,10 +2041,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>3889</v>
+        <v>3963</v>
       </c>
       <c r="D55">
-        <v>4801027</v>
+        <v>4884731</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2067,10 +2067,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>11146</v>
+        <v>11383</v>
       </c>
       <c r="D56">
-        <v>15271218</v>
+        <v>15597239</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2093,10 +2093,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>3907</v>
+        <v>3988</v>
       </c>
       <c r="D57">
-        <v>4696458</v>
+        <v>4780747</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2119,10 +2119,10 @@
         <v>9</v>
       </c>
       <c r="C58">
-        <v>12579</v>
+        <v>12725</v>
       </c>
       <c r="D58">
-        <v>16022083</v>
+        <v>16202888</v>
       </c>
       <c r="E58" t="s">
         <v>12</v>
@@ -2145,10 +2145,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>1476</v>
+        <v>1528</v>
       </c>
       <c r="D59">
-        <v>2036621</v>
+        <v>2104648</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
@@ -2171,10 +2171,10 @@
         <v>9</v>
       </c>
       <c r="C60">
-        <v>2920</v>
+        <v>2998</v>
       </c>
       <c r="D60">
-        <v>3744648</v>
+        <v>3847719</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
@@ -2197,10 +2197,10 @@
         <v>9</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D61">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -2223,10 +2223,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D62">
-        <v>158423</v>
+        <v>166854</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -2249,10 +2249,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>8859</v>
+        <v>9114</v>
       </c>
       <c r="D63">
-        <v>12709864</v>
+        <v>13075010</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -2275,10 +2275,10 @@
         <v>9</v>
       </c>
       <c r="C64">
-        <v>11870</v>
+        <v>12126</v>
       </c>
       <c r="D64">
-        <v>15716448</v>
+        <v>16051481</v>
       </c>
       <c r="E64" t="s">
         <v>13</v>
@@ -2301,10 +2301,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>1664</v>
+        <v>1726</v>
       </c>
       <c r="D65">
-        <v>2355421</v>
+        <v>2445321</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -2327,10 +2327,10 @@
         <v>9</v>
       </c>
       <c r="C66">
-        <v>8112</v>
+        <v>8291</v>
       </c>
       <c r="D66">
-        <v>11684814</v>
+        <v>11935752</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -2353,10 +2353,10 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>901</v>
+        <v>923</v>
       </c>
       <c r="D67">
-        <v>1164100</v>
+        <v>1192872</v>
       </c>
       <c r="E67" t="s">
         <v>13</v>
@@ -2379,10 +2379,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>441</v>
+        <v>456</v>
       </c>
       <c r="D68">
-        <v>624346</v>
+        <v>644257</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -2405,10 +2405,10 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>1846</v>
+        <v>1903</v>
       </c>
       <c r="D69">
-        <v>2494719</v>
+        <v>2562148</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -2431,10 +2431,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>4655</v>
+        <v>4761</v>
       </c>
       <c r="D70">
-        <v>6293513</v>
+        <v>6438199</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -2457,10 +2457,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>2483</v>
+        <v>2546</v>
       </c>
       <c r="D71">
-        <v>3155482</v>
+        <v>3238071</v>
       </c>
       <c r="E71" t="s">
         <v>13</v>
@@ -2483,10 +2483,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>2838</v>
+        <v>2895</v>
       </c>
       <c r="D72">
-        <v>3552858</v>
+        <v>3615651</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -2509,10 +2509,10 @@
         <v>9</v>
       </c>
       <c r="C73">
-        <v>5751</v>
+        <v>5872</v>
       </c>
       <c r="D73">
-        <v>7749459</v>
+        <v>7901016</v>
       </c>
       <c r="E73" t="s">
         <v>13</v>
@@ -2535,10 +2535,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>2839</v>
+        <v>2918</v>
       </c>
       <c r="D74">
-        <v>3482618</v>
+        <v>3576878</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -2561,10 +2561,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>9871</v>
+        <v>10022</v>
       </c>
       <c r="D75">
-        <v>12486553</v>
+        <v>12658485</v>
       </c>
       <c r="E75" t="s">
         <v>13</v>
@@ -2587,10 +2587,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>1186</v>
+        <v>1234</v>
       </c>
       <c r="D76">
-        <v>1645238</v>
+        <v>1715327</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
@@ -2613,10 +2613,10 @@
         <v>9</v>
       </c>
       <c r="C77">
-        <v>1102</v>
+        <v>1126</v>
       </c>
       <c r="D77">
-        <v>1466877</v>
+        <v>1500028</v>
       </c>
       <c r="E77" t="s">
         <v>14</v>
@@ -2639,10 +2639,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D78">
-        <v>17406</v>
+        <v>18906</v>
       </c>
       <c r="E78" t="s">
         <v>14</v>
@@ -2665,10 +2665,10 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>2939</v>
+        <v>3034</v>
       </c>
       <c r="D79">
-        <v>4181558</v>
+        <v>4320440</v>
       </c>
       <c r="E79" t="s">
         <v>14</v>
@@ -2691,10 +2691,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>2986</v>
+        <v>3074</v>
       </c>
       <c r="D80">
-        <v>4179664</v>
+        <v>4304257</v>
       </c>
       <c r="E80" t="s">
         <v>14</v>
@@ -2717,10 +2717,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="D81">
-        <v>606262</v>
+        <v>613762</v>
       </c>
       <c r="E81" t="s">
         <v>14</v>
@@ -2743,10 +2743,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>2746</v>
+        <v>2814</v>
       </c>
       <c r="D82">
-        <v>3948753</v>
+        <v>4045161</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2769,10 +2769,10 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D83">
-        <v>256466</v>
+        <v>265466</v>
       </c>
       <c r="E83" t="s">
         <v>14</v>
@@ -2795,10 +2795,10 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D84">
-        <v>104976</v>
+        <v>107476</v>
       </c>
       <c r="E84" t="s">
         <v>14</v>
@@ -2821,10 +2821,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>641</v>
+        <v>670</v>
       </c>
       <c r="D85">
-        <v>875733</v>
+        <v>917059</v>
       </c>
       <c r="E85" t="s">
         <v>14</v>
@@ -2847,10 +2847,10 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>1908</v>
+        <v>1959</v>
       </c>
       <c r="D86">
-        <v>2665293</v>
+        <v>2737550</v>
       </c>
       <c r="E86" t="s">
         <v>14</v>
@@ -2873,10 +2873,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>1063</v>
+        <v>1081</v>
       </c>
       <c r="D87">
-        <v>1355658</v>
+        <v>1379170</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -2899,10 +2899,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>547</v>
+        <v>559</v>
       </c>
       <c r="D88">
-        <v>679297</v>
+        <v>693001</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -2925,10 +2925,10 @@
         <v>9</v>
       </c>
       <c r="C89">
-        <v>1115</v>
+        <v>1136</v>
       </c>
       <c r="D89">
-        <v>1515762</v>
+        <v>1538524</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
@@ -2951,10 +2951,10 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>550</v>
+        <v>571</v>
       </c>
       <c r="D90">
-        <v>706424</v>
+        <v>733769</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
@@ -2977,10 +2977,10 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>1805</v>
+        <v>1835</v>
       </c>
       <c r="D91">
-        <v>2184477</v>
+        <v>2217451</v>
       </c>
       <c r="E91" t="s">
         <v>14</v>
@@ -3003,10 +3003,10 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>2607</v>
+        <v>2723</v>
       </c>
       <c r="D92">
-        <v>3623140</v>
+        <v>3783578</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -3055,10 +3055,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>6065</v>
+        <v>6224</v>
       </c>
       <c r="D94">
-        <v>7934690</v>
+        <v>8149404</v>
       </c>
       <c r="E94" t="s">
         <v>15</v>
@@ -3081,10 +3081,10 @@
         <v>9</v>
       </c>
       <c r="C95">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D95">
-        <v>13810</v>
+        <v>15310</v>
       </c>
       <c r="E95" t="s">
         <v>15</v>
@@ -3107,10 +3107,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>482</v>
+        <v>511</v>
       </c>
       <c r="D96">
-        <v>556534</v>
+        <v>591227</v>
       </c>
       <c r="E96" t="s">
         <v>15</v>
@@ -3133,10 +3133,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>18343</v>
+        <v>18888</v>
       </c>
       <c r="D97">
-        <v>26538966</v>
+        <v>27320862</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
@@ -3159,10 +3159,10 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>26262</v>
+        <v>26939</v>
       </c>
       <c r="D98">
-        <v>35492328</v>
+        <v>36393210</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -3185,10 +3185,10 @@
         <v>9</v>
       </c>
       <c r="C99">
-        <v>3539</v>
+        <v>3641</v>
       </c>
       <c r="D99">
-        <v>4846893</v>
+        <v>4980422</v>
       </c>
       <c r="E99" t="s">
         <v>15</v>
@@ -3211,10 +3211,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>16978</v>
+        <v>17332</v>
       </c>
       <c r="D100">
-        <v>24676439</v>
+        <v>25183079</v>
       </c>
       <c r="E100" t="s">
         <v>15</v>
@@ -3237,10 +3237,10 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>1883</v>
+        <v>1934</v>
       </c>
       <c r="D101">
-        <v>2429507</v>
+        <v>2498428</v>
       </c>
       <c r="E101" t="s">
         <v>15</v>
@@ -3263,10 +3263,10 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>1096</v>
+        <v>1123</v>
       </c>
       <c r="D102">
-        <v>1532391</v>
+        <v>1569504</v>
       </c>
       <c r="E102" t="s">
         <v>15</v>
@@ -3289,10 +3289,10 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>3034</v>
+        <v>3111</v>
       </c>
       <c r="D103">
-        <v>4145026</v>
+        <v>4248188</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
@@ -3315,10 +3315,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>10701</v>
+        <v>10998</v>
       </c>
       <c r="D104">
-        <v>14509711</v>
+        <v>14909127</v>
       </c>
       <c r="E104" t="s">
         <v>15</v>
@@ -3341,10 +3341,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>4826</v>
+        <v>4927</v>
       </c>
       <c r="D105">
-        <v>6178897</v>
+        <v>6301601</v>
       </c>
       <c r="E105" t="s">
         <v>15</v>
@@ -3393,10 +3393,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>5899</v>
+        <v>6015</v>
       </c>
       <c r="D107">
-        <v>7241104</v>
+        <v>7372258</v>
       </c>
       <c r="E107" t="s">
         <v>15</v>
@@ -3419,10 +3419,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>13202</v>
+        <v>13477</v>
       </c>
       <c r="D108">
-        <v>18243771</v>
+        <v>18619244</v>
       </c>
       <c r="E108" t="s">
         <v>15</v>
@@ -3445,10 +3445,10 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>5362</v>
+        <v>5487</v>
       </c>
       <c r="D109">
-        <v>6362522</v>
+        <v>6506624</v>
       </c>
       <c r="E109" t="s">
         <v>15</v>
@@ -3471,10 +3471,10 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>22166</v>
+        <v>22490</v>
       </c>
       <c r="D110">
-        <v>27333972</v>
+        <v>27729482</v>
       </c>
       <c r="E110" t="s">
         <v>15</v>
@@ -3497,10 +3497,10 @@
         <v>9</v>
       </c>
       <c r="C111">
-        <v>1262</v>
+        <v>1356</v>
       </c>
       <c r="D111">
-        <v>1764260</v>
+        <v>1895609</v>
       </c>
       <c r="E111" t="s">
         <v>16</v>
@@ -3523,10 +3523,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>1354</v>
+        <v>1411</v>
       </c>
       <c r="D112">
-        <v>1894086</v>
+        <v>1969143</v>
       </c>
       <c r="E112" t="s">
         <v>16</v>
@@ -3601,10 +3601,10 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>2256</v>
+        <v>2390</v>
       </c>
       <c r="D115">
-        <v>3265767</v>
+        <v>3458322</v>
       </c>
       <c r="E115" t="s">
         <v>16</v>
@@ -3627,10 +3627,10 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>3655</v>
+        <v>3839</v>
       </c>
       <c r="D116">
-        <v>5088516</v>
+        <v>5336575</v>
       </c>
       <c r="E116" t="s">
         <v>16</v>
@@ -3653,10 +3653,10 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>854</v>
+        <v>883</v>
       </c>
       <c r="D117">
-        <v>1211755</v>
+        <v>1252105</v>
       </c>
       <c r="E117" t="s">
         <v>16</v>
@@ -3679,10 +3679,10 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>2197</v>
+        <v>2329</v>
       </c>
       <c r="D118">
-        <v>3160958</v>
+        <v>3352105</v>
       </c>
       <c r="E118" t="s">
         <v>16</v>
@@ -3705,10 +3705,10 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="D119">
-        <v>484075</v>
+        <v>499187</v>
       </c>
       <c r="E119" t="s">
         <v>16</v>
@@ -3731,10 +3731,10 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D120">
-        <v>164436</v>
+        <v>173436</v>
       </c>
       <c r="E120" t="s">
         <v>16</v>
@@ -3757,10 +3757,10 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>498</v>
+        <v>517</v>
       </c>
       <c r="D121">
-        <v>697146</v>
+        <v>723626</v>
       </c>
       <c r="E121" t="s">
         <v>16</v>
@@ -3783,10 +3783,10 @@
         <v>9</v>
       </c>
       <c r="C122">
-        <v>1376</v>
+        <v>1446</v>
       </c>
       <c r="D122">
-        <v>1928270</v>
+        <v>2025033</v>
       </c>
       <c r="E122" t="s">
         <v>16</v>
@@ -3809,10 +3809,10 @@
         <v>9</v>
       </c>
       <c r="C123">
-        <v>1513</v>
+        <v>1564</v>
       </c>
       <c r="D123">
-        <v>2049281</v>
+        <v>2119704</v>
       </c>
       <c r="E123" t="s">
         <v>16</v>
@@ -3835,10 +3835,10 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>809</v>
+        <v>846</v>
       </c>
       <c r="D124">
-        <v>1042434</v>
+        <v>1087400</v>
       </c>
       <c r="E124" t="s">
         <v>16</v>
@@ -3861,10 +3861,10 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>1224</v>
+        <v>1271</v>
       </c>
       <c r="D125">
-        <v>1736935</v>
+        <v>1806665</v>
       </c>
       <c r="E125" t="s">
         <v>16</v>
@@ -3887,10 +3887,10 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>503</v>
+        <v>527</v>
       </c>
       <c r="D126">
-        <v>664991</v>
+        <v>696557</v>
       </c>
       <c r="E126" t="s">
         <v>16</v>
@@ -3913,10 +3913,10 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>1447</v>
+        <v>1518</v>
       </c>
       <c r="D127">
-        <v>1877011</v>
+        <v>1975358</v>
       </c>
       <c r="E127" t="s">
         <v>16</v>
@@ -3939,10 +3939,10 @@
         <v>9</v>
       </c>
       <c r="C128">
-        <v>524</v>
+        <v>566</v>
       </c>
       <c r="D128">
-        <v>711795</v>
+        <v>767982</v>
       </c>
       <c r="E128" t="s">
         <v>17</v>
@@ -3991,10 +3991,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="D130">
-        <v>365802</v>
+        <v>383619</v>
       </c>
       <c r="E130" t="s">
         <v>17</v>
@@ -4043,10 +4043,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>552</v>
+        <v>615</v>
       </c>
       <c r="D132">
-        <v>803969</v>
+        <v>897969</v>
       </c>
       <c r="E132" t="s">
         <v>17</v>
@@ -4069,10 +4069,10 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>688</v>
+        <v>726</v>
       </c>
       <c r="D133">
-        <v>975610</v>
+        <v>1029070</v>
       </c>
       <c r="E133" t="s">
         <v>17</v>
@@ -4095,10 +4095,10 @@
         <v>9</v>
       </c>
       <c r="C134">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="D134">
-        <v>245574</v>
+        <v>267859</v>
       </c>
       <c r="E134" t="s">
         <v>17</v>
@@ -4121,10 +4121,10 @@
         <v>9</v>
       </c>
       <c r="C135">
-        <v>447</v>
+        <v>485</v>
       </c>
       <c r="D135">
-        <v>639260</v>
+        <v>690826</v>
       </c>
       <c r="E135" t="s">
         <v>17</v>
@@ -4147,10 +4147,10 @@
         <v>9</v>
       </c>
       <c r="C136">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D136">
-        <v>97772</v>
+        <v>99272</v>
       </c>
       <c r="E136" t="s">
         <v>17</v>
@@ -4173,10 +4173,10 @@
         <v>9</v>
       </c>
       <c r="C137">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D137">
-        <v>62668</v>
+        <v>70329</v>
       </c>
       <c r="E137" t="s">
         <v>17</v>
@@ -4225,10 +4225,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="D139">
-        <v>490385</v>
+        <v>507810</v>
       </c>
       <c r="E139" t="s">
         <v>17</v>
@@ -4251,10 +4251,10 @@
         <v>9</v>
       </c>
       <c r="C140">
-        <v>271</v>
+        <v>292</v>
       </c>
       <c r="D140">
-        <v>376992</v>
+        <v>406289</v>
       </c>
       <c r="E140" t="s">
         <v>17</v>
@@ -4277,10 +4277,10 @@
         <v>9</v>
       </c>
       <c r="C141">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="D141">
-        <v>245460</v>
+        <v>260961</v>
       </c>
       <c r="E141" t="s">
         <v>17</v>
@@ -4303,10 +4303,10 @@
         <v>9</v>
       </c>
       <c r="C142">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="D142">
-        <v>317160</v>
+        <v>337670</v>
       </c>
       <c r="E142" t="s">
         <v>17</v>
@@ -4329,10 +4329,10 @@
         <v>9</v>
       </c>
       <c r="C143">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D143">
-        <v>136251</v>
+        <v>139991</v>
       </c>
       <c r="E143" t="s">
         <v>17</v>
@@ -4355,10 +4355,10 @@
         <v>9</v>
       </c>
       <c r="C144">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="D144">
-        <v>364506</v>
+        <v>379186</v>
       </c>
       <c r="E144" t="s">
         <v>17</v>
@@ -4381,10 +4381,10 @@
         <v>9</v>
       </c>
       <c r="C145">
-        <v>1555</v>
+        <v>1602</v>
       </c>
       <c r="D145">
-        <v>2109452</v>
+        <v>2176639</v>
       </c>
       <c r="E145" t="s">
         <v>18</v>
@@ -4433,10 +4433,10 @@
         <v>9</v>
       </c>
       <c r="C147">
-        <v>4790</v>
+        <v>4912</v>
       </c>
       <c r="D147">
-        <v>5967873</v>
+        <v>6129047</v>
       </c>
       <c r="E147" t="s">
         <v>18</v>
@@ -4485,10 +4485,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D149">
-        <v>285278</v>
+        <v>298498</v>
       </c>
       <c r="E149" t="s">
         <v>18</v>
@@ -4511,10 +4511,10 @@
         <v>9</v>
       </c>
       <c r="C150">
-        <v>15758</v>
+        <v>16151</v>
       </c>
       <c r="D150">
-        <v>22468221</v>
+        <v>23025876</v>
       </c>
       <c r="E150" t="s">
         <v>18</v>
@@ -4537,10 +4537,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>26001</v>
+        <v>26580</v>
       </c>
       <c r="D151">
-        <v>33731004</v>
+        <v>34466370</v>
       </c>
       <c r="E151" t="s">
         <v>18</v>
@@ -4563,10 +4563,10 @@
         <v>9</v>
       </c>
       <c r="C152">
-        <v>5493</v>
+        <v>5651</v>
       </c>
       <c r="D152">
-        <v>7592688</v>
+        <v>7789767</v>
       </c>
       <c r="E152" t="s">
         <v>18</v>
@@ -4589,10 +4589,10 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>16643</v>
+        <v>16985</v>
       </c>
       <c r="D153">
-        <v>24154089</v>
+        <v>24652705</v>
       </c>
       <c r="E153" t="s">
         <v>18</v>
@@ -4615,10 +4615,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>1857</v>
+        <v>1904</v>
       </c>
       <c r="D154">
-        <v>2405777</v>
+        <v>2468915</v>
       </c>
       <c r="E154" t="s">
         <v>18</v>
@@ -4641,10 +4641,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>1131</v>
+        <v>1147</v>
       </c>
       <c r="D155">
-        <v>1596287</v>
+        <v>1618169</v>
       </c>
       <c r="E155" t="s">
         <v>18</v>
@@ -4667,10 +4667,10 @@
         <v>9</v>
       </c>
       <c r="C156">
-        <v>2935</v>
+        <v>3005</v>
       </c>
       <c r="D156">
-        <v>3983391</v>
+        <v>4069252</v>
       </c>
       <c r="E156" t="s">
         <v>18</v>
@@ -4693,10 +4693,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>10690</v>
+        <v>10911</v>
       </c>
       <c r="D157">
-        <v>14598420</v>
+        <v>14895421</v>
       </c>
       <c r="E157" t="s">
         <v>18</v>
@@ -4719,10 +4719,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>4851</v>
+        <v>4961</v>
       </c>
       <c r="D158">
-        <v>6098449</v>
+        <v>6232599</v>
       </c>
       <c r="E158" t="s">
         <v>18</v>
@@ -4745,10 +4745,10 @@
         <v>9</v>
       </c>
       <c r="C159">
-        <v>5280</v>
+        <v>5367</v>
       </c>
       <c r="D159">
-        <v>6599725</v>
+        <v>6704405</v>
       </c>
       <c r="E159" t="s">
         <v>18</v>
@@ -4771,10 +4771,10 @@
         <v>9</v>
       </c>
       <c r="C160">
-        <v>13705</v>
+        <v>13979</v>
       </c>
       <c r="D160">
-        <v>18847655</v>
+        <v>19229617</v>
       </c>
       <c r="E160" t="s">
         <v>18</v>
@@ -4797,10 +4797,10 @@
         <v>9</v>
       </c>
       <c r="C161">
-        <v>5287</v>
+        <v>5419</v>
       </c>
       <c r="D161">
-        <v>6390693</v>
+        <v>6541109</v>
       </c>
       <c r="E161" t="s">
         <v>18</v>
@@ -4823,10 +4823,10 @@
         <v>9</v>
       </c>
       <c r="C162">
-        <v>21784</v>
+        <v>22026</v>
       </c>
       <c r="D162">
-        <v>26145722</v>
+        <v>26417729</v>
       </c>
       <c r="E162" t="s">
         <v>18</v>
@@ -4849,10 +4849,10 @@
         <v>9</v>
       </c>
       <c r="C163">
-        <v>1609</v>
+        <v>1693</v>
       </c>
       <c r="D163">
-        <v>2158498</v>
+        <v>2268744</v>
       </c>
       <c r="E163" t="s">
         <v>19</v>
@@ -4901,10 +4901,10 @@
         <v>9</v>
       </c>
       <c r="C165">
-        <v>2284</v>
+        <v>2350</v>
       </c>
       <c r="D165">
-        <v>3091358</v>
+        <v>3180759</v>
       </c>
       <c r="E165" t="s">
         <v>19</v>
@@ -4927,10 +4927,10 @@
         <v>9</v>
       </c>
       <c r="C166">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D166">
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="E166" t="s">
         <v>19</v>
@@ -4953,10 +4953,10 @@
         <v>9</v>
       </c>
       <c r="C167">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D167">
-        <v>62673</v>
+        <v>64173</v>
       </c>
       <c r="E167" t="s">
         <v>19</v>
@@ -4979,10 +4979,10 @@
         <v>9</v>
       </c>
       <c r="C168">
-        <v>4550</v>
+        <v>4638</v>
       </c>
       <c r="D168">
-        <v>6644564</v>
+        <v>6771624</v>
       </c>
       <c r="E168" t="s">
         <v>19</v>
@@ -5005,10 +5005,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>7547</v>
+        <v>7706</v>
       </c>
       <c r="D169">
-        <v>10427234</v>
+        <v>10627931</v>
       </c>
       <c r="E169" t="s">
         <v>19</v>
@@ -5031,10 +5031,10 @@
         <v>9</v>
       </c>
       <c r="C170">
-        <v>988</v>
+        <v>1030</v>
       </c>
       <c r="D170">
-        <v>1393425</v>
+        <v>1452012</v>
       </c>
       <c r="E170" t="s">
         <v>19</v>
@@ -5057,10 +5057,10 @@
         <v>9</v>
       </c>
       <c r="C171">
-        <v>3693</v>
+        <v>3762</v>
       </c>
       <c r="D171">
-        <v>5249322</v>
+        <v>5348519</v>
       </c>
       <c r="E171" t="s">
         <v>19</v>
@@ -5083,10 +5083,10 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="D172">
-        <v>686394</v>
+        <v>703539</v>
       </c>
       <c r="E172" t="s">
         <v>19</v>
@@ -5109,10 +5109,10 @@
         <v>9</v>
       </c>
       <c r="C173">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D173">
-        <v>323724</v>
+        <v>329724</v>
       </c>
       <c r="E173" t="s">
         <v>19</v>
@@ -5135,10 +5135,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>846</v>
+        <v>892</v>
       </c>
       <c r="D174">
-        <v>1196677</v>
+        <v>1263423</v>
       </c>
       <c r="E174" t="s">
         <v>19</v>
@@ -5161,10 +5161,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>2386</v>
+        <v>2447</v>
       </c>
       <c r="D175">
-        <v>3373957</v>
+        <v>3459325</v>
       </c>
       <c r="E175" t="s">
         <v>19</v>
@@ -5187,10 +5187,10 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>1320</v>
+        <v>1391</v>
       </c>
       <c r="D176">
-        <v>1831980</v>
+        <v>1934469</v>
       </c>
       <c r="E176" t="s">
         <v>19</v>
@@ -5213,10 +5213,10 @@
         <v>9</v>
       </c>
       <c r="C177">
-        <v>1914</v>
+        <v>1945</v>
       </c>
       <c r="D177">
-        <v>2513337</v>
+        <v>2554364</v>
       </c>
       <c r="E177" t="s">
         <v>19</v>
@@ -5239,10 +5239,10 @@
         <v>9</v>
       </c>
       <c r="C178">
-        <v>3045</v>
+        <v>3132</v>
       </c>
       <c r="D178">
-        <v>4332117</v>
+        <v>4459191</v>
       </c>
       <c r="E178" t="s">
         <v>19</v>
@@ -5265,10 +5265,10 @@
         <v>9</v>
       </c>
       <c r="C179">
-        <v>1106</v>
+        <v>1134</v>
       </c>
       <c r="D179">
-        <v>1449382</v>
+        <v>1484830</v>
       </c>
       <c r="E179" t="s">
         <v>19</v>
@@ -5291,10 +5291,10 @@
         <v>9</v>
       </c>
       <c r="C180">
-        <v>3174</v>
+        <v>3223</v>
       </c>
       <c r="D180">
-        <v>4108324</v>
+        <v>4171121</v>
       </c>
       <c r="E180" t="s">
         <v>19</v>
@@ -5317,10 +5317,10 @@
         <v>9</v>
       </c>
       <c r="C181">
-        <v>613</v>
+        <v>662</v>
       </c>
       <c r="D181">
-        <v>786021</v>
+        <v>849340</v>
       </c>
       <c r="E181" t="s">
         <v>20</v>
@@ -5343,10 +5343,10 @@
         <v>9</v>
       </c>
       <c r="C182">
-        <v>972</v>
+        <v>1019</v>
       </c>
       <c r="D182">
-        <v>1313019</v>
+        <v>1377239</v>
       </c>
       <c r="E182" t="s">
         <v>20</v>
@@ -5421,10 +5421,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>1472</v>
+        <v>1575</v>
       </c>
       <c r="D185">
-        <v>2129422</v>
+        <v>2280567</v>
       </c>
       <c r="E185" t="s">
         <v>20</v>
@@ -5447,10 +5447,10 @@
         <v>9</v>
       </c>
       <c r="C186">
-        <v>2674</v>
+        <v>2767</v>
       </c>
       <c r="D186">
-        <v>3705043</v>
+        <v>3830675</v>
       </c>
       <c r="E186" t="s">
         <v>20</v>
@@ -5473,10 +5473,10 @@
         <v>9</v>
       </c>
       <c r="C187">
-        <v>820</v>
+        <v>872</v>
       </c>
       <c r="D187">
-        <v>1158612</v>
+        <v>1233839</v>
       </c>
       <c r="E187" t="s">
         <v>20</v>
@@ -5499,10 +5499,10 @@
         <v>9</v>
       </c>
       <c r="C188">
-        <v>1504</v>
+        <v>1556</v>
       </c>
       <c r="D188">
-        <v>2179697</v>
+        <v>2251799</v>
       </c>
       <c r="E188" t="s">
         <v>20</v>
@@ -5525,10 +5525,10 @@
         <v>9</v>
       </c>
       <c r="C189">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="D189">
-        <v>298014</v>
+        <v>324234</v>
       </c>
       <c r="E189" t="s">
         <v>20</v>
@@ -5551,10 +5551,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D190">
-        <v>160920</v>
+        <v>165420</v>
       </c>
       <c r="E190" t="s">
         <v>20</v>
@@ -5577,10 +5577,10 @@
         <v>9</v>
       </c>
       <c r="C191">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="D191">
-        <v>458850</v>
+        <v>472350</v>
       </c>
       <c r="E191" t="s">
         <v>20</v>
@@ -5603,10 +5603,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>1265</v>
+        <v>1322</v>
       </c>
       <c r="D192">
-        <v>1766490</v>
+        <v>1846883</v>
       </c>
       <c r="E192" t="s">
         <v>20</v>
@@ -5629,10 +5629,10 @@
         <v>9</v>
       </c>
       <c r="C193">
-        <v>1091</v>
+        <v>1156</v>
       </c>
       <c r="D193">
-        <v>1498664</v>
+        <v>1593561</v>
       </c>
       <c r="E193" t="s">
         <v>20</v>
@@ -5655,10 +5655,10 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>635</v>
+        <v>658</v>
       </c>
       <c r="D194">
-        <v>828698</v>
+        <v>854633</v>
       </c>
       <c r="E194" t="s">
         <v>20</v>
@@ -5681,10 +5681,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>1141</v>
+        <v>1179</v>
       </c>
       <c r="D195">
-        <v>1599038</v>
+        <v>1653988</v>
       </c>
       <c r="E195" t="s">
         <v>20</v>
@@ -5707,10 +5707,10 @@
         <v>9</v>
       </c>
       <c r="C196">
-        <v>434</v>
+        <v>453</v>
       </c>
       <c r="D196">
-        <v>573318</v>
+        <v>598382</v>
       </c>
       <c r="E196" t="s">
         <v>20</v>
@@ -5733,10 +5733,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>1465</v>
+        <v>1499</v>
       </c>
       <c r="D197">
-        <v>1931360</v>
+        <v>1980768</v>
       </c>
       <c r="E197" t="s">
         <v>20</v>
@@ -5759,10 +5759,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="D198">
-        <v>251629</v>
+        <v>275329</v>
       </c>
       <c r="E198" t="s">
         <v>21</v>
@@ -5785,10 +5785,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D199">
-        <v>199617</v>
+        <v>213267</v>
       </c>
       <c r="E199" t="s">
         <v>21</v>
@@ -5837,10 +5837,10 @@
         <v>9</v>
       </c>
       <c r="C201">
-        <v>365</v>
+        <v>403</v>
       </c>
       <c r="D201">
-        <v>535868</v>
+        <v>592868</v>
       </c>
       <c r="E201" t="s">
         <v>21</v>
@@ -5863,10 +5863,10 @@
         <v>9</v>
       </c>
       <c r="C202">
-        <v>1129</v>
+        <v>1265</v>
       </c>
       <c r="D202">
-        <v>1556268</v>
+        <v>1749508</v>
       </c>
       <c r="E202" t="s">
         <v>21</v>
@@ -5889,10 +5889,10 @@
         <v>9</v>
       </c>
       <c r="C203">
-        <v>346</v>
+        <v>391</v>
       </c>
       <c r="D203">
-        <v>508614</v>
+        <v>575408</v>
       </c>
       <c r="E203" t="s">
         <v>21</v>
@@ -5915,10 +5915,10 @@
         <v>9</v>
       </c>
       <c r="C204">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="D204">
-        <v>366751</v>
+        <v>381751</v>
       </c>
       <c r="E204" t="s">
         <v>21</v>
@@ -5941,10 +5941,10 @@
         <v>9</v>
       </c>
       <c r="C205">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D205">
-        <v>50080</v>
+        <v>54580</v>
       </c>
       <c r="E205" t="s">
         <v>21</v>
@@ -5967,10 +5967,10 @@
         <v>9</v>
       </c>
       <c r="C206">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D206">
-        <v>12000</v>
+        <v>13500</v>
       </c>
       <c r="E206" t="s">
         <v>21</v>
@@ -6019,10 +6019,10 @@
         <v>9</v>
       </c>
       <c r="C208">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D208">
-        <v>173349</v>
+        <v>180849</v>
       </c>
       <c r="E208" t="s">
         <v>21</v>
@@ -6045,10 +6045,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D209">
-        <v>125543</v>
+        <v>130043</v>
       </c>
       <c r="E209" t="s">
         <v>21</v>
@@ -6071,10 +6071,10 @@
         <v>9</v>
       </c>
       <c r="C210">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D210">
-        <v>141272</v>
+        <v>144839</v>
       </c>
       <c r="E210" t="s">
         <v>21</v>
@@ -6097,10 +6097,10 @@
         <v>9</v>
       </c>
       <c r="C211">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D211">
-        <v>98255</v>
+        <v>105755</v>
       </c>
       <c r="E211" t="s">
         <v>21</v>
@@ -6149,10 +6149,10 @@
         <v>9</v>
       </c>
       <c r="C213">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="D213">
-        <v>149598</v>
+        <v>170598</v>
       </c>
       <c r="E213" t="s">
         <v>21</v>
@@ -6175,10 +6175,10 @@
         <v>9</v>
       </c>
       <c r="C214">
-        <v>1800</v>
+        <v>1851</v>
       </c>
       <c r="D214">
-        <v>2460381</v>
+        <v>2532261</v>
       </c>
       <c r="E214" t="s">
         <v>22</v>
@@ -6227,10 +6227,10 @@
         <v>9</v>
       </c>
       <c r="C216">
-        <v>3319</v>
+        <v>3430</v>
       </c>
       <c r="D216">
-        <v>4237921</v>
+        <v>4387111</v>
       </c>
       <c r="E216" t="s">
         <v>22</v>
@@ -6279,10 +6279,10 @@
         <v>9</v>
       </c>
       <c r="C218">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D218">
-        <v>235741</v>
+        <v>242581</v>
       </c>
       <c r="E218" t="s">
         <v>22</v>
@@ -6305,10 +6305,10 @@
         <v>9</v>
       </c>
       <c r="C219">
-        <v>9714</v>
+        <v>9996</v>
       </c>
       <c r="D219">
-        <v>13955652</v>
+        <v>14364326</v>
       </c>
       <c r="E219" t="s">
         <v>22</v>
@@ -6331,10 +6331,10 @@
         <v>9</v>
       </c>
       <c r="C220">
-        <v>16793</v>
+        <v>17173</v>
       </c>
       <c r="D220">
-        <v>22386552</v>
+        <v>22866655</v>
       </c>
       <c r="E220" t="s">
         <v>22</v>
@@ -6357,10 +6357,10 @@
         <v>9</v>
       </c>
       <c r="C221">
-        <v>1966</v>
+        <v>2011</v>
       </c>
       <c r="D221">
-        <v>2717687</v>
+        <v>2776853</v>
       </c>
       <c r="E221" t="s">
         <v>22</v>
@@ -6383,10 +6383,10 @@
         <v>9</v>
       </c>
       <c r="C222">
-        <v>11307</v>
+        <v>11522</v>
       </c>
       <c r="D222">
-        <v>16321634</v>
+        <v>16625829</v>
       </c>
       <c r="E222" t="s">
         <v>22</v>
@@ -6409,10 +6409,10 @@
         <v>9</v>
       </c>
       <c r="C223">
-        <v>1006</v>
+        <v>1026</v>
       </c>
       <c r="D223">
-        <v>1276323</v>
+        <v>1297348</v>
       </c>
       <c r="E223" t="s">
         <v>22</v>
@@ -6435,10 +6435,10 @@
         <v>9</v>
       </c>
       <c r="C224">
-        <v>673</v>
+        <v>689</v>
       </c>
       <c r="D224">
-        <v>942360</v>
+        <v>965871</v>
       </c>
       <c r="E224" t="s">
         <v>22</v>
@@ -6461,10 +6461,10 @@
         <v>9</v>
       </c>
       <c r="C225">
-        <v>2068</v>
+        <v>2130</v>
       </c>
       <c r="D225">
-        <v>2768167</v>
+        <v>2848540</v>
       </c>
       <c r="E225" t="s">
         <v>22</v>
@@ -6487,10 +6487,10 @@
         <v>9</v>
       </c>
       <c r="C226">
-        <v>6215</v>
+        <v>6336</v>
       </c>
       <c r="D226">
-        <v>8485806</v>
+        <v>8642933</v>
       </c>
       <c r="E226" t="s">
         <v>22</v>
@@ -6513,10 +6513,10 @@
         <v>9</v>
       </c>
       <c r="C227">
-        <v>2813</v>
+        <v>2892</v>
       </c>
       <c r="D227">
-        <v>3525853</v>
+        <v>3627061</v>
       </c>
       <c r="E227" t="s">
         <v>22</v>
@@ -6539,10 +6539,10 @@
         <v>9</v>
       </c>
       <c r="C228">
-        <v>3415</v>
+        <v>3466</v>
       </c>
       <c r="D228">
-        <v>4149918</v>
+        <v>4207624</v>
       </c>
       <c r="E228" t="s">
         <v>22</v>
@@ -6565,10 +6565,10 @@
         <v>9</v>
       </c>
       <c r="C229">
-        <v>6897</v>
+        <v>7049</v>
       </c>
       <c r="D229">
-        <v>9291142</v>
+        <v>9496688</v>
       </c>
       <c r="E229" t="s">
         <v>22</v>
@@ -6591,10 +6591,10 @@
         <v>9</v>
       </c>
       <c r="C230">
-        <v>3546</v>
+        <v>3651</v>
       </c>
       <c r="D230">
-        <v>4343920</v>
+        <v>4463908</v>
       </c>
       <c r="E230" t="s">
         <v>22</v>
@@ -6617,10 +6617,10 @@
         <v>9</v>
       </c>
       <c r="C231">
-        <v>13372</v>
+        <v>13547</v>
       </c>
       <c r="D231">
-        <v>16712648</v>
+        <v>16917914</v>
       </c>
       <c r="E231" t="s">
         <v>22</v>
@@ -6643,10 +6643,10 @@
         <v>9</v>
       </c>
       <c r="C232">
-        <v>6326</v>
+        <v>6615</v>
       </c>
       <c r="D232">
-        <v>8778961</v>
+        <v>9177754</v>
       </c>
       <c r="E232" t="s">
         <v>23</v>
@@ -6669,10 +6669,10 @@
         <v>9</v>
       </c>
       <c r="C233">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D233">
-        <v>47623</v>
+        <v>50300</v>
       </c>
       <c r="E233" t="s">
         <v>23</v>
@@ -6695,10 +6695,10 @@
         <v>9</v>
       </c>
       <c r="C234">
-        <v>10357</v>
+        <v>10605</v>
       </c>
       <c r="D234">
-        <v>12887104</v>
+        <v>13190873</v>
       </c>
       <c r="E234" t="s">
         <v>23</v>
@@ -6721,10 +6721,10 @@
         <v>9</v>
       </c>
       <c r="C235">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D235">
-        <v>46319</v>
+        <v>47819</v>
       </c>
       <c r="E235" t="s">
         <v>23</v>
@@ -6747,10 +6747,10 @@
         <v>9</v>
       </c>
       <c r="C236">
-        <v>497</v>
+        <v>516</v>
       </c>
       <c r="D236">
-        <v>550948</v>
+        <v>569527</v>
       </c>
       <c r="E236" t="s">
         <v>23</v>
@@ -6773,10 +6773,10 @@
         <v>9</v>
       </c>
       <c r="C237">
-        <v>27958</v>
+        <v>28770</v>
       </c>
       <c r="D237">
-        <v>39930562</v>
+        <v>41080136</v>
       </c>
       <c r="E237" t="s">
         <v>23</v>
@@ -6799,10 +6799,10 @@
         <v>9</v>
       </c>
       <c r="C238">
-        <v>38738</v>
+        <v>39565</v>
       </c>
       <c r="D238">
-        <v>51740294</v>
+        <v>52808243</v>
       </c>
       <c r="E238" t="s">
         <v>23</v>
@@ -6825,10 +6825,10 @@
         <v>9</v>
       </c>
       <c r="C239">
-        <v>5001</v>
+        <v>5126</v>
       </c>
       <c r="D239">
-        <v>6870338</v>
+        <v>7045083</v>
       </c>
       <c r="E239" t="s">
         <v>23</v>
@@ -6851,10 +6851,10 @@
         <v>9</v>
       </c>
       <c r="C240">
-        <v>24924</v>
+        <v>25368</v>
       </c>
       <c r="D240">
-        <v>35475922</v>
+        <v>36097816</v>
       </c>
       <c r="E240" t="s">
         <v>23</v>
@@ -6877,10 +6877,10 @@
         <v>9</v>
       </c>
       <c r="C241">
-        <v>2991</v>
+        <v>3076</v>
       </c>
       <c r="D241">
-        <v>3885368</v>
+        <v>3992019</v>
       </c>
       <c r="E241" t="s">
         <v>23</v>
@@ -6903,10 +6903,10 @@
         <v>9</v>
       </c>
       <c r="C242">
-        <v>1696</v>
+        <v>1720</v>
       </c>
       <c r="D242">
-        <v>2387041</v>
+        <v>2419967</v>
       </c>
       <c r="E242" t="s">
         <v>23</v>
@@ -6929,10 +6929,10 @@
         <v>9</v>
       </c>
       <c r="C243">
-        <v>6188</v>
+        <v>6345</v>
       </c>
       <c r="D243">
-        <v>8291744</v>
+        <v>8484598</v>
       </c>
       <c r="E243" t="s">
         <v>23</v>
@@ -6955,10 +6955,10 @@
         <v>9</v>
       </c>
       <c r="C244">
-        <v>18187</v>
+        <v>18598</v>
       </c>
       <c r="D244">
-        <v>24550326</v>
+        <v>25093349</v>
       </c>
       <c r="E244" t="s">
         <v>23</v>
@@ -6981,10 +6981,10 @@
         <v>9</v>
       </c>
       <c r="C245">
-        <v>9065</v>
+        <v>9290</v>
       </c>
       <c r="D245">
-        <v>11368940</v>
+        <v>11647176</v>
       </c>
       <c r="E245" t="s">
         <v>23</v>
@@ -7033,10 +7033,10 @@
         <v>9</v>
       </c>
       <c r="C247">
-        <v>9810</v>
+        <v>10014</v>
       </c>
       <c r="D247">
-        <v>11580536</v>
+        <v>11801493</v>
       </c>
       <c r="E247" t="s">
         <v>23</v>
@@ -7059,10 +7059,10 @@
         <v>9</v>
       </c>
       <c r="C248">
-        <v>22357</v>
+        <v>22811</v>
       </c>
       <c r="D248">
-        <v>29974839</v>
+        <v>30592646</v>
       </c>
       <c r="E248" t="s">
         <v>23</v>
@@ -7085,10 +7085,10 @@
         <v>9</v>
       </c>
       <c r="C249">
-        <v>8761</v>
+        <v>8948</v>
       </c>
       <c r="D249">
-        <v>10555994</v>
+        <v>10769994</v>
       </c>
       <c r="E249" t="s">
         <v>23</v>
@@ -7111,10 +7111,10 @@
         <v>9</v>
       </c>
       <c r="C250">
-        <v>29732</v>
+        <v>30151</v>
       </c>
       <c r="D250">
-        <v>36651256</v>
+        <v>37136046</v>
       </c>
       <c r="E250" t="s">
         <v>23</v>
@@ -7137,10 +7137,10 @@
         <v>9</v>
       </c>
       <c r="C251">
-        <v>6534</v>
+        <v>6772</v>
       </c>
       <c r="D251">
-        <v>8815209</v>
+        <v>9140475</v>
       </c>
       <c r="E251" t="s">
         <v>24</v>
@@ -7163,10 +7163,10 @@
         <v>9</v>
       </c>
       <c r="C252">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D252">
-        <v>34662</v>
+        <v>37662</v>
       </c>
       <c r="E252" t="s">
         <v>24</v>
@@ -7189,10 +7189,10 @@
         <v>9</v>
       </c>
       <c r="C253">
-        <v>10878</v>
+        <v>11143</v>
       </c>
       <c r="D253">
-        <v>13574488</v>
+        <v>13902500</v>
       </c>
       <c r="E253" t="s">
         <v>24</v>
@@ -7241,10 +7241,10 @@
         <v>9</v>
       </c>
       <c r="C255">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="D255">
-        <v>467490</v>
+        <v>474990</v>
       </c>
       <c r="E255" t="s">
         <v>24</v>
@@ -7267,10 +7267,10 @@
         <v>9</v>
       </c>
       <c r="C256">
-        <v>34776</v>
+        <v>35846</v>
       </c>
       <c r="D256">
-        <v>49505851</v>
+        <v>51030203</v>
       </c>
       <c r="E256" t="s">
         <v>24</v>
@@ -7293,10 +7293,10 @@
         <v>9</v>
       </c>
       <c r="C257">
-        <v>43023</v>
+        <v>43932</v>
       </c>
       <c r="D257">
-        <v>57131850</v>
+        <v>58317196</v>
       </c>
       <c r="E257" t="s">
         <v>24</v>
@@ -7319,10 +7319,10 @@
         <v>9</v>
       </c>
       <c r="C258">
-        <v>5607</v>
+        <v>5774</v>
       </c>
       <c r="D258">
-        <v>7530584</v>
+        <v>7744477</v>
       </c>
       <c r="E258" t="s">
         <v>24</v>
@@ -7345,10 +7345,10 @@
         <v>9</v>
       </c>
       <c r="C259">
-        <v>29231</v>
+        <v>29795</v>
       </c>
       <c r="D259">
-        <v>41649482</v>
+        <v>42444332</v>
       </c>
       <c r="E259" t="s">
         <v>24</v>
@@ -7371,10 +7371,10 @@
         <v>9</v>
       </c>
       <c r="C260">
-        <v>3534</v>
+        <v>3617</v>
       </c>
       <c r="D260">
-        <v>4542496</v>
+        <v>4639772</v>
       </c>
       <c r="E260" t="s">
         <v>24</v>
@@ -7397,10 +7397,10 @@
         <v>9</v>
       </c>
       <c r="C261">
-        <v>1739</v>
+        <v>1782</v>
       </c>
       <c r="D261">
-        <v>2417244</v>
+        <v>2475471</v>
       </c>
       <c r="E261" t="s">
         <v>24</v>
@@ -7423,10 +7423,10 @@
         <v>9</v>
       </c>
       <c r="C262">
-        <v>7079</v>
+        <v>7256</v>
       </c>
       <c r="D262">
-        <v>9528905</v>
+        <v>9750630</v>
       </c>
       <c r="E262" t="s">
         <v>24</v>
@@ -7449,10 +7449,10 @@
         <v>9</v>
       </c>
       <c r="C263">
-        <v>20344</v>
+        <v>20853</v>
       </c>
       <c r="D263">
-        <v>27814269</v>
+        <v>28493480</v>
       </c>
       <c r="E263" t="s">
         <v>24</v>
@@ -7475,10 +7475,10 @@
         <v>9</v>
       </c>
       <c r="C264">
-        <v>9977</v>
+        <v>10235</v>
       </c>
       <c r="D264">
-        <v>12549172</v>
+        <v>12877893</v>
       </c>
       <c r="E264" t="s">
         <v>24</v>
@@ -7501,10 +7501,10 @@
         <v>9</v>
       </c>
       <c r="C265">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D265">
-        <v>5796</v>
+        <v>7296</v>
       </c>
       <c r="E265" t="s">
         <v>24</v>
@@ -7527,10 +7527,10 @@
         <v>9</v>
       </c>
       <c r="C266">
-        <v>11964</v>
+        <v>12183</v>
       </c>
       <c r="D266">
-        <v>14142879</v>
+        <v>14389657</v>
       </c>
       <c r="E266" t="s">
         <v>24</v>
@@ -7553,10 +7553,10 @@
         <v>9</v>
       </c>
       <c r="C267">
-        <v>23221</v>
+        <v>23750</v>
       </c>
       <c r="D267">
-        <v>31191584</v>
+        <v>31904275</v>
       </c>
       <c r="E267" t="s">
         <v>24</v>
@@ -7579,10 +7579,10 @@
         <v>9</v>
       </c>
       <c r="C268">
-        <v>10050</v>
+        <v>10308</v>
       </c>
       <c r="D268">
-        <v>12070743</v>
+        <v>12369495</v>
       </c>
       <c r="E268" t="s">
         <v>24</v>
@@ -7605,10 +7605,10 @@
         <v>9</v>
       </c>
       <c r="C269">
-        <v>30091</v>
+        <v>30496</v>
       </c>
       <c r="D269">
-        <v>35940608</v>
+        <v>36399907</v>
       </c>
       <c r="E269" t="s">
         <v>24</v>
@@ -7631,10 +7631,10 @@
         <v>9</v>
       </c>
       <c r="C270">
-        <v>2273</v>
+        <v>2355</v>
       </c>
       <c r="D270">
-        <v>3177868</v>
+        <v>3290223</v>
       </c>
       <c r="E270" t="s">
         <v>25</v>
@@ -7657,10 +7657,10 @@
         <v>9</v>
       </c>
       <c r="C271">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D271">
-        <v>68336</v>
+        <v>69686</v>
       </c>
       <c r="E271" t="s">
         <v>25</v>
@@ -7683,10 +7683,10 @@
         <v>9</v>
       </c>
       <c r="C272">
-        <v>4571</v>
+        <v>4668</v>
       </c>
       <c r="D272">
-        <v>5735031</v>
+        <v>5857892</v>
       </c>
       <c r="E272" t="s">
         <v>25</v>
@@ -7735,10 +7735,10 @@
         <v>9</v>
       </c>
       <c r="C274">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="D274">
-        <v>358628</v>
+        <v>369285</v>
       </c>
       <c r="E274" t="s">
         <v>25</v>
@@ -7761,10 +7761,10 @@
         <v>9</v>
       </c>
       <c r="C275">
-        <v>11463</v>
+        <v>11792</v>
       </c>
       <c r="D275">
-        <v>16510592</v>
+        <v>16989561</v>
       </c>
       <c r="E275" t="s">
         <v>25</v>
@@ -7787,10 +7787,10 @@
         <v>9</v>
       </c>
       <c r="C276">
-        <v>17639</v>
+        <v>17946</v>
       </c>
       <c r="D276">
-        <v>23476556</v>
+        <v>23887528</v>
       </c>
       <c r="E276" t="s">
         <v>25</v>
@@ -7813,10 +7813,10 @@
         <v>9</v>
       </c>
       <c r="C277">
-        <v>2271</v>
+        <v>2324</v>
       </c>
       <c r="D277">
-        <v>3191550</v>
+        <v>3263715</v>
       </c>
       <c r="E277" t="s">
         <v>25</v>
@@ -7839,10 +7839,10 @@
         <v>9</v>
       </c>
       <c r="C278">
-        <v>12133</v>
+        <v>12340</v>
       </c>
       <c r="D278">
-        <v>17545118</v>
+        <v>17838112</v>
       </c>
       <c r="E278" t="s">
         <v>25</v>
@@ -7865,10 +7865,10 @@
         <v>9</v>
       </c>
       <c r="C279">
-        <v>1634</v>
+        <v>1660</v>
       </c>
       <c r="D279">
-        <v>2090260</v>
+        <v>2122832</v>
       </c>
       <c r="E279" t="s">
         <v>25</v>
@@ -7891,10 +7891,10 @@
         <v>9</v>
       </c>
       <c r="C280">
-        <v>1003</v>
+        <v>1023</v>
       </c>
       <c r="D280">
-        <v>1423046</v>
+        <v>1449146</v>
       </c>
       <c r="E280" t="s">
         <v>25</v>
@@ -7917,10 +7917,10 @@
         <v>9</v>
       </c>
       <c r="C281">
-        <v>3211</v>
+        <v>3279</v>
       </c>
       <c r="D281">
-        <v>4357371</v>
+        <v>4446778</v>
       </c>
       <c r="E281" t="s">
         <v>25</v>
@@ -7943,10 +7943,10 @@
         <v>9</v>
       </c>
       <c r="C282">
-        <v>9418</v>
+        <v>9588</v>
       </c>
       <c r="D282">
-        <v>12849812</v>
+        <v>13082122</v>
       </c>
       <c r="E282" t="s">
         <v>25</v>
@@ -7969,10 +7969,10 @@
         <v>9</v>
       </c>
       <c r="C283">
-        <v>3571</v>
+        <v>3656</v>
       </c>
       <c r="D283">
-        <v>4628745</v>
+        <v>4739751</v>
       </c>
       <c r="E283" t="s">
         <v>25</v>
@@ -7995,10 +7995,10 @@
         <v>9</v>
       </c>
       <c r="C284">
-        <v>4364</v>
+        <v>4450</v>
       </c>
       <c r="D284">
-        <v>5336373</v>
+        <v>5436384</v>
       </c>
       <c r="E284" t="s">
         <v>25</v>
@@ -8021,10 +8021,10 @@
         <v>9</v>
       </c>
       <c r="C285">
-        <v>12434</v>
+        <v>12659</v>
       </c>
       <c r="D285">
-        <v>16747869</v>
+        <v>17043380</v>
       </c>
       <c r="E285" t="s">
         <v>25</v>
@@ -8047,10 +8047,10 @@
         <v>9</v>
       </c>
       <c r="C286">
-        <v>4858</v>
+        <v>4982</v>
       </c>
       <c r="D286">
-        <v>5948036</v>
+        <v>6096003</v>
       </c>
       <c r="E286" t="s">
         <v>25</v>
@@ -8073,10 +8073,10 @@
         <v>9</v>
       </c>
       <c r="C287">
-        <v>15485</v>
+        <v>15648</v>
       </c>
       <c r="D287">
-        <v>19597420</v>
+        <v>19787834</v>
       </c>
       <c r="E287" t="s">
         <v>25</v>
@@ -8099,10 +8099,10 @@
         <v>9</v>
       </c>
       <c r="C288">
-        <v>3092</v>
+        <v>3180</v>
       </c>
       <c r="D288">
-        <v>4234766</v>
+        <v>4353821</v>
       </c>
       <c r="E288" t="s">
         <v>26</v>
@@ -8151,10 +8151,10 @@
         <v>9</v>
       </c>
       <c r="C290">
-        <v>10428</v>
+        <v>10681</v>
       </c>
       <c r="D290">
-        <v>13650197</v>
+        <v>13987503</v>
       </c>
       <c r="E290" t="s">
         <v>26</v>
@@ -8177,10 +8177,10 @@
         <v>9</v>
       </c>
       <c r="C291">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D291">
-        <v>46359</v>
+        <v>49359</v>
       </c>
       <c r="E291" t="s">
         <v>26</v>
@@ -8203,10 +8203,10 @@
         <v>9</v>
       </c>
       <c r="C292">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D292">
-        <v>250382</v>
+        <v>254289</v>
       </c>
       <c r="E292" t="s">
         <v>26</v>
@@ -8229,10 +8229,10 @@
         <v>9</v>
       </c>
       <c r="C293">
-        <v>30365</v>
+        <v>31327</v>
       </c>
       <c r="D293">
-        <v>43464092</v>
+        <v>44848369</v>
       </c>
       <c r="E293" t="s">
         <v>26</v>
@@ -8255,10 +8255,10 @@
         <v>9</v>
       </c>
       <c r="C294">
-        <v>45605</v>
+        <v>46659</v>
       </c>
       <c r="D294">
-        <v>61420377</v>
+        <v>62794481</v>
       </c>
       <c r="E294" t="s">
         <v>26</v>
@@ -8281,10 +8281,10 @@
         <v>9</v>
       </c>
       <c r="C295">
-        <v>9728</v>
+        <v>10000</v>
       </c>
       <c r="D295">
-        <v>13653606</v>
+        <v>14028966</v>
       </c>
       <c r="E295" t="s">
         <v>26</v>
@@ -8307,10 +8307,10 @@
         <v>9</v>
       </c>
       <c r="C296">
-        <v>28507</v>
+        <v>29023</v>
       </c>
       <c r="D296">
-        <v>41303728</v>
+        <v>42045005</v>
       </c>
       <c r="E296" t="s">
         <v>26</v>
@@ -8333,10 +8333,10 @@
         <v>9</v>
       </c>
       <c r="C297">
-        <v>3896</v>
+        <v>3990</v>
       </c>
       <c r="D297">
-        <v>5106279</v>
+        <v>5221454</v>
       </c>
       <c r="E297" t="s">
         <v>26</v>
@@ -8359,10 +8359,10 @@
         <v>9</v>
       </c>
       <c r="C298">
-        <v>1961</v>
+        <v>2011</v>
       </c>
       <c r="D298">
-        <v>2781025</v>
+        <v>2850550</v>
       </c>
       <c r="E298" t="s">
         <v>26</v>
@@ -8385,10 +8385,10 @@
         <v>9</v>
       </c>
       <c r="C299">
-        <v>8664</v>
+        <v>8869</v>
       </c>
       <c r="D299">
-        <v>12020480</v>
+        <v>12305469</v>
       </c>
       <c r="E299" t="s">
         <v>26</v>
@@ -8411,10 +8411,10 @@
         <v>9</v>
       </c>
       <c r="C300">
-        <v>22361</v>
+        <v>22929</v>
       </c>
       <c r="D300">
-        <v>30624626</v>
+        <v>31388059</v>
       </c>
       <c r="E300" t="s">
         <v>26</v>
@@ -8437,10 +8437,10 @@
         <v>9</v>
       </c>
       <c r="C301">
-        <v>11937</v>
+        <v>12242</v>
       </c>
       <c r="D301">
-        <v>15460499</v>
+        <v>15862227</v>
       </c>
       <c r="E301" t="s">
         <v>26</v>
@@ -8489,10 +8489,10 @@
         <v>9</v>
       </c>
       <c r="C303">
-        <v>12958</v>
+        <v>13234</v>
       </c>
       <c r="D303">
-        <v>15898835</v>
+        <v>16208651</v>
       </c>
       <c r="E303" t="s">
         <v>26</v>
@@ -8515,10 +8515,10 @@
         <v>9</v>
       </c>
       <c r="C304">
-        <v>21986</v>
+        <v>22504</v>
       </c>
       <c r="D304">
-        <v>29603280</v>
+        <v>30287713</v>
       </c>
       <c r="E304" t="s">
         <v>26</v>
@@ -8541,10 +8541,10 @@
         <v>9</v>
       </c>
       <c r="C305">
-        <v>9679</v>
+        <v>9931</v>
       </c>
       <c r="D305">
-        <v>12056831</v>
+        <v>12355152</v>
       </c>
       <c r="E305" t="s">
         <v>26</v>
@@ -8567,10 +8567,10 @@
         <v>9</v>
       </c>
       <c r="C306">
-        <v>28873</v>
+        <v>29315</v>
       </c>
       <c r="D306">
-        <v>35075155</v>
+        <v>35590611</v>
       </c>
       <c r="E306" t="s">
         <v>26</v>
@@ -8593,10 +8593,10 @@
         <v>9</v>
       </c>
       <c r="C307">
-        <v>477</v>
+        <v>492</v>
       </c>
       <c r="D307">
-        <v>659134</v>
+        <v>680530</v>
       </c>
       <c r="E307" t="s">
         <v>27</v>
@@ -8619,10 +8619,10 @@
         <v>9</v>
       </c>
       <c r="C308">
-        <v>11932</v>
+        <v>12308</v>
       </c>
       <c r="D308">
-        <v>16091397</v>
+        <v>16582540</v>
       </c>
       <c r="E308" t="s">
         <v>27</v>
@@ -8645,10 +8645,10 @@
         <v>9</v>
       </c>
       <c r="C309">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D309">
-        <v>113566</v>
+        <v>115666</v>
       </c>
       <c r="E309" t="s">
         <v>27</v>
@@ -8671,10 +8671,10 @@
         <v>9</v>
       </c>
       <c r="C310">
-        <v>352</v>
+        <v>369</v>
       </c>
       <c r="D310">
-        <v>463301</v>
+        <v>485105</v>
       </c>
       <c r="E310" t="s">
         <v>27</v>
@@ -8697,10 +8697,10 @@
         <v>9</v>
       </c>
       <c r="C311">
-        <v>36307</v>
+        <v>37654</v>
       </c>
       <c r="D311">
-        <v>52546552</v>
+        <v>54503523</v>
       </c>
       <c r="E311" t="s">
         <v>27</v>
@@ -8723,10 +8723,10 @@
         <v>9</v>
       </c>
       <c r="C312">
-        <v>64260</v>
+        <v>66101</v>
       </c>
       <c r="D312">
-        <v>88735492</v>
+        <v>91270986</v>
       </c>
       <c r="E312" t="s">
         <v>27</v>
@@ -8749,10 +8749,10 @@
         <v>9</v>
       </c>
       <c r="C313">
-        <v>62037</v>
+        <v>63559</v>
       </c>
       <c r="D313">
-        <v>89342776</v>
+        <v>91485057</v>
       </c>
       <c r="E313" t="s">
         <v>27</v>
@@ -8775,10 +8775,10 @@
         <v>9</v>
       </c>
       <c r="C314">
-        <v>39660</v>
+        <v>40790</v>
       </c>
       <c r="D314">
-        <v>58549386</v>
+        <v>60214917</v>
       </c>
       <c r="E314" t="s">
         <v>27</v>
@@ -8801,10 +8801,10 @@
         <v>9</v>
       </c>
       <c r="C315">
-        <v>17299</v>
+        <v>17778</v>
       </c>
       <c r="D315">
-        <v>23767936</v>
+        <v>24427233</v>
       </c>
       <c r="E315" t="s">
         <v>27</v>
@@ -8827,10 +8827,10 @@
         <v>9</v>
       </c>
       <c r="C316">
-        <v>4353</v>
+        <v>4468</v>
       </c>
       <c r="D316">
-        <v>6263899</v>
+        <v>6427778</v>
       </c>
       <c r="E316" t="s">
         <v>27</v>
@@ -8853,10 +8853,10 @@
         <v>9</v>
       </c>
       <c r="C317">
-        <v>11312</v>
+        <v>11622</v>
       </c>
       <c r="D317">
-        <v>16126301</v>
+        <v>16561594</v>
       </c>
       <c r="E317" t="s">
         <v>27</v>
@@ -8879,10 +8879,10 @@
         <v>9</v>
       </c>
       <c r="C318">
-        <v>67712</v>
+        <v>69569</v>
       </c>
       <c r="D318">
-        <v>93846229</v>
+        <v>96387842</v>
       </c>
       <c r="E318" t="s">
         <v>27</v>
@@ -8905,10 +8905,10 @@
         <v>9</v>
       </c>
       <c r="C319">
-        <v>17793</v>
+        <v>18266</v>
       </c>
       <c r="D319">
-        <v>23972539</v>
+        <v>24606080</v>
       </c>
       <c r="E319" t="s">
         <v>27</v>
@@ -8957,10 +8957,10 @@
         <v>9</v>
       </c>
       <c r="C321">
-        <v>18977</v>
+        <v>19467</v>
       </c>
       <c r="D321">
-        <v>23609317</v>
+        <v>24189998</v>
       </c>
       <c r="E321" t="s">
         <v>27</v>
@@ -8983,10 +8983,10 @@
         <v>9</v>
       </c>
       <c r="C322">
-        <v>36754</v>
+        <v>37612</v>
       </c>
       <c r="D322">
-        <v>50456568</v>
+        <v>51634211</v>
       </c>
       <c r="E322" t="s">
         <v>27</v>
@@ -9009,10 +9009,10 @@
         <v>9</v>
       </c>
       <c r="C323">
-        <v>25805</v>
+        <v>26626</v>
       </c>
       <c r="D323">
-        <v>33459674</v>
+        <v>34488828</v>
       </c>
       <c r="E323" t="s">
         <v>27</v>
@@ -9035,10 +9035,10 @@
         <v>9</v>
       </c>
       <c r="C324">
-        <v>38982</v>
+        <v>39769</v>
       </c>
       <c r="D324">
-        <v>51353503</v>
+        <v>52408582</v>
       </c>
       <c r="E324" t="s">
         <v>27</v>

</xml_diff>